<commit_message>
Added Amazon Premier and Alibaba Qwen
</commit_message>
<xml_diff>
--- a/data/benchmarks.xlsx
+++ b/data/benchmarks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sean/Coding/genai-explorer/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sean.betts/Library/Mobile Documents/com~apple~CloudDocs/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5C3B35-E8A0-5A41-98FF-7BB508AAF194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7E80D3-1BB9-2E48-9716-37F328340E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57600" yWindow="0" windowWidth="60160" windowHeight="33840" activeTab="2" xr2:uid="{683877ED-707A-FC42-8592-F58A6955B3A6}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="36000" windowHeight="22520" activeTab="2" xr2:uid="{683877ED-707A-FC42-8592-F58A6955B3A6}"/>
   </bookViews>
   <sheets>
     <sheet name="model-meta" sheetId="3" r:id="rId1"/>
@@ -19,8 +19,8 @@
   </sheets>
   <definedNames>
     <definedName name="benchmark_id">'benchmark-meta'!$A$2:$A$1000</definedName>
-    <definedName name="model_id">'model-meta'!$A$2:$A$1012</definedName>
-    <definedName name="ModelMeta">'model-meta'!$A$1012:$B$1012</definedName>
+    <definedName name="model_id">'model-meta'!$A$2:$A$1020</definedName>
+    <definedName name="ModelMeta">'model-meta'!$A$1020:$B$1020</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5654" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6134" uniqueCount="369">
   <si>
     <t>model_id</t>
   </si>
@@ -1112,6 +1112,45 @@
   <si>
     <t>BrowseComp announcement</t>
   </si>
+  <si>
+    <t>Amazon Nova Premier announcement</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/blogs/aws/amazon-nova-premier-our-most-capable-model-for-complex-tasks-and-teacher-for-model-distillation/</t>
+  </si>
+  <si>
+    <t>nova-premier-1-0</t>
+  </si>
+  <si>
+    <t>alibaba</t>
+  </si>
+  <si>
+    <t>qwen-3-235b-a22b</t>
+  </si>
+  <si>
+    <t>qwen-3-32b</t>
+  </si>
+  <si>
+    <t>qwen-3-14b</t>
+  </si>
+  <si>
+    <t>qwen-3-8b</t>
+  </si>
+  <si>
+    <t>qwen-3-4b</t>
+  </si>
+  <si>
+    <t>qwen-3-1-7b</t>
+  </si>
+  <si>
+    <t>qwen-3-0-6b</t>
+  </si>
+  <si>
+    <t>Qwen 3 announcement</t>
+  </si>
+  <si>
+    <t>https://qwenlm.github.io/blog/qwen3/</t>
+  </si>
 </sst>
 </file>
 
@@ -1562,11 +1601,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5579D913-ECD6-6A42-858D-C12502E32020}">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1608,159 +1645,159 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>324</v>
+        <v>358</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>162</v>
+        <v>360</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>359</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>361</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>359</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>362</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>48</v>
+        <v>359</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>363</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>48</v>
+        <v>359</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>219</v>
+        <v>364</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>129</v>
+        <v>359</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>365</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>129</v>
+        <v>359</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>347</v>
+        <v>366</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>129</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>129</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>126</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>126</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>163</v>
+        <v>47</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>124</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>124</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>143</v>
+        <v>219</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>181</v>
+        <v>123</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>180</v>
+        <v>347</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>179</v>
+        <v>348</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>182</v>
+        <v>114</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>217</v>
+        <v>116</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>163</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>124</v>
@@ -1768,7 +1805,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>218</v>
+        <v>117</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>124</v>
@@ -1776,7 +1813,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>297</v>
+        <v>143</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>124</v>
@@ -1784,7 +1821,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>298</v>
+        <v>181</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>124</v>
@@ -1792,7 +1829,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>299</v>
+        <v>180</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>124</v>
@@ -1800,151 +1837,151 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>119</v>
+        <v>179</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>208</v>
+        <v>111</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>122</v>
+        <v>218</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>115</v>
+        <v>297</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>327</v>
+        <v>298</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>121</v>
+        <v>299</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>328</v>
+        <v>119</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>333</v>
+        <v>212</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>211</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>7</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>61</v>
+        <v>208</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>7</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>7</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>64</v>
+        <v>115</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>7</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>131</v>
+        <v>327</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>7</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>121</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>328</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>42</v>
+        <v>333</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>132</v>
+        <v>60</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>7</v>
@@ -1952,7 +1989,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>7</v>
@@ -1960,7 +1997,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>7</v>
@@ -1968,7 +2005,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>7</v>
@@ -1976,7 +2013,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>43</v>
+        <v>131</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>7</v>
@@ -1984,96 +2021,160 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>154</v>
+        <v>53</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>125</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>120</v>
+        <v>63</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>125</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>155</v>
+        <v>42</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>125</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>125</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>140</v>
+        <v>45</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>125</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>319</v>
+        <v>8</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>354</v>
+        <v>38</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>341</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>340</v>
+        <v>43</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>341</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>344</v>
+        <v>154</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>341</v>
+        <v>125</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>345</v>
+        <v>120</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>341</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>155</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>113</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>140</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>319</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>354</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>340</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>344</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>345</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>346</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>341</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B56">
-    <sortCondition ref="B2:B56"/>
-    <sortCondition ref="A2:A56"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B64">
+    <sortCondition ref="B2:B64"/>
+    <sortCondition ref="A2:A64"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
@@ -3045,10 +3146,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A72D42-DDBC-2B44-AB6C-55AD4AA1061B}">
-  <dimension ref="A1:H1837"/>
+  <dimension ref="A1:H1794"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1187" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G1229" sqref="G1229:H1229"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1311" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1319" sqref="A1319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -33706,786 +33808,2874 @@
       </c>
     </row>
     <row r="1230" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1230" s="2" t="s">
+        <v>358</v>
+      </c>
       <c r="B1230" s="1" t="str">
         <f>IF(A1230="", "", VLOOKUP(A1230, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>amazon</v>
+      </c>
+      <c r="C1230" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1230" s="12">
+        <v>87.4</v>
+      </c>
+      <c r="E1230" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1230" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1230" s="13" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="1231" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1231" s="2" t="s">
+        <v>292</v>
+      </c>
       <c r="B1231" s="1" t="str">
         <f>IF(A1231="", "", VLOOKUP(A1231, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>amazon</v>
+      </c>
+      <c r="C1231" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1231" s="12">
+        <v>85.9</v>
+      </c>
+      <c r="E1231" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1231" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1231" s="13" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="1232" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1232" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="B1232" s="1" t="str">
         <f>IF(A1232="", "", VLOOKUP(A1232, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1233" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1232" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1232" s="12">
+        <v>88.3</v>
+      </c>
+      <c r="E1232" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1232" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1232" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1233" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1233" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="B1233" s="1" t="str">
         <f>IF(A1233="", "", VLOOKUP(A1233, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1234" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1233" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1233" s="12">
+        <v>90.1</v>
+      </c>
+      <c r="E1233" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1233" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1233" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1234" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="B1234" s="1" t="str">
         <f>IF(A1234="", "", VLOOKUP(A1234, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1235" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1234" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1234" s="12">
+        <v>91.3</v>
+      </c>
+      <c r="E1234" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1234" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1234" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1235" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1235" s="2" t="s">
+        <v>358</v>
+      </c>
       <c r="B1235" s="1" t="str">
         <f>IF(A1235="", "", VLOOKUP(A1235, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1236" spans="2:2" x14ac:dyDescent="0.2">
+        <v>amazon</v>
+      </c>
+      <c r="C1235" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1235" s="12">
+        <v>57.1</v>
+      </c>
+      <c r="E1235" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1235" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1235" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1236" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1236" s="2" t="s">
+        <v>292</v>
+      </c>
       <c r="B1236" s="1" t="str">
         <f>IF(A1236="", "", VLOOKUP(A1236, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1237" spans="2:2" x14ac:dyDescent="0.2">
+        <v>amazon</v>
+      </c>
+      <c r="C1236" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1236" s="12">
+        <v>50</v>
+      </c>
+      <c r="E1236" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1236" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1236" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1237" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1237" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="B1237" s="1" t="str">
         <f>IF(A1237="", "", VLOOKUP(A1237, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1238" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1237" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1237" s="12">
+        <v>65</v>
+      </c>
+      <c r="E1237" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1237" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1237" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1238" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="B1238" s="1" t="str">
         <f>IF(A1238="", "", VLOOKUP(A1238, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1239" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1238" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1238" s="12">
+        <v>68</v>
+      </c>
+      <c r="E1238" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1238" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1238" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1239" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="B1239" s="1" t="str">
         <f>IF(A1239="", "", VLOOKUP(A1239, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1240" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1239" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1239" s="12">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="E1239" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1239" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1239" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1240" s="2" t="s">
+        <v>358</v>
+      </c>
       <c r="B1240" s="1" t="str">
         <f>IF(A1240="", "", VLOOKUP(A1240, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1241" spans="2:2" x14ac:dyDescent="0.2">
+        <v>amazon</v>
+      </c>
+      <c r="C1240" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1240" s="12">
+        <v>16</v>
+      </c>
+      <c r="E1240" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1240" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1240" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1241" s="2" t="s">
+        <v>292</v>
+      </c>
       <c r="B1241" s="1" t="str">
         <f>IF(A1241="", "", VLOOKUP(A1241, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1242" spans="2:2" x14ac:dyDescent="0.2">
+        <v>amazon</v>
+      </c>
+      <c r="C1241" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1241" s="12">
+        <v>5.3</v>
+      </c>
+      <c r="E1241" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1241" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1241" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1242" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="B1242" s="1" t="str">
         <f>IF(A1242="", "", VLOOKUP(A1242, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1243" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1242" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1242" s="12">
+        <v>4.7</v>
+      </c>
+      <c r="E1242" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1242" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1242" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1243" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="B1243" s="1" t="str">
         <f>IF(A1243="", "", VLOOKUP(A1243, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1244" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1243" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1243" s="12">
+        <v>18</v>
+      </c>
+      <c r="E1243" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1243" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1243" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1244" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="B1244" s="1" t="str">
         <f>IF(A1244="", "", VLOOKUP(A1244, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1245" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1244" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1244" s="12">
+        <v>30</v>
+      </c>
+      <c r="E1244" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1244" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1244" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1245" s="2" t="s">
+        <v>358</v>
+      </c>
       <c r="B1245" s="1" t="str">
         <f>IF(A1245="", "", VLOOKUP(A1245, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1246" spans="2:2" x14ac:dyDescent="0.2">
+        <v>amazon</v>
+      </c>
+      <c r="C1245" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1245" s="12">
+        <v>82</v>
+      </c>
+      <c r="E1245" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1245" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1245" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1246" s="2" t="s">
+        <v>292</v>
+      </c>
       <c r="B1246" s="1" t="str">
         <f>IF(A1246="", "", VLOOKUP(A1246, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1247" spans="2:2" x14ac:dyDescent="0.2">
+        <v>amazon</v>
+      </c>
+      <c r="C1246" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1246" s="12">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="E1246" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1246" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1246" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1247" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="B1247" s="1" t="str">
         <f>IF(A1247="", "", VLOOKUP(A1247, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1248" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1247" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1247" s="12">
+        <v>78</v>
+      </c>
+      <c r="E1247" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1247" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1247" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1248" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="B1248" s="1" t="str">
         <f>IF(A1248="", "", VLOOKUP(A1248, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1249" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1248" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1248" s="12">
+        <v>82.2</v>
+      </c>
+      <c r="E1248" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1248" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1248" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1249" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="B1249" s="1" t="str">
         <f>IF(A1249="", "", VLOOKUP(A1249, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1250" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1249" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1249" s="12">
+        <v>88</v>
+      </c>
+      <c r="E1249" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1249" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1249" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1250" s="2" t="s">
+        <v>358</v>
+      </c>
       <c r="B1250" s="1" t="str">
         <f>IF(A1250="", "", VLOOKUP(A1250, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1251" spans="2:2" x14ac:dyDescent="0.2">
+        <v>amazon</v>
+      </c>
+      <c r="C1250" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1250" s="12">
+        <v>28.1</v>
+      </c>
+      <c r="E1250" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1250" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1250" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1251" s="2" t="s">
+        <v>292</v>
+      </c>
       <c r="B1251" s="1" t="str">
         <f>IF(A1251="", "", VLOOKUP(A1251, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1252" spans="2:2" x14ac:dyDescent="0.2">
+        <v>amazon</v>
+      </c>
+      <c r="C1251" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1251" s="12">
+        <v>22.3</v>
+      </c>
+      <c r="E1251" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1251" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1251" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1252" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="B1252" s="1" t="str">
         <f>IF(A1252="", "", VLOOKUP(A1252, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1253" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1252" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1252" s="12">
+        <v>30.4</v>
+      </c>
+      <c r="E1252" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1252" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1252" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1253" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="B1253" s="1" t="str">
         <f>IF(A1253="", "", VLOOKUP(A1253, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1254" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1253" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1253" s="12">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="E1253" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1253" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1253" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1254" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="B1254" s="1" t="str">
         <f>IF(A1254="", "", VLOOKUP(A1254, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1255" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1254" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1254" s="12">
+        <v>33.1</v>
+      </c>
+      <c r="E1254" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1254" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1254" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1255" s="2" t="s">
+        <v>358</v>
+      </c>
       <c r="B1255" s="1" t="str">
         <f>IF(A1255="", "", VLOOKUP(A1255, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1256" spans="2:2" x14ac:dyDescent="0.2">
+        <v>amazon</v>
+      </c>
+      <c r="C1255" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1255" s="12">
+        <v>91.5</v>
+      </c>
+      <c r="E1255" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1255" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1255" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1256" s="2" t="s">
+        <v>292</v>
+      </c>
       <c r="B1256" s="1" t="str">
         <f>IF(A1256="", "", VLOOKUP(A1256, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1257" spans="2:2" x14ac:dyDescent="0.2">
+        <v>amazon</v>
+      </c>
+      <c r="C1256" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1256" s="12">
+        <v>92.1</v>
+      </c>
+      <c r="E1256" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1256" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1256" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1257" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="B1257" s="1" t="str">
         <f>IF(A1257="", "", VLOOKUP(A1257, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1258" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1257" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1257" s="12">
+        <v>90.2</v>
+      </c>
+      <c r="E1257" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1257" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1257" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1258" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="B1258" s="1" t="str">
         <f>IF(A1258="", "", VLOOKUP(A1258, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1259" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1258" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1258" s="12">
+        <v>90.8</v>
+      </c>
+      <c r="E1258" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1258" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1258" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1259" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="B1259" s="1" t="str">
         <f>IF(A1259="", "", VLOOKUP(A1259, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1260" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1259" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1259" s="12">
+        <v>93.3</v>
+      </c>
+      <c r="E1259" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1259" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1259" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1260" s="2" t="s">
+        <v>358</v>
+      </c>
       <c r="B1260" s="1" t="str">
         <f>IF(A1260="", "", VLOOKUP(A1260, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1261" spans="2:2" x14ac:dyDescent="0.2">
+        <v>amazon</v>
+      </c>
+      <c r="C1260" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1260" s="12">
+        <v>68</v>
+      </c>
+      <c r="E1260" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1260" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1260" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1261" s="2" t="s">
+        <v>292</v>
+      </c>
       <c r="B1261" s="1" t="str">
         <f>IF(A1261="", "", VLOOKUP(A1261, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1262" spans="2:2" x14ac:dyDescent="0.2">
+        <v>amazon</v>
+      </c>
+      <c r="C1261" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1261" s="12">
+        <v>62</v>
+      </c>
+      <c r="E1261" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1261" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1261" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1262" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="B1262" s="1" t="str">
         <f>IF(A1262="", "", VLOOKUP(A1262, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1263" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1262" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1262" s="12">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="E1262" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1262" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1262" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1263" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="B1263" s="1" t="str">
         <f>IF(A1263="", "", VLOOKUP(A1263, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1264" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1263" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1263" s="12">
+        <v>71.8</v>
+      </c>
+      <c r="E1263" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1263" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1263" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1264" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="B1264" s="1" t="str">
         <f>IF(A1264="", "", VLOOKUP(A1264, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1265" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1264" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1264" s="12">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="E1264" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1264" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1264" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1265" s="2" t="s">
+        <v>358</v>
+      </c>
       <c r="B1265" s="1" t="str">
         <f>IF(A1265="", "", VLOOKUP(A1265, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1266" spans="2:2" x14ac:dyDescent="0.2">
+        <v>amazon</v>
+      </c>
+      <c r="C1265" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1265" s="12">
+        <v>48.8</v>
+      </c>
+      <c r="E1265" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1265" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1265" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1266" s="2" t="s">
+        <v>292</v>
+      </c>
       <c r="B1266" s="1" t="str">
         <f>IF(A1266="", "", VLOOKUP(A1266, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1267" spans="2:2" x14ac:dyDescent="0.2">
+        <v>amazon</v>
+      </c>
+      <c r="C1266" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1266" s="12">
+        <v>40.6</v>
+      </c>
+      <c r="E1266" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1266" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1266" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1267" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="B1267" s="1" t="str">
         <f>IF(A1267="", "", VLOOKUP(A1267, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1268" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1267" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1267" s="12">
+        <v>60.2</v>
+      </c>
+      <c r="E1267" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1267" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1267" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1268" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="B1268" s="1" t="str">
         <f>IF(A1268="", "", VLOOKUP(A1268, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1269" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1268" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1268" s="12">
+        <v>64.2</v>
+      </c>
+      <c r="E1268" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1268" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1268" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1269" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="B1269" s="1" t="str">
         <f>IF(A1269="", "", VLOOKUP(A1269, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1270" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1269" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1269" s="12">
+        <v>55.4</v>
+      </c>
+      <c r="E1269" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1269" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1269" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1270" s="2" t="s">
+        <v>358</v>
+      </c>
       <c r="B1270" s="1" t="str">
         <f>IF(A1270="", "", VLOOKUP(A1270, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1271" spans="2:2" x14ac:dyDescent="0.2">
+        <v>amazon</v>
+      </c>
+      <c r="C1270" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1270" s="12">
+        <v>73.8</v>
+      </c>
+      <c r="E1270" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1270" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1270" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1271" s="2" t="s">
+        <v>292</v>
+      </c>
       <c r="B1271" s="1" t="str">
         <f>IF(A1271="", "", VLOOKUP(A1271, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1272" spans="2:2" x14ac:dyDescent="0.2">
+        <v>amazon</v>
+      </c>
+      <c r="C1271" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1271" s="12">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="E1271" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1271" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1271" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1272" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="B1272" s="1" t="str">
         <f>IF(A1272="", "", VLOOKUP(A1272, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1273" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1272" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1272" s="12">
+        <v>68.8</v>
+      </c>
+      <c r="E1272" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1272" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1272" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1273" s="2" t="s">
+        <v>358</v>
+      </c>
       <c r="B1273" s="1" t="str">
         <f>IF(A1273="", "", VLOOKUP(A1273, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1274" spans="2:2" x14ac:dyDescent="0.2">
+        <v>amazon</v>
+      </c>
+      <c r="C1273" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1273" s="12">
+        <v>86.3</v>
+      </c>
+      <c r="E1273" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1273" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1273" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1274" s="2" t="s">
+        <v>292</v>
+      </c>
       <c r="B1274" s="1" t="str">
         <f>IF(A1274="", "", VLOOKUP(A1274, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1275" spans="2:2" x14ac:dyDescent="0.2">
+        <v>amazon</v>
+      </c>
+      <c r="C1274" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1274" s="12">
+        <v>84.6</v>
+      </c>
+      <c r="E1274" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1274" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1274" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1275" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="B1275" s="1" t="str">
         <f>IF(A1275="", "", VLOOKUP(A1275, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1276" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1275" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1275" s="12">
+        <v>87.4</v>
+      </c>
+      <c r="E1275" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1275" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1275" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1276" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="B1276" s="1" t="str">
         <f>IF(A1276="", "", VLOOKUP(A1276, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1277" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1276" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1276" s="12">
+        <v>91.1</v>
+      </c>
+      <c r="E1276" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1276" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1276" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1277" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="B1277" s="1" t="str">
         <f>IF(A1277="", "", VLOOKUP(A1277, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1278" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1277" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1277" s="12">
+        <v>89.1</v>
+      </c>
+      <c r="E1277" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1277" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1277" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1278" s="2" t="s">
+        <v>358</v>
+      </c>
       <c r="B1278" s="1" t="str">
         <f>IF(A1278="", "", VLOOKUP(A1278, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1279" spans="2:2" x14ac:dyDescent="0.2">
+        <v>amazon</v>
+      </c>
+      <c r="C1278" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1278" s="12">
+        <v>42.4</v>
+      </c>
+      <c r="E1278" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1278" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1278" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1279" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1279" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="B1279" s="1" t="str">
         <f>IF(A1279="", "", VLOOKUP(A1279, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1280" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1279" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1279" s="12">
+        <v>49</v>
+      </c>
+      <c r="E1279" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1279" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1279" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1280" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="B1280" s="1" t="str">
         <f>IF(A1280="", "", VLOOKUP(A1280, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1281" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1280" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1280" s="12">
+        <v>62.3</v>
+      </c>
+      <c r="E1280" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1280" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1280" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1281" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="B1281" s="1" t="str">
         <f>IF(A1281="", "", VLOOKUP(A1281, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1282" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1281" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1281" s="12">
+        <v>38</v>
+      </c>
+      <c r="E1281" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1281" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1281" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1282" s="2" t="s">
+        <v>360</v>
+      </c>
       <c r="B1282" s="1" t="str">
         <f>IF(A1282="", "", VLOOKUP(A1282, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1283" spans="2:2" x14ac:dyDescent="0.2">
+        <v>alibaba</v>
+      </c>
+      <c r="C1282" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1282" s="12">
+        <v>85.7</v>
+      </c>
+      <c r="E1282" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1282" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1282" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1283" s="2" t="s">
+        <v>361</v>
+      </c>
       <c r="B1283" s="1" t="str">
         <f>IF(A1283="", "", VLOOKUP(A1283, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1284" spans="2:2" x14ac:dyDescent="0.2">
+        <v>alibaba</v>
+      </c>
+      <c r="C1283" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1283" s="12">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="E1283" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1283" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1283" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1284" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="B1284" s="1" t="str">
         <f>IF(A1284="", "", VLOOKUP(A1284, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1285" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1284" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1284" s="12">
+        <v>74.3</v>
+      </c>
+      <c r="E1284" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1284" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1284" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1285" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="B1285" s="1" t="str">
         <f>IF(A1285="", "", VLOOKUP(A1285, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1286" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1285" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1285" s="12">
+        <v>79.8</v>
+      </c>
+      <c r="E1285" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1285" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1285" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1286" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="B1286" s="1" t="str">
         <f>IF(A1286="", "", VLOOKUP(A1286, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1287" spans="2:2" x14ac:dyDescent="0.2">
+        <v>xai</v>
+      </c>
+      <c r="C1286" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1286" s="12">
+        <v>83.9</v>
+      </c>
+      <c r="E1286" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1286" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1286" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1287" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1287" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="B1287" s="1" t="str">
         <f>IF(A1287="", "", VLOOKUP(A1287, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1288" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google</v>
+      </c>
+      <c r="C1287" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1287" s="12">
+        <v>92</v>
+      </c>
+      <c r="E1287" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1287" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1287" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1288" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1288" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="B1288" s="1" t="str">
         <f>IF(A1288="", "", VLOOKUP(A1288, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1289" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1288" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1288" s="12">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="E1288" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1288" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1288" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1289" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1289" s="2" t="s">
+        <v>360</v>
+      </c>
       <c r="B1289" s="1" t="str">
         <f>IF(A1289="", "", VLOOKUP(A1289, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1290" spans="2:2" x14ac:dyDescent="0.2">
+        <v>alibaba</v>
+      </c>
+      <c r="C1289" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1289" s="12">
+        <v>81.5</v>
+      </c>
+      <c r="E1289" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1289" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1289" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1290" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1290" s="2" t="s">
+        <v>361</v>
+      </c>
       <c r="B1290" s="1" t="str">
         <f>IF(A1290="", "", VLOOKUP(A1290, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1291" spans="2:2" x14ac:dyDescent="0.2">
+        <v>alibaba</v>
+      </c>
+      <c r="C1290" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1290" s="12">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="E1290" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1290" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1290" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1291" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1291" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="B1291" s="1" t="str">
         <f>IF(A1291="", "", VLOOKUP(A1291, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1292" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1291" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1291" s="12">
+        <v>79.2</v>
+      </c>
+      <c r="E1291" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1291" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1291" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1292" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1292" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="B1292" s="1" t="str">
         <f>IF(A1292="", "", VLOOKUP(A1292, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1293" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1292" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1292" s="12">
+        <v>70</v>
+      </c>
+      <c r="E1292" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1292" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1292" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1293" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1293" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="B1293" s="1" t="str">
         <f>IF(A1293="", "", VLOOKUP(A1293, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1294" spans="2:2" x14ac:dyDescent="0.2">
+        <v>xai</v>
+      </c>
+      <c r="C1293" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1293" s="12">
+        <v>77.3</v>
+      </c>
+      <c r="E1293" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1293" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1293" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1294" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1294" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="B1294" s="1" t="str">
         <f>IF(A1294="", "", VLOOKUP(A1294, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1295" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google</v>
+      </c>
+      <c r="C1294" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1294" s="12">
+        <v>86.7</v>
+      </c>
+      <c r="E1294" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1294" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1294" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1295" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1295" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="B1295" s="1" t="str">
         <f>IF(A1295="", "", VLOOKUP(A1295, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1296" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1295" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1295" s="12">
+        <v>74.8</v>
+      </c>
+      <c r="E1295" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1295" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1295" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1296" s="2" t="s">
+        <v>360</v>
+      </c>
       <c r="B1296" s="1" t="str">
         <f>IF(A1296="", "", VLOOKUP(A1296, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1297" spans="2:2" x14ac:dyDescent="0.2">
+        <v>alibaba</v>
+      </c>
+      <c r="C1296" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1296" s="12">
+        <v>70.7</v>
+      </c>
+      <c r="E1296" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1296" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1296" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1297" s="2" t="s">
+        <v>361</v>
+      </c>
       <c r="B1297" s="1" t="str">
         <f>IF(A1297="", "", VLOOKUP(A1297, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1298" spans="2:2" x14ac:dyDescent="0.2">
+        <v>alibaba</v>
+      </c>
+      <c r="C1297" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1297" s="12">
+        <v>65.7</v>
+      </c>
+      <c r="E1297" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1297" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1297" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1298" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="B1298" s="1" t="str">
         <f>IF(A1298="", "", VLOOKUP(A1298, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1299" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1298" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1298" s="12">
+        <v>63.9</v>
+      </c>
+      <c r="E1298" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1298" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1298" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1299" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1299" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="B1299" s="1" t="str">
         <f>IF(A1299="", "", VLOOKUP(A1299, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1300" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1299" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1299" s="12">
+        <v>64.3</v>
+      </c>
+      <c r="E1299" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1299" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1299" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1300" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="B1300" s="1" t="str">
         <f>IF(A1300="", "", VLOOKUP(A1300, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1301" spans="2:2" x14ac:dyDescent="0.2">
+        <v>xai</v>
+      </c>
+      <c r="C1300" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1300" s="12">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="E1300" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1300" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1300" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1301" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="B1301" s="1" t="str">
         <f>IF(A1301="", "", VLOOKUP(A1301, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1302" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google</v>
+      </c>
+      <c r="C1301" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1301" s="12">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="E1301" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1301" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1301" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1302" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1302" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="B1302" s="1" t="str">
         <f>IF(A1302="", "", VLOOKUP(A1302, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1303" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1302" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1302" s="12">
+        <v>66.3</v>
+      </c>
+      <c r="E1302" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1302" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1302" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1303" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1303" s="2" t="s">
+        <v>360</v>
+      </c>
       <c r="B1303" s="1" t="str">
         <f>IF(A1303="", "", VLOOKUP(A1303, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1304" spans="2:2" x14ac:dyDescent="0.2">
+        <v>alibaba</v>
+      </c>
+      <c r="C1303" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1303" s="12">
+        <v>2056</v>
+      </c>
+      <c r="E1303" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1303" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1303" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1304" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1304" s="2" t="s">
+        <v>361</v>
+      </c>
       <c r="B1304" s="1" t="str">
         <f>IF(A1304="", "", VLOOKUP(A1304, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1305" spans="2:2" x14ac:dyDescent="0.2">
+        <v>alibaba</v>
+      </c>
+      <c r="C1304" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1304" s="12">
+        <v>1977</v>
+      </c>
+      <c r="E1304" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1304" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1304" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1305" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1305" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="B1305" s="1" t="str">
         <f>IF(A1305="", "", VLOOKUP(A1305, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1306" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1305" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1305" s="12">
+        <v>1891</v>
+      </c>
+      <c r="E1305" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1305" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1305" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1306" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="B1306" s="1" t="str">
         <f>IF(A1306="", "", VLOOKUP(A1306, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1307" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1306" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1306" s="12">
+        <v>2029</v>
+      </c>
+      <c r="E1306" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1306" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1306" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1307" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1307" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="B1307" s="1" t="str">
         <f>IF(A1307="", "", VLOOKUP(A1307, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1308" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google</v>
+      </c>
+      <c r="C1307" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1307" s="12">
+        <v>2001</v>
+      </c>
+      <c r="E1307" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1307" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1307" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1308" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="B1308" s="1" t="str">
         <f>IF(A1308="", "", VLOOKUP(A1308, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1309" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1308" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1308" s="12">
+        <v>2036</v>
+      </c>
+      <c r="E1308" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1308" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1308" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1309" s="2" t="s">
+        <v>360</v>
+      </c>
       <c r="B1309" s="1" t="str">
         <f>IF(A1309="", "", VLOOKUP(A1309, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1310" spans="2:2" x14ac:dyDescent="0.2">
+        <v>alibaba</v>
+      </c>
+      <c r="C1309" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D1309" s="12">
+        <v>61.8</v>
+      </c>
+      <c r="E1309" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1309" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1309" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1310" s="2" t="s">
+        <v>361</v>
+      </c>
       <c r="B1310" s="1" t="str">
         <f>IF(A1310="", "", VLOOKUP(A1310, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1311" spans="2:2" x14ac:dyDescent="0.2">
+        <v>alibaba</v>
+      </c>
+      <c r="C1310" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D1310" s="12">
+        <v>50.2</v>
+      </c>
+      <c r="E1310" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1310" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1310" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1311" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="B1311" s="1" t="str">
         <f>IF(A1311="", "", VLOOKUP(A1311, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1312" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1311" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D1311" s="12">
+        <v>61.7</v>
+      </c>
+      <c r="E1311" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1311" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1311" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1312" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="B1312" s="1" t="str">
         <f>IF(A1312="", "", VLOOKUP(A1312, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1313" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1312" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D1312" s="12">
+        <v>56.9</v>
+      </c>
+      <c r="E1312" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1312" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1312" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1313" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="B1313" s="1" t="str">
         <f>IF(A1313="", "", VLOOKUP(A1313, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1314" spans="2:2" x14ac:dyDescent="0.2">
+        <v>xai</v>
+      </c>
+      <c r="C1313" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D1313" s="12">
+        <v>53.3</v>
+      </c>
+      <c r="E1313" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1313" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1313" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1314" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="B1314" s="1" t="str">
         <f>IF(A1314="", "", VLOOKUP(A1314, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1315" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google</v>
+      </c>
+      <c r="C1314" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D1314" s="12">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="E1314" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1314" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1314" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1315" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="B1315" s="1" t="str">
         <f>IF(A1315="", "", VLOOKUP(A1315, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1316" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1315" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D1315" s="12">
+        <v>53.8</v>
+      </c>
+      <c r="E1315" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1315" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1315" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1316" s="2" t="s">
+        <v>360</v>
+      </c>
       <c r="B1316" s="1" t="str">
         <f>IF(A1316="", "", VLOOKUP(A1316, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1317" spans="2:2" x14ac:dyDescent="0.2">
+        <v>alibaba</v>
+      </c>
+      <c r="C1316" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1316" s="12">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="E1316" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1316" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1316" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1317" s="2" t="s">
+        <v>361</v>
+      </c>
       <c r="B1317" s="1" t="str">
         <f>IF(A1317="", "", VLOOKUP(A1317, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1318" spans="2:2" x14ac:dyDescent="0.2">
+        <v>alibaba</v>
+      </c>
+      <c r="C1317" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1317" s="12">
+        <v>73</v>
+      </c>
+      <c r="E1317" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1317" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1317" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1318" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="B1318" s="1" t="str">
         <f>IF(A1318="", "", VLOOKUP(A1318, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1319" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1318" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1318" s="12">
+        <v>48.8</v>
+      </c>
+      <c r="E1318" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1318" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1318" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1319" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="B1319" s="1" t="str">
         <f>IF(A1319="", "", VLOOKUP(A1319, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1320" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1319" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1319" s="12">
+        <v>67.7</v>
+      </c>
+      <c r="E1319" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1319" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1319" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1320" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="B1320" s="1" t="str">
         <f>IF(A1320="", "", VLOOKUP(A1320, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1321" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google</v>
+      </c>
+      <c r="C1320" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1320" s="12">
+        <v>77.8</v>
+      </c>
+      <c r="E1320" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1320" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1320" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1321" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="B1321" s="1" t="str">
         <f>IF(A1321="", "", VLOOKUP(A1321, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1322" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1321" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1321" s="12">
+        <v>48.4</v>
+      </c>
+      <c r="E1321" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1321" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1321" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1322" s="2" t="s">
+        <v>364</v>
+      </c>
       <c r="B1322" s="1" t="str">
         <f>IF(A1322="", "", VLOOKUP(A1322, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1323" spans="2:2" x14ac:dyDescent="0.2">
+        <v>alibaba</v>
+      </c>
+      <c r="C1322" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1322" s="12">
+        <v>73.8</v>
+      </c>
+      <c r="E1322" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1322" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1322" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1323" s="2" t="s">
+        <v>218</v>
+      </c>
       <c r="B1323" s="1" t="str">
         <f>IF(A1323="", "", VLOOKUP(A1323, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1324" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google</v>
+      </c>
+      <c r="C1323" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1323" s="12">
+        <v>32.6</v>
+      </c>
+      <c r="E1323" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1323" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1323" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1324" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="B1324" s="1" t="str">
         <f>IF(A1324="", "", VLOOKUP(A1324, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1325" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1324" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1324" s="12">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="E1324" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1324" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1324" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1325" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1325" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B1325" s="1" t="str">
         <f>IF(A1325="", "", VLOOKUP(A1325, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1326" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1325" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1325" s="12">
+        <v>11.1</v>
+      </c>
+      <c r="E1325" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1325" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1325" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1326" s="2" t="s">
+        <v>364</v>
+      </c>
       <c r="B1326" s="1" t="str">
         <f>IF(A1326="", "", VLOOKUP(A1326, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1327" spans="2:2" x14ac:dyDescent="0.2">
+        <v>alibaba</v>
+      </c>
+      <c r="C1326" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1326" s="12">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="E1326" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1326" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1326" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1327" s="2" t="s">
+        <v>218</v>
+      </c>
       <c r="B1327" s="1" t="str">
         <f>IF(A1327="", "", VLOOKUP(A1327, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1328" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google</v>
+      </c>
+      <c r="C1327" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1327" s="12">
+        <v>24</v>
+      </c>
+      <c r="E1327" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1327" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1327" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1328" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="B1328" s="1" t="str">
         <f>IF(A1328="", "", VLOOKUP(A1328, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1329" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1328" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1328" s="12">
+        <v>28.8</v>
+      </c>
+      <c r="E1328" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1328" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1328" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1329" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B1329" s="1" t="str">
         <f>IF(A1329="", "", VLOOKUP(A1329, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1330" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1329" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1329" s="12">
+        <v>7.6</v>
+      </c>
+      <c r="E1329" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1329" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1329" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1330" s="2" t="s">
+        <v>364</v>
+      </c>
       <c r="B1330" s="1" t="str">
         <f>IF(A1330="", "", VLOOKUP(A1330, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1331" spans="2:2" x14ac:dyDescent="0.2">
+        <v>alibaba</v>
+      </c>
+      <c r="C1330" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1330" s="12">
+        <v>54.2</v>
+      </c>
+      <c r="E1330" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1330" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1330" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1331" s="2" t="s">
+        <v>218</v>
+      </c>
       <c r="B1331" s="1" t="str">
         <f>IF(A1331="", "", VLOOKUP(A1331, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1332" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google</v>
+      </c>
+      <c r="C1331" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1331" s="12">
+        <v>26.9</v>
+      </c>
+      <c r="E1331" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1331" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1331" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1332" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1332" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="B1332" s="1" t="str">
         <f>IF(A1332="", "", VLOOKUP(A1332, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1333" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1332" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1332" s="12">
+        <v>33.1</v>
+      </c>
+      <c r="E1332" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1332" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1332" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1333" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1333" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B1333" s="1" t="str">
         <f>IF(A1333="", "", VLOOKUP(A1333, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1334" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1333" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1333" s="12">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="E1333" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1333" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1333" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1334" s="2" t="s">
+        <v>364</v>
+      </c>
       <c r="B1334" s="1" t="str">
         <f>IF(A1334="", "", VLOOKUP(A1334, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1335" spans="2:2" x14ac:dyDescent="0.2">
+        <v>alibaba</v>
+      </c>
+      <c r="C1334" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1334" s="12">
+        <v>1671</v>
+      </c>
+      <c r="E1334" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1334" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1334" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1335" s="2" t="s">
+        <v>218</v>
+      </c>
       <c r="B1335" s="1" t="str">
         <f>IF(A1335="", "", VLOOKUP(A1335, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1336" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google</v>
+      </c>
+      <c r="C1335" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1335" s="12">
+        <v>1063</v>
+      </c>
+      <c r="E1335" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1335" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1335" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1336" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="B1336" s="1" t="str">
         <f>IF(A1336="", "", VLOOKUP(A1336, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1337" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1336" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1336" s="12">
+        <v>1134</v>
+      </c>
+      <c r="E1336" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1336" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1336" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1337" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1337" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B1337" s="1" t="str">
         <f>IF(A1337="", "", VLOOKUP(A1337, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1338" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1337" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1337" s="12">
+        <v>864</v>
+      </c>
+      <c r="E1337" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1337" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1337" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1338" s="2" t="s">
+        <v>364</v>
+      </c>
       <c r="B1338" s="1" t="str">
         <f>IF(A1338="", "", VLOOKUP(A1338, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1339" spans="2:2" x14ac:dyDescent="0.2">
+        <v>alibaba</v>
+      </c>
+      <c r="C1338" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1338" s="12">
+        <v>55.9</v>
+      </c>
+      <c r="E1338" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1338" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1338" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1339" s="2" t="s">
+        <v>218</v>
+      </c>
       <c r="B1339" s="1" t="str">
         <f>IF(A1339="", "", VLOOKUP(A1339, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1340" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google</v>
+      </c>
+      <c r="C1339" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1339" s="12">
+        <v>42.4</v>
+      </c>
+      <c r="E1339" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1339" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1339" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1340" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="B1340" s="1" t="str">
         <f>IF(A1340="", "", VLOOKUP(A1340, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1341" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1340" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1340" s="12">
+        <v>59.1</v>
+      </c>
+      <c r="E1340" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1340" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1340" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1341" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B1341" s="1" t="str">
         <f>IF(A1341="", "", VLOOKUP(A1341, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1342" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1341" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1341" s="12">
+        <v>46</v>
+      </c>
+      <c r="E1341" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1341" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1341" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1342" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1342" s="2" t="s">
+        <v>364</v>
+      </c>
       <c r="B1342" s="1" t="str">
         <f>IF(A1342="", "", VLOOKUP(A1342, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1343" spans="2:2" x14ac:dyDescent="0.2">
+        <v>alibaba</v>
+      </c>
+      <c r="C1342" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1342" s="12">
+        <v>66.3</v>
+      </c>
+      <c r="E1342" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1342" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1342" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1343" s="2" t="s">
+        <v>218</v>
+      </c>
       <c r="B1343" s="1" t="str">
         <f>IF(A1343="", "", VLOOKUP(A1343, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1344" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google</v>
+      </c>
+      <c r="C1343" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1343" s="12">
+        <v>69.8</v>
+      </c>
+      <c r="E1343" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1343" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1343" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1344" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="B1344" s="1" t="str">
         <f>IF(A1344="", "", VLOOKUP(A1344, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1345" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1344" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1344" s="12">
+        <v>55.6</v>
+      </c>
+      <c r="E1344" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1344" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1344" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1345" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B1345" s="1" t="str">
         <f>IF(A1345="", "", VLOOKUP(A1345, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1346" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1345" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1345" s="12">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="E1345" s="4">
+        <v>45776</v>
+      </c>
+      <c r="G1345" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1345" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1346" s="1" t="str">
         <f>IF(A1346="", "", VLOOKUP(A1346, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1347" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1347" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1347" s="1" t="str">
         <f>IF(A1347="", "", VLOOKUP(A1347, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1348" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1348" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1348" s="1" t="str">
         <f>IF(A1348="", "", VLOOKUP(A1348, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1349" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1349" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1349" s="1" t="str">
         <f>IF(A1349="", "", VLOOKUP(A1349, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1350" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1350" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1350" s="1" t="str">
         <f>IF(A1350="", "", VLOOKUP(A1350, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1351" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1351" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1351" s="1" t="str">
         <f>IF(A1351="", "", VLOOKUP(A1351, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1352" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1352" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1352" s="1" t="str">
         <f>IF(A1352="", "", VLOOKUP(A1352, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1353" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1353" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1353" s="1" t="str">
         <f>IF(A1353="", "", VLOOKUP(A1353, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1354" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1354" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1354" s="1" t="str">
         <f>IF(A1354="", "", VLOOKUP(A1354, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1355" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1355" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1355" s="1" t="str">
         <f>IF(A1355="", "", VLOOKUP(A1355, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1356" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1356" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1356" s="1" t="str">
         <f>IF(A1356="", "", VLOOKUP(A1356, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1357" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1357" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1357" s="1" t="str">
         <f>IF(A1357="", "", VLOOKUP(A1357, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1358" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1358" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1358" s="1" t="str">
         <f>IF(A1358="", "", VLOOKUP(A1358, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1359" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1359" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1359" s="1" t="str">
         <f>IF(A1359="", "", VLOOKUP(A1359, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1360" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1360" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1360" s="1" t="str">
         <f>IF(A1360="", "", VLOOKUP(A1360, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
@@ -37095,267 +39285,9 @@
         <v/>
       </c>
     </row>
-    <row r="1795" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1795" s="1" t="str">
-        <f>IF(A1795="", "", VLOOKUP(A1795, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1796" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1796" s="1" t="str">
-        <f>IF(A1796="", "", VLOOKUP(A1796, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1797" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1797" s="1" t="str">
-        <f>IF(A1797="", "", VLOOKUP(A1797, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1798" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1798" s="1" t="str">
-        <f>IF(A1798="", "", VLOOKUP(A1798, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1799" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1799" s="1" t="str">
-        <f>IF(A1799="", "", VLOOKUP(A1799, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1800" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1800" s="1" t="str">
-        <f>IF(A1800="", "", VLOOKUP(A1800, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1801" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1801" s="1" t="str">
-        <f>IF(A1801="", "", VLOOKUP(A1801, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1802" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1802" s="1" t="str">
-        <f>IF(A1802="", "", VLOOKUP(A1802, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1803" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1803" s="1" t="str">
-        <f>IF(A1803="", "", VLOOKUP(A1803, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1804" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1804" s="1" t="str">
-        <f>IF(A1804="", "", VLOOKUP(A1804, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1805" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1805" s="1" t="str">
-        <f>IF(A1805="", "", VLOOKUP(A1805, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1806" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1806" s="1" t="str">
-        <f>IF(A1806="", "", VLOOKUP(A1806, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1807" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1807" s="1" t="str">
-        <f>IF(A1807="", "", VLOOKUP(A1807, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1808" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1808" s="1" t="str">
-        <f>IF(A1808="", "", VLOOKUP(A1808, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1809" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1809" s="1" t="str">
-        <f>IF(A1809="", "", VLOOKUP(A1809, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1810" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1810" s="1" t="str">
-        <f>IF(A1810="", "", VLOOKUP(A1810, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1811" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1811" s="1" t="str">
-        <f>IF(A1811="", "", VLOOKUP(A1811, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1812" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1812" s="1" t="str">
-        <f>IF(A1812="", "", VLOOKUP(A1812, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1813" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1813" s="1" t="str">
-        <f>IF(A1813="", "", VLOOKUP(A1813, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1814" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1814" s="1" t="str">
-        <f>IF(A1814="", "", VLOOKUP(A1814, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1815" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1815" s="1" t="str">
-        <f>IF(A1815="", "", VLOOKUP(A1815, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1816" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1816" s="1" t="str">
-        <f>IF(A1816="", "", VLOOKUP(A1816, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1817" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1817" s="1" t="str">
-        <f>IF(A1817="", "", VLOOKUP(A1817, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1818" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1818" s="1" t="str">
-        <f>IF(A1818="", "", VLOOKUP(A1818, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1819" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1819" s="1" t="str">
-        <f>IF(A1819="", "", VLOOKUP(A1819, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1820" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1820" s="1" t="str">
-        <f>IF(A1820="", "", VLOOKUP(A1820, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1821" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1821" s="1" t="str">
-        <f>IF(A1821="", "", VLOOKUP(A1821, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1822" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1822" s="1" t="str">
-        <f>IF(A1822="", "", VLOOKUP(A1822, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1823" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1823" s="1" t="str">
-        <f>IF(A1823="", "", VLOOKUP(A1823, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1824" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1824" s="1" t="str">
-        <f>IF(A1824="", "", VLOOKUP(A1824, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1825" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1825" s="1" t="str">
-        <f>IF(A1825="", "", VLOOKUP(A1825, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1826" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1826" s="1" t="str">
-        <f>IF(A1826="", "", VLOOKUP(A1826, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1827" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1827" s="1" t="str">
-        <f>IF(A1827="", "", VLOOKUP(A1827, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1828" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1828" s="1" t="str">
-        <f>IF(A1828="", "", VLOOKUP(A1828, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1829" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1829" s="1" t="str">
-        <f>IF(A1829="", "", VLOOKUP(A1829, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1830" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1830" s="1" t="str">
-        <f>IF(A1830="", "", VLOOKUP(A1830, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1831" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1831" s="1" t="str">
-        <f>IF(A1831="", "", VLOOKUP(A1831, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1832" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1832" s="1" t="str">
-        <f>IF(A1832="", "", VLOOKUP(A1832, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1833" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1833" s="1" t="str">
-        <f>IF(A1833="", "", VLOOKUP(A1833, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1834" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1834" s="1" t="str">
-        <f>IF(A1834="", "", VLOOKUP(A1834, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1835" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1835" s="1" t="str">
-        <f>IF(A1835="", "", VLOOKUP(A1835, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1836" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1836" s="1" t="str">
-        <f>IF(A1836="", "", VLOOKUP(A1836, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1837" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1837" s="1" t="str">
-        <f>IF(A1837="", "", VLOOKUP(A1837, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H1837">
-    <sortCondition ref="G2:G1837"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H1794">
+    <sortCondition ref="G2:G1794"/>
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="2">
@@ -37655,6 +39587,122 @@
     <hyperlink ref="H1227" r:id="rId286" xr:uid="{90B6E38B-E30B-8C47-9389-BF74C0BA8822}"/>
     <hyperlink ref="H1228" r:id="rId287" xr:uid="{89726A7C-9D94-3547-91C5-187D9F48BFC8}"/>
     <hyperlink ref="H1229" r:id="rId288" xr:uid="{C8A856CB-58FC-044F-8495-C77C622ECAE4}"/>
+    <hyperlink ref="H1230" r:id="rId289" xr:uid="{C4B9D6AB-6678-674F-8A66-51829021C717}"/>
+    <hyperlink ref="H1231" r:id="rId290" xr:uid="{AC42F576-33F4-1249-B993-0B750D5660A0}"/>
+    <hyperlink ref="H1232" r:id="rId291" xr:uid="{19D53961-2154-5248-9797-F99F9A3A5093}"/>
+    <hyperlink ref="H1233" r:id="rId292" xr:uid="{61042EC8-944B-544C-BEAD-0CEB20EC4D33}"/>
+    <hyperlink ref="H1234" r:id="rId293" xr:uid="{5277A271-CD35-BC4C-9C9F-64C901A2592F}"/>
+    <hyperlink ref="H1235" r:id="rId294" xr:uid="{ED5DA2F9-D44F-F544-8B4A-DD375F0B33F7}"/>
+    <hyperlink ref="H1236" r:id="rId295" xr:uid="{0F352EE0-EB85-4E49-823C-6400314AD599}"/>
+    <hyperlink ref="H1237" r:id="rId296" xr:uid="{9BCF0971-08F8-3944-BD59-F36A1CB3D39E}"/>
+    <hyperlink ref="H1238" r:id="rId297" xr:uid="{D315A02F-4181-144E-BC12-2DEA4CB8014E}"/>
+    <hyperlink ref="H1239" r:id="rId298" xr:uid="{5AC24D0E-4548-2B44-8F88-54F77900B90C}"/>
+    <hyperlink ref="H1240" r:id="rId299" xr:uid="{4AB999BA-475F-F84A-A3CB-9E29A23D03D3}"/>
+    <hyperlink ref="H1241" r:id="rId300" xr:uid="{04B062D7-1878-034C-B893-973847199BEC}"/>
+    <hyperlink ref="H1242" r:id="rId301" xr:uid="{6D47CD0E-A633-0540-ADDC-CC9ADA13DB56}"/>
+    <hyperlink ref="H1243" r:id="rId302" xr:uid="{17EFF3D9-09C5-CE42-AC95-CFD352A5640E}"/>
+    <hyperlink ref="H1244" r:id="rId303" xr:uid="{FDF07543-6F61-9841-AAEE-51E418D6448D}"/>
+    <hyperlink ref="H1245" r:id="rId304" xr:uid="{C8A05969-2534-A64C-8094-FD236191A8A1}"/>
+    <hyperlink ref="H1246" r:id="rId305" xr:uid="{38213849-8D57-B147-B39B-B19D3ED37C5C}"/>
+    <hyperlink ref="H1247" r:id="rId306" xr:uid="{A3F81FBB-F6B5-6C4E-8B06-DE046D32436C}"/>
+    <hyperlink ref="H1248" r:id="rId307" xr:uid="{AA82C233-9E97-7F4F-A606-1CB5E84DCAA8}"/>
+    <hyperlink ref="H1249" r:id="rId308" xr:uid="{A8BBEDF3-E3A6-CB4D-A92B-DCADE43375D1}"/>
+    <hyperlink ref="H1250" r:id="rId309" xr:uid="{34096634-9550-6247-B2D9-5121A75197B6}"/>
+    <hyperlink ref="H1251" r:id="rId310" xr:uid="{0B41675B-6644-174C-B872-5E65FF4E53F9}"/>
+    <hyperlink ref="H1252" r:id="rId311" xr:uid="{A0C892EF-90FB-9246-BB22-1FA76E20FCC3}"/>
+    <hyperlink ref="H1253" r:id="rId312" xr:uid="{B16B26D0-7EB6-9142-B938-E069FEA766B8}"/>
+    <hyperlink ref="H1254" r:id="rId313" xr:uid="{89A6FB63-5BE1-C947-A862-9F442B2DE5EC}"/>
+    <hyperlink ref="H1255" r:id="rId314" xr:uid="{68628E2C-411F-E34C-A2E2-DDE78D02820F}"/>
+    <hyperlink ref="H1256" r:id="rId315" xr:uid="{6EF66539-6D99-AE4B-A410-25B39B65C14B}"/>
+    <hyperlink ref="H1257" r:id="rId316" xr:uid="{BD7B873E-6A1F-5247-987B-DFA4A0C0E5FE}"/>
+    <hyperlink ref="H1258" r:id="rId317" xr:uid="{50FF2E6F-9E50-4443-AB2D-9DE751EC421B}"/>
+    <hyperlink ref="H1259" r:id="rId318" xr:uid="{E54DCC44-8B67-3941-A355-5B490326CFF9}"/>
+    <hyperlink ref="H1260" r:id="rId319" xr:uid="{9F60311D-F111-4843-B415-03854C321407}"/>
+    <hyperlink ref="H1261" r:id="rId320" xr:uid="{C31799BF-ACCE-1E45-A8DD-1C5FE1126E90}"/>
+    <hyperlink ref="H1262" r:id="rId321" xr:uid="{9B373598-1770-0F46-8D4C-2C499F422DCB}"/>
+    <hyperlink ref="H1263" r:id="rId322" xr:uid="{0E4D8422-3506-684C-BC0D-F8636E279A88}"/>
+    <hyperlink ref="H1264" r:id="rId323" xr:uid="{F94924FC-0858-434F-A686-B6348FC26F9A}"/>
+    <hyperlink ref="H1265" r:id="rId324" xr:uid="{72F30653-C45E-4446-830D-698132EC06EF}"/>
+    <hyperlink ref="H1266" r:id="rId325" xr:uid="{5791A451-449D-5C43-9C2E-4E59D53B600C}"/>
+    <hyperlink ref="H1267" r:id="rId326" xr:uid="{5146C9B3-F95E-3648-8546-8B88F4F263EB}"/>
+    <hyperlink ref="H1268" r:id="rId327" xr:uid="{C5700125-A6D5-B840-9B11-B85B9F3E4B40}"/>
+    <hyperlink ref="H1269" r:id="rId328" xr:uid="{9EDDE0B5-20B5-484B-9AE2-39B5B407725D}"/>
+    <hyperlink ref="H1270" r:id="rId329" xr:uid="{E1988E4C-8E18-4D4D-906F-6B989C073311}"/>
+    <hyperlink ref="H1271" r:id="rId330" xr:uid="{F9509E28-456B-2142-BFCF-19BC7F05EA11}"/>
+    <hyperlink ref="H1272" r:id="rId331" xr:uid="{3DD7EB50-6793-7B45-9FBD-FC434C7045D2}"/>
+    <hyperlink ref="H1273" r:id="rId332" xr:uid="{15A72486-3682-9642-B531-9817FF907B42}"/>
+    <hyperlink ref="H1274" r:id="rId333" xr:uid="{193C93CD-9E1E-8C40-96CB-48F90C81202F}"/>
+    <hyperlink ref="H1275" r:id="rId334" xr:uid="{049E4037-21B8-5D43-97FF-3239F6A0731E}"/>
+    <hyperlink ref="H1276" r:id="rId335" xr:uid="{04E2F783-CD75-4243-8AF1-7A50A46E32E2}"/>
+    <hyperlink ref="H1277" r:id="rId336" xr:uid="{7228F9C9-5CA8-594D-8E60-FA43CEA29EC3}"/>
+    <hyperlink ref="H1278" r:id="rId337" xr:uid="{199BAA7B-7425-BD44-8983-A586AB816B82}"/>
+    <hyperlink ref="H1279" r:id="rId338" xr:uid="{8CC93953-94FF-8745-93E9-B5B483997062}"/>
+    <hyperlink ref="H1280" r:id="rId339" xr:uid="{A338FC83-6882-234B-A34D-9560AAFF25DE}"/>
+    <hyperlink ref="H1281" r:id="rId340" xr:uid="{C7579364-BF50-1B45-A316-31D88D7E925F}"/>
+    <hyperlink ref="H1282" r:id="rId341" xr:uid="{EC90A219-860A-EA4E-93A7-2E222ADD6FC0}"/>
+    <hyperlink ref="H1283" r:id="rId342" xr:uid="{FCF7B885-EC11-4145-A8B2-29D57E564212}"/>
+    <hyperlink ref="H1284" r:id="rId343" xr:uid="{38B99A17-241C-9147-80F5-D78FC1B39945}"/>
+    <hyperlink ref="H1285" r:id="rId344" xr:uid="{4391B04B-0D4A-6F4D-B032-8F8233A887A5}"/>
+    <hyperlink ref="H1286" r:id="rId345" xr:uid="{F3157B48-6009-EF42-8751-887B78A68614}"/>
+    <hyperlink ref="H1287" r:id="rId346" xr:uid="{54CE2715-1122-694E-AC17-85AD1AAB4420}"/>
+    <hyperlink ref="H1288" r:id="rId347" xr:uid="{A5F93E45-B83B-8641-B130-DEB5C13C4B2B}"/>
+    <hyperlink ref="H1289" r:id="rId348" xr:uid="{5CCE232C-F202-3645-8C41-363BC952319D}"/>
+    <hyperlink ref="H1290" r:id="rId349" xr:uid="{BE5E0334-89DB-F144-83FA-B5D46C3E4818}"/>
+    <hyperlink ref="H1291" r:id="rId350" xr:uid="{0175C396-6B14-2A49-B4DA-8D9DA70B03A7}"/>
+    <hyperlink ref="H1292" r:id="rId351" xr:uid="{E0099805-D015-3642-8916-6F64273CA88B}"/>
+    <hyperlink ref="H1293" r:id="rId352" xr:uid="{982B43C9-70E1-6345-BA74-4F19F7BA1959}"/>
+    <hyperlink ref="H1294" r:id="rId353" xr:uid="{1A5614AB-5F80-AC47-AE50-265CF931F3E5}"/>
+    <hyperlink ref="H1295" r:id="rId354" xr:uid="{1398019E-DA2D-234C-B80F-D454A4F2F09F}"/>
+    <hyperlink ref="H1296" r:id="rId355" xr:uid="{8923D099-4C5D-FD40-8AD6-AA684336E62A}"/>
+    <hyperlink ref="H1297" r:id="rId356" xr:uid="{D1CF93D0-1844-A948-BF43-7E266829862D}"/>
+    <hyperlink ref="H1298" r:id="rId357" xr:uid="{C14AAFC6-6CE9-CF48-A5EB-53FE9ECE0CC7}"/>
+    <hyperlink ref="H1299" r:id="rId358" xr:uid="{C08EA976-D382-1C40-8D75-FC2A660CF893}"/>
+    <hyperlink ref="H1300" r:id="rId359" xr:uid="{623536C5-1FAE-014C-87E1-C00D62A6C391}"/>
+    <hyperlink ref="H1301" r:id="rId360" xr:uid="{771A0034-26E1-F64B-944A-F3563B4B0A56}"/>
+    <hyperlink ref="H1302" r:id="rId361" xr:uid="{D8FF8F41-6B15-454C-9FFF-6626DA9EA62F}"/>
+    <hyperlink ref="H1303" r:id="rId362" xr:uid="{8F817AD9-4F9C-6E45-A4B4-D9FF8404A398}"/>
+    <hyperlink ref="H1304" r:id="rId363" xr:uid="{9D656168-5DB0-2640-9022-C92942AB6986}"/>
+    <hyperlink ref="H1305" r:id="rId364" xr:uid="{DE8C94F4-87AE-4047-9E33-6FDB5BE34365}"/>
+    <hyperlink ref="H1306" r:id="rId365" xr:uid="{B14E458B-AAC8-3E49-AC54-5599CF8869AF}"/>
+    <hyperlink ref="H1307" r:id="rId366" xr:uid="{1FA3E185-504E-784A-9651-757579A7C215}"/>
+    <hyperlink ref="H1308" r:id="rId367" xr:uid="{20451F6D-44BB-2544-AE62-0F7757B51541}"/>
+    <hyperlink ref="H1309" r:id="rId368" xr:uid="{85418F5B-ABF5-E848-9C00-7CBA82AB53C6}"/>
+    <hyperlink ref="H1310" r:id="rId369" xr:uid="{6196DCC7-0F85-264E-B2E6-EE88EC3932DF}"/>
+    <hyperlink ref="H1311" r:id="rId370" xr:uid="{07E2354E-DF3B-1848-8BBF-AAF3CD5B9B53}"/>
+    <hyperlink ref="H1312" r:id="rId371" xr:uid="{9C8D9C0A-C7A6-3049-AB80-C9918539EDF8}"/>
+    <hyperlink ref="H1313" r:id="rId372" xr:uid="{D82D4F3D-27BE-F94E-8DFF-8577A2E7FAD1}"/>
+    <hyperlink ref="H1314" r:id="rId373" xr:uid="{C34E79C2-F542-6E4A-99B6-4393596BBD55}"/>
+    <hyperlink ref="H1315" r:id="rId374" xr:uid="{076FA58C-8E2F-C54C-8CD3-D2C1A92DD01F}"/>
+    <hyperlink ref="H1316" r:id="rId375" xr:uid="{DB7D9306-EA34-7845-8ECF-F07BF817160C}"/>
+    <hyperlink ref="H1317" r:id="rId376" xr:uid="{2D6D390F-9BEC-E846-BF5A-04468389F078}"/>
+    <hyperlink ref="H1318" r:id="rId377" xr:uid="{BB4D0BDF-0B0F-AB40-A67E-EBB7C470C55B}"/>
+    <hyperlink ref="H1319" r:id="rId378" xr:uid="{36F9FC08-49E0-FE43-9E71-291CE63DC067}"/>
+    <hyperlink ref="H1320" r:id="rId379" xr:uid="{9C4E0203-86B5-4643-BE58-54D2785AD7C5}"/>
+    <hyperlink ref="H1321" r:id="rId380" xr:uid="{9B12D740-3537-FA47-868E-386791254F29}"/>
+    <hyperlink ref="H1322" r:id="rId381" xr:uid="{D34C889F-A6F8-3C47-BD33-FC4CE31F456E}"/>
+    <hyperlink ref="H1323" r:id="rId382" xr:uid="{61BE1C88-E6B3-7842-9844-E8AB5EAD182C}"/>
+    <hyperlink ref="H1324" r:id="rId383" xr:uid="{60147E03-C1CD-FE4F-B7B3-5E86F2D75F9E}"/>
+    <hyperlink ref="H1325" r:id="rId384" xr:uid="{29B6ECA7-E73D-D844-9ECB-A3A4EACF2B2B}"/>
+    <hyperlink ref="H1326" r:id="rId385" xr:uid="{6A91D879-D2A6-DA44-98DC-D382C30FF8E0}"/>
+    <hyperlink ref="H1327" r:id="rId386" xr:uid="{A7AAC4B9-CE12-034E-81AE-99DCB689EF9D}"/>
+    <hyperlink ref="H1328" r:id="rId387" xr:uid="{A2E2851E-24E8-8040-AFF6-8D7E20E3EF1A}"/>
+    <hyperlink ref="H1329" r:id="rId388" xr:uid="{4F5D3A85-3288-5442-8AF1-94DF0EC622F0}"/>
+    <hyperlink ref="H1330" r:id="rId389" xr:uid="{12BFBCB8-76E0-1D48-922E-93C4C395726C}"/>
+    <hyperlink ref="H1331" r:id="rId390" xr:uid="{FEE983F4-2A50-D746-97A2-2E66CDDFA085}"/>
+    <hyperlink ref="H1332" r:id="rId391" xr:uid="{02148E0C-F833-AE4A-A9C9-5EF716CFD6D8}"/>
+    <hyperlink ref="H1333" r:id="rId392" xr:uid="{D0CC1D42-7A94-2F47-A143-168A7E62C356}"/>
+    <hyperlink ref="H1334" r:id="rId393" xr:uid="{312D2048-DCF7-4A47-A9A9-A737DBF20F3D}"/>
+    <hyperlink ref="H1335" r:id="rId394" xr:uid="{CAE69AE2-DD2A-D54A-A8A5-51388E519A54}"/>
+    <hyperlink ref="H1336" r:id="rId395" xr:uid="{45A47DF8-B5D2-5B41-8425-A31F44B1E599}"/>
+    <hyperlink ref="H1337" r:id="rId396" xr:uid="{C44D8B16-EA19-E34F-9EE1-49AA9589A20D}"/>
+    <hyperlink ref="H1338" r:id="rId397" xr:uid="{6A136BC4-6C8E-0647-8552-5A457D2D0249}"/>
+    <hyperlink ref="H1339" r:id="rId398" xr:uid="{81CA2DF1-D439-B34B-9F99-3B072694796B}"/>
+    <hyperlink ref="H1340" r:id="rId399" xr:uid="{128C846B-C38A-604B-AC61-9AE34861EA1E}"/>
+    <hyperlink ref="H1341" r:id="rId400" xr:uid="{0E71662C-B08B-8943-B217-2423E385E074}"/>
+    <hyperlink ref="H1342" r:id="rId401" xr:uid="{0FCD3A12-DFDE-3045-8A1A-B59B1ECD46B3}"/>
+    <hyperlink ref="H1343" r:id="rId402" xr:uid="{52575CEA-8663-2E46-9D03-C3CFB034DAAB}"/>
+    <hyperlink ref="H1344" r:id="rId403" xr:uid="{D519A24D-BF84-7140-85EE-DABD71B51B4E}"/>
+    <hyperlink ref="H1345" r:id="rId404" xr:uid="{1A77FB89-E8CE-9743-9797-E296C6278FBE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
Added ph-4 models and benchmarks
</commit_message>
<xml_diff>
--- a/data/benchmarks.xlsx
+++ b/data/benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sean/Coding/genai-explorer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F718EDA5-C036-E449-B09D-BA0EDF1B99C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63DFA79-3EAC-9145-81E5-37A836D9037F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="57600" windowHeight="32400" xr2:uid="{683877ED-707A-FC42-8592-F58A6955B3A6}"/>
+    <workbookView xWindow="57600" yWindow="0" windowWidth="60160" windowHeight="33840" activeTab="2" xr2:uid="{683877ED-707A-FC42-8592-F58A6955B3A6}"/>
   </bookViews>
   <sheets>
     <sheet name="model-meta" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6123" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6410" uniqueCount="370">
   <si>
     <t>model_id</t>
   </si>
@@ -1124,6 +1124,36 @@
   <si>
     <t>google-deepmind</t>
   </si>
+  <si>
+    <t>Phi-4 Reasoning announcement</t>
+  </si>
+  <si>
+    <t>https://azure.microsoft.com/en-us/blog/one-year-of-phi-small-language-models-making-big-leaps-in-ai/</t>
+  </si>
+  <si>
+    <t>phi-4-reasoning-plus</t>
+  </si>
+  <si>
+    <t>phi-4-reasoning</t>
+  </si>
+  <si>
+    <t>phi-4-mini-reasoning</t>
+  </si>
+  <si>
+    <t>phi-4-mini</t>
+  </si>
+  <si>
+    <t>https://huggingface.co/microsoft/Phi-4-reasoning-plus</t>
+  </si>
+  <si>
+    <t>Plus</t>
+  </si>
+  <si>
+    <t>Strict</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/pdf/2504.21318</t>
+  </si>
 </sst>
 </file>
 
@@ -1244,7 +1274,18 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1574,10 +1615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5579D913-ECD6-6A42-858D-C12502E32020}">
-  <dimension ref="A1:B70"/>
+  <dimension ref="A1:B74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:B36"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2143,6 +2184,38 @@
         <v>335</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>362</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>363</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>364</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>365</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>330</v>
       </c>
     </row>
@@ -3084,11 +3157,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A72D42-DDBC-2B44-AB6C-55AD4AA1061B}">
-  <dimension ref="A1:H1794"/>
+  <dimension ref="A1:H1735"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1308" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1333" sqref="E1333"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1353" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1385" sqref="C1385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36464,474 +36537,1713 @@
       </c>
     </row>
     <row r="1346" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1346" s="2" t="s">
+        <v>173</v>
+      </c>
       <c r="B1346" s="1" t="str">
         <f>IF(A1346="", "", VLOOKUP(A1346, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1346" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1346" s="12">
+        <v>74.5</v>
+      </c>
+      <c r="E1346" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1346" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1346" s="13" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="1347" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1347" s="2" t="s">
+        <v>343</v>
+      </c>
       <c r="B1347" s="1" t="str">
         <f>IF(A1347="", "", VLOOKUP(A1347, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>microsoft</v>
+      </c>
+      <c r="C1347" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1347" s="12">
+        <v>28</v>
+      </c>
+      <c r="E1347" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1347" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1347" s="13" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="1348" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1348" s="2" t="s">
+        <v>173</v>
+      </c>
       <c r="B1348" s="1" t="str">
         <f>IF(A1348="", "", VLOOKUP(A1348, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1348" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1348" s="12">
+        <v>60.7</v>
+      </c>
+      <c r="E1348" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1348" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1348" s="13" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="1349" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1349" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="B1349" s="1" t="str">
         <f>IF(A1349="", "", VLOOKUP(A1349, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>openai</v>
+      </c>
+      <c r="C1349" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1349" s="12">
+        <v>82.5</v>
+      </c>
+      <c r="E1349" s="4">
+        <v>45777</v>
+      </c>
+      <c r="F1349" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1349" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1349" s="13" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="1350" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1350" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="B1350" s="1" t="str">
         <f>IF(A1350="", "", VLOOKUP(A1350, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>deepseek</v>
+      </c>
+      <c r="C1350" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1350" s="12">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="E1350" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1350" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1350" s="13" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="1351" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1351" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="B1351" s="1" t="str">
         <f>IF(A1351="", "", VLOOKUP(A1351, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>openai</v>
+      </c>
+      <c r="C1351" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1351" s="12">
+        <v>1891</v>
+      </c>
+      <c r="E1351" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1351" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1351" s="13" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="1352" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1352" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="B1352" s="1" t="str">
         <f>IF(A1352="", "", VLOOKUP(A1352, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>openai</v>
+      </c>
+      <c r="C1352" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1352" s="12">
+        <v>1650</v>
+      </c>
+      <c r="E1352" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1352" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1352" s="13" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="1353" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1353" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="B1353" s="1" t="str">
         <f>IF(A1353="", "", VLOOKUP(A1353, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>openai</v>
+      </c>
+      <c r="C1353" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1353" s="12">
+        <v>2130</v>
+      </c>
+      <c r="E1353" s="4">
+        <v>45777</v>
+      </c>
+      <c r="F1353" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1353" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1353" s="13" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="1354" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1354" s="2" t="s">
+        <v>363</v>
+      </c>
       <c r="B1354" s="1" t="str">
         <f>IF(A1354="", "", VLOOKUP(A1354, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>microsoft</v>
+      </c>
+      <c r="C1354" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1354" s="12">
+        <v>1736</v>
+      </c>
+      <c r="E1354" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1354" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1354" s="13" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="1355" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1355" s="2" t="s">
+        <v>362</v>
+      </c>
       <c r="B1355" s="1" t="str">
         <f>IF(A1355="", "", VLOOKUP(A1355, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>microsoft</v>
+      </c>
+      <c r="C1355" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1355" s="12">
+        <v>1723</v>
+      </c>
+      <c r="E1355" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1355" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1355" s="13" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="1356" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1356" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="B1356" s="1" t="str">
         <f>IF(A1356="", "", VLOOKUP(A1356, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>deepseek</v>
+      </c>
+      <c r="C1356" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1356" s="12">
+        <v>2029</v>
+      </c>
+      <c r="E1356" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1356" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1356" s="13" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="1357" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1357" s="2" t="s">
+        <v>173</v>
+      </c>
       <c r="B1357" s="1" t="str">
         <f>IF(A1357="", "", VLOOKUP(A1357, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1357" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1357" s="12">
+        <v>72</v>
+      </c>
+      <c r="E1357" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1357" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1357" s="13" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="1358" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1358" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="B1358" s="1" t="str">
         <f>IF(A1358="", "", VLOOKUP(A1358, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>openai</v>
+      </c>
+      <c r="C1358" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1358" s="12">
+        <v>63.6</v>
+      </c>
+      <c r="E1358" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1358" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1358" s="13" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="1359" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1359" s="2" t="s">
+        <v>365</v>
+      </c>
       <c r="B1359" s="1" t="str">
         <f>IF(A1359="", "", VLOOKUP(A1359, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>microsoft</v>
+      </c>
+      <c r="C1359" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1359" s="12">
+        <v>10</v>
+      </c>
+      <c r="E1359" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1359" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1359" s="13" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="1360" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1360" s="2" t="s">
+        <v>364</v>
+      </c>
       <c r="B1360" s="1" t="str">
         <f>IF(A1360="", "", VLOOKUP(A1360, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1361" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1360" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1360" s="12">
+        <v>57.5</v>
+      </c>
+      <c r="E1360" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1360" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1360" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1361" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1361" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="B1361" s="1" t="str">
         <f>IF(A1361="", "", VLOOKUP(A1361, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1362" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1361" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1361" s="12">
+        <v>54.8</v>
+      </c>
+      <c r="E1361" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1361" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1361" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1362" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1362" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="B1362" s="1" t="str">
         <f>IF(A1362="", "", VLOOKUP(A1362, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1363" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1362" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1362" s="12">
+        <v>82.5</v>
+      </c>
+      <c r="E1362" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1362" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1362" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1363" s="2" t="s">
+        <v>343</v>
+      </c>
       <c r="B1363" s="1" t="str">
         <f>IF(A1363="", "", VLOOKUP(A1363, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1364" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1363" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1363" s="12">
+        <v>12.9</v>
+      </c>
+      <c r="E1363" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1363" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1363" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1364" s="2" t="s">
+        <v>363</v>
+      </c>
       <c r="B1364" s="1" t="str">
         <f>IF(A1364="", "", VLOOKUP(A1364, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1365" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1364" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1364" s="12">
+        <v>63.1</v>
+      </c>
+      <c r="E1364" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1364" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1364" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1365" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1365" s="2" t="s">
+        <v>362</v>
+      </c>
       <c r="B1365" s="1" t="str">
         <f>IF(A1365="", "", VLOOKUP(A1365, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1366" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1365" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1365" s="12">
+        <v>78</v>
+      </c>
+      <c r="E1365" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1365" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1365" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1366" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1366" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="B1366" s="1" t="str">
         <f>IF(A1366="", "", VLOOKUP(A1366, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1367" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1366" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1366" s="12">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="E1366" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1366" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1366" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1367" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1367" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="B1367" s="1" t="str">
         <f>IF(A1367="", "", VLOOKUP(A1367, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1368" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1367" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1367" s="12">
+        <v>60</v>
+      </c>
+      <c r="E1367" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1367" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1367" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1368" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1368" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="B1368" s="1" t="str">
         <f>IF(A1368="", "", VLOOKUP(A1368, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1369" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1368" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1368" s="12">
+        <v>77.7</v>
+      </c>
+      <c r="E1368" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1368" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1368" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1369" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1369" s="2" t="s">
+        <v>343</v>
+      </c>
       <c r="B1369" s="1" t="str">
         <f>IF(A1369="", "", VLOOKUP(A1369, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1370" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1369" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1369" s="12">
+        <v>54.7</v>
+      </c>
+      <c r="E1369" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1369" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1369" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1370" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1370" s="2" t="s">
+        <v>365</v>
+      </c>
       <c r="B1370" s="1" t="str">
         <f>IF(A1370="", "", VLOOKUP(A1370, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1371" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1370" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1370" s="12">
+        <v>36.9</v>
+      </c>
+      <c r="E1370" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1370" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1370" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1371" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1371" s="2" t="s">
+        <v>364</v>
+      </c>
       <c r="B1371" s="1" t="str">
         <f>IF(A1371="", "", VLOOKUP(A1371, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1372" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1371" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1371" s="12">
+        <v>52</v>
+      </c>
+      <c r="E1371" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1371" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1371" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1372" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1372" s="2" t="s">
+        <v>363</v>
+      </c>
       <c r="B1372" s="1" t="str">
         <f>IF(A1372="", "", VLOOKUP(A1372, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1373" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1372" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1372" s="12">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="E1372" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1372" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1372" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1373" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1373" s="2" t="s">
+        <v>362</v>
+      </c>
       <c r="B1373" s="1" t="str">
         <f>IF(A1373="", "", VLOOKUP(A1373, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1374" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1373" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1373" s="12">
+        <v>69.3</v>
+      </c>
+      <c r="E1373" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1373" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1373" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1374" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1374" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="B1374" s="1" t="str">
         <f>IF(A1374="", "", VLOOKUP(A1374, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1375" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1374" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1374" s="12">
+        <v>73</v>
+      </c>
+      <c r="E1374" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1374" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1374" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1375" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1375" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B1375" s="1" t="str">
         <f>IF(A1375="", "", VLOOKUP(A1375, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1376" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1375" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1375" s="12">
+        <v>84.9</v>
+      </c>
+      <c r="E1375" s="4">
+        <v>45777</v>
+      </c>
+      <c r="F1375" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="G1375" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1375" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1376" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1376" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="B1376" s="1" t="str">
         <f>IF(A1376="", "", VLOOKUP(A1376, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1377" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1376" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1376" s="12">
+        <v>94</v>
+      </c>
+      <c r="E1376" s="4">
+        <v>45777</v>
+      </c>
+      <c r="F1376" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="G1376" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1376" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1377" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1377" s="2" t="s">
+        <v>343</v>
+      </c>
       <c r="B1377" s="1" t="str">
         <f>IF(A1377="", "", VLOOKUP(A1377, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1378" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1377" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1377" s="12">
+        <v>83.5</v>
+      </c>
+      <c r="E1377" s="4">
+        <v>45777</v>
+      </c>
+      <c r="F1377" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="G1377" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1377" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1378" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1378" s="2" t="s">
+        <v>363</v>
+      </c>
       <c r="B1378" s="1" t="str">
         <f>IF(A1378="", "", VLOOKUP(A1378, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1379" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1378" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1378" s="12">
+        <v>92.9</v>
+      </c>
+      <c r="E1378" s="4">
+        <v>45777</v>
+      </c>
+      <c r="F1378" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="G1378" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1378" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1379" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1379" s="2" t="s">
+        <v>362</v>
+      </c>
       <c r="B1379" s="1" t="str">
         <f>IF(A1379="", "", VLOOKUP(A1379, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1380" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1379" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1379" s="12">
+        <v>92.3</v>
+      </c>
+      <c r="E1379" s="4">
+        <v>45777</v>
+      </c>
+      <c r="F1379" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="G1379" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1379" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1380" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1380" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B1380" s="1" t="str">
         <f>IF(A1380="", "", VLOOKUP(A1380, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1381" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1380" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1380" s="12">
+        <v>81.8</v>
+      </c>
+      <c r="E1380" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1380" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1380" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1381" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="B1381" s="1" t="str">
         <f>IF(A1381="", "", VLOOKUP(A1381, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1382" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1381" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1381" s="12">
+        <v>91.5</v>
+      </c>
+      <c r="E1381" s="4">
+        <v>45777</v>
+      </c>
+      <c r="F1381" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="G1381" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1381" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1382" s="2" t="s">
+        <v>343</v>
+      </c>
       <c r="B1382" s="1" t="str">
         <f>IF(A1382="", "", VLOOKUP(A1382, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1383" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1382" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1382" s="12">
+        <v>62.3</v>
+      </c>
+      <c r="E1382" s="4">
+        <v>45777</v>
+      </c>
+      <c r="F1382" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="G1382" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1382" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1383" s="2" t="s">
+        <v>363</v>
+      </c>
       <c r="B1383" s="1" t="str">
         <f>IF(A1383="", "", VLOOKUP(A1383, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1384" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1383" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1383" s="12">
+        <v>83.4</v>
+      </c>
+      <c r="E1383" s="4">
+        <v>45777</v>
+      </c>
+      <c r="F1383" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="G1383" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1383" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1384" s="2" t="s">
+        <v>362</v>
+      </c>
       <c r="B1384" s="1" t="str">
         <f>IF(A1384="", "", VLOOKUP(A1384, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1385" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1384" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1384" s="12">
+        <v>84.9</v>
+      </c>
+      <c r="E1384" s="4">
+        <v>45777</v>
+      </c>
+      <c r="F1384" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="G1384" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1384" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1385" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1385" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="B1385" s="1" t="str">
         <f>IF(A1385="", "", VLOOKUP(A1385, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1386" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1385" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1385" s="12">
+        <v>90</v>
+      </c>
+      <c r="E1385" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1385" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1385" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1386" s="2" t="s">
+        <v>365</v>
+      </c>
       <c r="B1386" s="1" t="str">
         <f>IF(A1386="", "", VLOOKUP(A1386, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1387" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1386" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1386" s="12">
+        <v>71.8</v>
+      </c>
+      <c r="E1386" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1386" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1386" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1387" s="2" t="s">
+        <v>364</v>
+      </c>
       <c r="B1387" s="1" t="str">
         <f>IF(A1387="", "", VLOOKUP(A1387, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1388" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1387" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1387" s="12">
+        <v>94.6</v>
+      </c>
+      <c r="E1387" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1387" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1387" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1388" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B1388" s="1" t="str">
         <f>IF(A1388="", "", VLOOKUP(A1388, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1389" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1388" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1388" s="12">
+        <v>73.5</v>
+      </c>
+      <c r="E1388" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1388" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1388" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1389" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="B1389" s="1" t="str">
         <f>IF(A1389="", "", VLOOKUP(A1389, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1390" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1389" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1389" s="12">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="E1389" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1389" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1389" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1390" s="2" t="s">
+        <v>343</v>
+      </c>
       <c r="B1390" s="1" t="str">
         <f>IF(A1390="", "", VLOOKUP(A1390, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1391" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1390" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1390" s="12">
+        <v>71.5</v>
+      </c>
+      <c r="E1390" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1390" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1390" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1391" s="2" t="s">
+        <v>363</v>
+      </c>
       <c r="B1391" s="1" t="str">
         <f>IF(A1391="", "", VLOOKUP(A1391, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1392" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1391" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1391" s="12">
+        <v>74.3</v>
+      </c>
+      <c r="E1391" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1391" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1391" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1392" s="2" t="s">
+        <v>362</v>
+      </c>
       <c r="B1392" s="1" t="str">
         <f>IF(A1392="", "", VLOOKUP(A1392, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1393" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1392" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1392" s="12">
+        <v>76</v>
+      </c>
+      <c r="E1392" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1392" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1392" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1393" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="B1393" s="1" t="str">
         <f>IF(A1393="", "", VLOOKUP(A1393, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1394" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1393" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1393" s="12">
+        <v>55.3</v>
+      </c>
+      <c r="E1393" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1393" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1393" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1394" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="B1394" s="1" t="str">
         <f>IF(A1394="", "", VLOOKUP(A1394, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1395" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1394" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1394" s="12">
+        <v>92</v>
+      </c>
+      <c r="E1394" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1394" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1394" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1395" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="B1395" s="1" t="str">
         <f>IF(A1395="", "", VLOOKUP(A1395, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1396" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1395" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1395" s="12">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="E1395" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1395" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1395" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1396" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="B1396" s="1" t="str">
         <f>IF(A1396="", "", VLOOKUP(A1396, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1397" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1396" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1396" s="12">
+        <v>88</v>
+      </c>
+      <c r="E1396" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1396" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1396" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1397" s="2" t="s">
+        <v>363</v>
+      </c>
       <c r="B1397" s="1" t="str">
         <f>IF(A1397="", "", VLOOKUP(A1397, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1398" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1397" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1397" s="12">
+        <v>75.3</v>
+      </c>
+      <c r="E1397" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1397" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1397" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1398" s="2" t="s">
+        <v>362</v>
+      </c>
       <c r="B1398" s="1" t="str">
         <f>IF(A1398="", "", VLOOKUP(A1398, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1399" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1398" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1398" s="12">
+        <v>81.3</v>
+      </c>
+      <c r="E1398" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1398" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1398" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1399" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="B1399" s="1" t="str">
         <f>IF(A1399="", "", VLOOKUP(A1399, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1400" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1399" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1399" s="12">
+        <v>78.7</v>
+      </c>
+      <c r="E1399" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1399" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1399" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1400" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="B1400" s="1" t="str">
         <f>IF(A1400="", "", VLOOKUP(A1400, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1401" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1400" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1400" s="12">
+        <v>58.7</v>
+      </c>
+      <c r="E1400" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1400" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1400" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1401" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="B1401" s="1" t="str">
         <f>IF(A1401="", "", VLOOKUP(A1401, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1402" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1401" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1401" s="12">
+        <v>86.7</v>
+      </c>
+      <c r="E1401" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1401" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1401" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1402" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="B1402" s="1" t="str">
         <f>IF(A1402="", "", VLOOKUP(A1402, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1403" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1402" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1402" s="12">
+        <v>75.3</v>
+      </c>
+      <c r="E1402" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1402" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1402" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1403" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="B1403" s="1" t="str">
         <f>IF(A1403="", "", VLOOKUP(A1403, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1404" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1403" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1403" s="12">
+        <v>76.8</v>
+      </c>
+      <c r="E1403" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1403" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1403" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1404" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="B1404" s="1" t="str">
         <f>IF(A1404="", "", VLOOKUP(A1404, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1405" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1404" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1404" s="12">
+        <v>84</v>
+      </c>
+      <c r="E1404" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1404" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1404" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1405" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="B1405" s="1" t="str">
         <f>IF(A1405="", "", VLOOKUP(A1405, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1406" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1405" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1405" s="12">
+        <v>76.7</v>
+      </c>
+      <c r="E1405" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1405" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1405" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1406" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="B1406" s="1" t="str">
         <f>IF(A1406="", "", VLOOKUP(A1406, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1407" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1406" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D1406" s="12">
+        <v>69.2</v>
+      </c>
+      <c r="E1406" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1406" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1406" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1407" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="B1407" s="1" t="str">
         <f>IF(A1407="", "", VLOOKUP(A1407, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1408" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1407" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D1407" s="12">
+        <v>71</v>
+      </c>
+      <c r="E1407" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1407" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1407" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1408" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="B1408" s="1" t="str">
         <f>IF(A1408="", "", VLOOKUP(A1408, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1409" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1408" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D1408" s="12">
+        <v>53.8</v>
+      </c>
+      <c r="E1408" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1408" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1408" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1409" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="B1409" s="1" t="str">
         <f>IF(A1409="", "", VLOOKUP(A1409, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1410" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1409" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D1409" s="12">
+        <v>69.5</v>
+      </c>
+      <c r="E1409" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1409" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1409" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1410" s="2" t="s">
+        <v>363</v>
+      </c>
       <c r="B1410" s="1" t="str">
         <f>IF(A1410="", "", VLOOKUP(A1410, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1411" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1410" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D1410" s="12">
+        <v>53.8</v>
+      </c>
+      <c r="E1410" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1410" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1410" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1411" s="2" t="s">
+        <v>362</v>
+      </c>
       <c r="B1411" s="1" t="str">
         <f>IF(A1411="", "", VLOOKUP(A1411, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1412" spans="2:2" x14ac:dyDescent="0.2">
+        <v>microsoft</v>
+      </c>
+      <c r="C1411" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D1411" s="12">
+        <v>53.1</v>
+      </c>
+      <c r="E1411" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1411" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1411" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1412" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="B1412" s="1" t="str">
         <f>IF(A1412="", "", VLOOKUP(A1412, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1413" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1412" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D1412" s="12">
+        <v>62.8</v>
+      </c>
+      <c r="E1412" s="4">
+        <v>45777</v>
+      </c>
+      <c r="G1412" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1412" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1413" s="1" t="str">
         <f>IF(A1413="", "", VLOOKUP(A1413, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1414" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1414" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1414" s="1" t="str">
         <f>IF(A1414="", "", VLOOKUP(A1414, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1415" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1415" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1415" s="1" t="str">
         <f>IF(A1415="", "", VLOOKUP(A1415, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1416" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1416" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1416" s="1" t="str">
         <f>IF(A1416="", "", VLOOKUP(A1416, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1417" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1417" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1417" s="1" t="str">
         <f>IF(A1417="", "", VLOOKUP(A1417, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1418" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1418" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1418" s="1" t="str">
         <f>IF(A1418="", "", VLOOKUP(A1418, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1419" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1419" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1419" s="1" t="str">
         <f>IF(A1419="", "", VLOOKUP(A1419, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1420" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1420" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1420" s="1" t="str">
         <f>IF(A1420="", "", VLOOKUP(A1420, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1421" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1421" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1421" s="1" t="str">
         <f>IF(A1421="", "", VLOOKUP(A1421, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1422" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1422" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1422" s="1" t="str">
         <f>IF(A1422="", "", VLOOKUP(A1422, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1423" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1423" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1423" s="1" t="str">
         <f>IF(A1423="", "", VLOOKUP(A1423, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1424" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1424" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1424" s="1" t="str">
         <f>IF(A1424="", "", VLOOKUP(A1424, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
@@ -38803,366 +40115,11 @@
         <v/>
       </c>
     </row>
-    <row r="1736" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1736" s="1" t="str">
-        <f>IF(A1736="", "", VLOOKUP(A1736, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1737" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1737" s="1" t="str">
-        <f>IF(A1737="", "", VLOOKUP(A1737, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1738" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1738" s="1" t="str">
-        <f>IF(A1738="", "", VLOOKUP(A1738, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1739" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1739" s="1" t="str">
-        <f>IF(A1739="", "", VLOOKUP(A1739, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1740" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1740" s="1" t="str">
-        <f>IF(A1740="", "", VLOOKUP(A1740, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1741" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1741" s="1" t="str">
-        <f>IF(A1741="", "", VLOOKUP(A1741, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1742" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1742" s="1" t="str">
-        <f>IF(A1742="", "", VLOOKUP(A1742, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1743" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1743" s="1" t="str">
-        <f>IF(A1743="", "", VLOOKUP(A1743, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1744" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1744" s="1" t="str">
-        <f>IF(A1744="", "", VLOOKUP(A1744, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1745" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1745" s="1" t="str">
-        <f>IF(A1745="", "", VLOOKUP(A1745, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1746" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1746" s="1" t="str">
-        <f>IF(A1746="", "", VLOOKUP(A1746, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1747" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1747" s="1" t="str">
-        <f>IF(A1747="", "", VLOOKUP(A1747, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1748" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1748" s="1" t="str">
-        <f>IF(A1748="", "", VLOOKUP(A1748, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1749" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1749" s="1" t="str">
-        <f>IF(A1749="", "", VLOOKUP(A1749, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1750" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1750" s="1" t="str">
-        <f>IF(A1750="", "", VLOOKUP(A1750, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1751" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1751" s="1" t="str">
-        <f>IF(A1751="", "", VLOOKUP(A1751, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1752" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1752" s="1" t="str">
-        <f>IF(A1752="", "", VLOOKUP(A1752, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1753" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1753" s="1" t="str">
-        <f>IF(A1753="", "", VLOOKUP(A1753, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1754" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1754" s="1" t="str">
-        <f>IF(A1754="", "", VLOOKUP(A1754, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1755" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1755" s="1" t="str">
-        <f>IF(A1755="", "", VLOOKUP(A1755, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1756" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1756" s="1" t="str">
-        <f>IF(A1756="", "", VLOOKUP(A1756, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1757" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1757" s="1" t="str">
-        <f>IF(A1757="", "", VLOOKUP(A1757, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1758" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1758" s="1" t="str">
-        <f>IF(A1758="", "", VLOOKUP(A1758, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1759" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1759" s="1" t="str">
-        <f>IF(A1759="", "", VLOOKUP(A1759, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1760" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1760" s="1" t="str">
-        <f>IF(A1760="", "", VLOOKUP(A1760, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1761" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1761" s="1" t="str">
-        <f>IF(A1761="", "", VLOOKUP(A1761, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1762" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1762" s="1" t="str">
-        <f>IF(A1762="", "", VLOOKUP(A1762, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1763" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1763" s="1" t="str">
-        <f>IF(A1763="", "", VLOOKUP(A1763, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1764" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1764" s="1" t="str">
-        <f>IF(A1764="", "", VLOOKUP(A1764, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1765" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1765" s="1" t="str">
-        <f>IF(A1765="", "", VLOOKUP(A1765, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1766" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1766" s="1" t="str">
-        <f>IF(A1766="", "", VLOOKUP(A1766, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1767" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1767" s="1" t="str">
-        <f>IF(A1767="", "", VLOOKUP(A1767, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1768" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1768" s="1" t="str">
-        <f>IF(A1768="", "", VLOOKUP(A1768, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1769" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1769" s="1" t="str">
-        <f>IF(A1769="", "", VLOOKUP(A1769, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1770" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1770" s="1" t="str">
-        <f>IF(A1770="", "", VLOOKUP(A1770, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1771" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1771" s="1" t="str">
-        <f>IF(A1771="", "", VLOOKUP(A1771, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1772" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1772" s="1" t="str">
-        <f>IF(A1772="", "", VLOOKUP(A1772, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1773" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1773" s="1" t="str">
-        <f>IF(A1773="", "", VLOOKUP(A1773, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1774" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1774" s="1" t="str">
-        <f>IF(A1774="", "", VLOOKUP(A1774, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1775" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1775" s="1" t="str">
-        <f>IF(A1775="", "", VLOOKUP(A1775, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1776" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1776" s="1" t="str">
-        <f>IF(A1776="", "", VLOOKUP(A1776, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1777" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1777" s="1" t="str">
-        <f>IF(A1777="", "", VLOOKUP(A1777, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1778" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1778" s="1" t="str">
-        <f>IF(A1778="", "", VLOOKUP(A1778, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1779" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1779" s="1" t="str">
-        <f>IF(A1779="", "", VLOOKUP(A1779, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1780" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1780" s="1" t="str">
-        <f>IF(A1780="", "", VLOOKUP(A1780, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1781" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1781" s="1" t="str">
-        <f>IF(A1781="", "", VLOOKUP(A1781, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1782" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1782" s="1" t="str">
-        <f>IF(A1782="", "", VLOOKUP(A1782, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1783" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1783" s="1" t="str">
-        <f>IF(A1783="", "", VLOOKUP(A1783, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1784" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1784" s="1" t="str">
-        <f>IF(A1784="", "", VLOOKUP(A1784, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1785" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1785" s="1" t="str">
-        <f>IF(A1785="", "", VLOOKUP(A1785, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1786" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1786" s="1" t="str">
-        <f>IF(A1786="", "", VLOOKUP(A1786, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1787" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1787" s="1" t="str">
-        <f>IF(A1787="", "", VLOOKUP(A1787, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1788" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1788" s="1" t="str">
-        <f>IF(A1788="", "", VLOOKUP(A1788, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1789" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1789" s="1" t="str">
-        <f>IF(A1789="", "", VLOOKUP(A1789, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1790" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1790" s="1" t="str">
-        <f>IF(A1790="", "", VLOOKUP(A1790, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1791" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1791" s="1" t="str">
-        <f>IF(A1791="", "", VLOOKUP(A1791, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1792" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1792" s="1" t="str">
-        <f>IF(A1792="", "", VLOOKUP(A1792, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1793" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1793" s="1" t="str">
-        <f>IF(A1793="", "", VLOOKUP(A1793, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1794" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1794" s="1" t="str">
-        <f>IF(A1794="", "", VLOOKUP(A1794, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H1794">
-    <sortCondition ref="E2:E1794"/>
-    <sortCondition ref="C2:C1794"/>
-    <sortCondition ref="B2:B1794"/>
-    <sortCondition ref="A2:A1794"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1346:H1412">
+    <sortCondition ref="H1346:H1412"/>
+    <sortCondition ref="C1346:C1412"/>
+    <sortCondition ref="A1346:A1412"/>
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="2">
@@ -39578,6 +40535,41 @@
     <hyperlink ref="H1285" r:id="rId402" xr:uid="{52575CEA-8663-2E46-9D03-C3CFB034DAAB}"/>
     <hyperlink ref="H1290" r:id="rId403" xr:uid="{D519A24D-BF84-7140-85EE-DABD71B51B4E}"/>
     <hyperlink ref="H1291" r:id="rId404" xr:uid="{1A77FB89-E8CE-9743-9797-E296C6278FBE}"/>
+    <hyperlink ref="H1363" r:id="rId405" xr:uid="{BC8E6DA5-C43E-C145-8F7F-9A8A32B0C4A7}"/>
+    <hyperlink ref="H1364" r:id="rId406" xr:uid="{249FF0EC-8F04-F348-84F4-692D67275368}"/>
+    <hyperlink ref="H1365" r:id="rId407" xr:uid="{D6610A69-9095-2945-B999-20BC546494A8}"/>
+    <hyperlink ref="H1366" r:id="rId408" xr:uid="{27C98620-EFAB-1F4F-9503-6826A47807A0}"/>
+    <hyperlink ref="H1361" r:id="rId409" xr:uid="{10927082-D17D-B84B-9D18-F006C0EF47E7}"/>
+    <hyperlink ref="H1362" r:id="rId410" xr:uid="{3B397CEB-616F-5846-921A-551FDEB24164}"/>
+    <hyperlink ref="H1369" r:id="rId411" xr:uid="{BED91B06-E491-B14B-B135-328F9D71548C}"/>
+    <hyperlink ref="H1372" r:id="rId412" xr:uid="{FBC2EB98-E41E-9E41-A717-D8EB7C18C2DD}"/>
+    <hyperlink ref="H1373" r:id="rId413" xr:uid="{E32EA69E-3799-3945-9555-6F6FCE5B1FFF}"/>
+    <hyperlink ref="H1374" r:id="rId414" xr:uid="{75839044-8116-9043-B1F2-E0B397401EA5}"/>
+    <hyperlink ref="H1367" r:id="rId415" xr:uid="{56166624-9378-1146-A797-4C530CBBCB6C}"/>
+    <hyperlink ref="H1368" r:id="rId416" xr:uid="{2C787AD6-40A3-5D4F-A0E7-FA97ACCA3530}"/>
+    <hyperlink ref="H1382" r:id="rId417" xr:uid="{2EFE49C9-E7C8-174D-8234-B0CDBE73402C}"/>
+    <hyperlink ref="H1383" r:id="rId418" xr:uid="{89E01762-5B95-1046-BEA1-7207C656C57F}"/>
+    <hyperlink ref="H1384" r:id="rId419" xr:uid="{FA358546-27AC-EC41-B520-30BF55105054}"/>
+    <hyperlink ref="H1380" r:id="rId420" xr:uid="{02C6CC2B-2291-1548-A14B-491F25B308D5}"/>
+    <hyperlink ref="H1381" r:id="rId421" xr:uid="{22EE8ED4-3380-1749-896E-7BE54AE3777F}"/>
+    <hyperlink ref="H1377" r:id="rId422" xr:uid="{89FF5C0F-1FFB-1F43-B5F1-A41368814859}"/>
+    <hyperlink ref="H1378" r:id="rId423" xr:uid="{99567DD4-7F5C-4D45-B5F1-AB7406ABB022}"/>
+    <hyperlink ref="H1379" r:id="rId424" xr:uid="{D5384BF3-3497-9541-BD96-383A53D296FD}"/>
+    <hyperlink ref="H1375" r:id="rId425" xr:uid="{7D25DBAF-89DB-7A42-86F0-996AD3239335}"/>
+    <hyperlink ref="H1376" r:id="rId426" xr:uid="{BFA75EE1-A5F2-6E4C-8DB0-FEADFF8857DE}"/>
+    <hyperlink ref="H1390" r:id="rId427" xr:uid="{749CF3BC-4D34-364B-B2A8-9C0CE7E6426A}"/>
+    <hyperlink ref="H1391" r:id="rId428" xr:uid="{B992A77E-B153-884F-A9FC-8C3F9E09797D}"/>
+    <hyperlink ref="H1392" r:id="rId429" xr:uid="{7018C2D8-53FA-1147-9EA6-375902D20707}"/>
+    <hyperlink ref="H1388" r:id="rId430" xr:uid="{46A8E7F5-6306-834A-9E87-029B4F63B49B}"/>
+    <hyperlink ref="H1389" r:id="rId431" xr:uid="{653684CB-15B0-294C-A3D5-E976633C0D01}"/>
+    <hyperlink ref="H1359" r:id="rId432" xr:uid="{E6E245B0-94F2-674A-9E36-4F5A304D9D8B}"/>
+    <hyperlink ref="H1360" r:id="rId433" xr:uid="{474A4FA9-1541-9241-9496-A67C773D6E58}"/>
+    <hyperlink ref="H1358" r:id="rId434" xr:uid="{3D68B70A-24BA-324E-97A6-38775901ABBD}"/>
+    <hyperlink ref="H1386" r:id="rId435" xr:uid="{D828A74A-A80F-CE4A-9531-BAA460488487}"/>
+    <hyperlink ref="H1387" r:id="rId436" xr:uid="{F2E15E96-970E-124B-878B-16B96C286E72}"/>
+    <hyperlink ref="H1385" r:id="rId437" xr:uid="{CC20F719-ACE1-8E4F-8882-5CD8D8EA84B8}"/>
+    <hyperlink ref="H1370" r:id="rId438" xr:uid="{12D1A7BE-2581-0040-9C1E-AB8500309425}"/>
+    <hyperlink ref="H1371" r:id="rId439" xr:uid="{698C3618-3329-C444-9B94-E16F652E2499}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
Added o3-pro and updated gemini 2.5 pro
</commit_message>
<xml_diff>
--- a/data/benchmarks.xlsx
+++ b/data/benchmarks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sean/Coding/genai-explorer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8C9B8D-4724-A94D-BC0E-23D74713A0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DA2BFF-7F56-2E44-82FB-DBFE7EBCCA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="57600" windowHeight="32400" activeTab="2" xr2:uid="{683877ED-707A-FC42-8592-F58A6955B3A6}"/>
   </bookViews>
@@ -19,8 +19,8 @@
   </sheets>
   <definedNames>
     <definedName name="benchmark_id">'benchmark-meta'!$A$2:$A$998</definedName>
-    <definedName name="model_id">'model-meta'!$A$2:$A$1024</definedName>
-    <definedName name="ModelMeta">'model-meta'!$A$1024:$B$1024</definedName>
+    <definedName name="model_id">'model-meta'!$A$2:$A$1025</definedName>
+    <definedName name="ModelMeta">'model-meta'!$A$1025:$B$1025</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6878" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7120" uniqueCount="382">
   <si>
     <t>model_id</t>
   </si>
@@ -1175,6 +1175,21 @@
   <si>
     <t>May 28th update</t>
   </si>
+  <si>
+    <t>Gemini 2.5 Pro update</t>
+  </si>
+  <si>
+    <t>https://blog.google/products/gemini/gemini-2-5-pro-latest-preview/</t>
+  </si>
+  <si>
+    <t>o3-pro release notes</t>
+  </si>
+  <si>
+    <t>https://help.openai.com/en/articles/9624314-model-release-notes</t>
+  </si>
+  <si>
+    <t>o3-pro</t>
+  </si>
 </sst>
 </file>
 
@@ -1625,10 +1640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5579D913-ECD6-6A42-858D-C12502E32020}">
-  <dimension ref="A1:B78"/>
+  <dimension ref="A1:B79"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2127,7 +2142,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>34</v>
+        <v>381</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>6</v>
@@ -2135,7 +2150,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>6</v>
@@ -2143,15 +2158,15 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>352</v>
+        <v>39</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>116</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>112</v>
+        <v>352</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>116</v>
@@ -2159,7 +2174,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>145</v>
+        <v>112</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>116</v>
@@ -2167,7 +2182,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>105</v>
+        <v>145</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>116</v>
@@ -2175,7 +2190,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>116</v>
@@ -2183,23 +2198,23 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>302</v>
+        <v>131</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>337</v>
+        <v>302</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>324</v>
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>323</v>
+        <v>337</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>324</v>
@@ -2207,7 +2222,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>324</v>
@@ -2215,7 +2230,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>324</v>
@@ -2223,7 +2238,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>324</v>
@@ -2231,7 +2246,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>356</v>
+        <v>329</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>324</v>
@@ -2239,7 +2254,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>324</v>
@@ -2247,7 +2262,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>324</v>
@@ -2255,16 +2270,24 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>324</v>
       </c>
     </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>359</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B68">
-    <sortCondition ref="B2:B68"/>
-    <sortCondition ref="A2:A68"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B69">
+    <sortCondition ref="B2:B69"/>
+    <sortCondition ref="A2:A69"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
@@ -3199,11 +3222,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A72D42-DDBC-2B44-AB6C-55AD4AA1061B}">
-  <dimension ref="A1:H1729"/>
+  <dimension ref="A1:H1708"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1478" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1511" sqref="A1511"/>
+      <pane ySplit="1" topLeftCell="A1538" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1583" sqref="D1583"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -40980,438 +41003,1518 @@
       </c>
     </row>
     <row r="1528" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1528" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="B1528" s="1" t="str">
         <f>IF(A1528="", "", VLOOKUP(A1528, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1528" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1528" s="12">
+        <v>21.6</v>
+      </c>
+      <c r="E1528" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1528" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1528" s="13" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="1529" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1529" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1529" s="1" t="str">
         <f>IF(A1529="", "", VLOOKUP(A1529, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>openai</v>
+      </c>
+      <c r="C1529" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1529" s="12">
+        <v>20.3</v>
+      </c>
+      <c r="E1529" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1529" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1529" s="13" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="1530" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1530" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B1530" s="1" t="str">
         <f>IF(A1530="", "", VLOOKUP(A1530, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>openai</v>
+      </c>
+      <c r="C1530" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1530" s="12">
+        <v>14.3</v>
+      </c>
+      <c r="E1530" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1530" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1530" s="13" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="1531" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1531" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="B1531" s="1" t="str">
         <f>IF(A1531="", "", VLOOKUP(A1531, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>anthropic</v>
+      </c>
+      <c r="C1531" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1531" s="12">
+        <v>10.7</v>
+      </c>
+      <c r="E1531" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1531" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1531" s="13" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="1532" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1532" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="B1532" s="1" t="str">
         <f>IF(A1532="", "", VLOOKUP(A1532, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>deepseek</v>
+      </c>
+      <c r="C1532" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1532" s="12">
+        <v>14</v>
+      </c>
+      <c r="E1532" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1532" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1532" s="13" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="1533" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1533" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="B1533" s="1" t="str">
         <f>IF(A1533="", "", VLOOKUP(A1533, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1533" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1533" s="12">
+        <v>86.4</v>
+      </c>
+      <c r="E1533" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1533" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1533" s="13" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="1534" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1534" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1534" s="1" t="str">
         <f>IF(A1534="", "", VLOOKUP(A1534, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>openai</v>
+      </c>
+      <c r="C1534" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1534" s="12">
+        <v>83.3</v>
+      </c>
+      <c r="E1534" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1534" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1534" s="13" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="1535" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1535" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B1535" s="1" t="str">
         <f>IF(A1535="", "", VLOOKUP(A1535, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>openai</v>
+      </c>
+      <c r="C1535" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1535" s="12">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="E1535" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1535" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1535" s="13" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="1536" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1536" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="B1536" s="1" t="str">
         <f>IF(A1536="", "", VLOOKUP(A1536, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1537" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1536" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1536" s="12">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="E1536" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1536" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1536" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1537" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1537" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="B1537" s="1" t="str">
         <f>IF(A1537="", "", VLOOKUP(A1537, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1538" spans="2:2" x14ac:dyDescent="0.2">
+        <v>xai</v>
+      </c>
+      <c r="C1537" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1537" s="12">
+        <v>80.2</v>
+      </c>
+      <c r="E1537" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1537" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1537" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1538" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1538" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="B1538" s="1" t="str">
         <f>IF(A1538="", "", VLOOKUP(A1538, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1539" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1538" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1538" s="12">
+        <v>81</v>
+      </c>
+      <c r="E1538" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1538" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1538" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1539" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1539" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="B1539" s="1" t="str">
         <f>IF(A1539="", "", VLOOKUP(A1539, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1540" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1539" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1539" s="12">
+        <v>88</v>
+      </c>
+      <c r="E1539" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1539" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1539" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1540" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1540" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1540" s="1" t="str">
         <f>IF(A1540="", "", VLOOKUP(A1540, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1541" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1540" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1540" s="12">
+        <v>88.9</v>
+      </c>
+      <c r="E1540" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1540" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1540" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1541" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1541" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B1541" s="1" t="str">
         <f>IF(A1541="", "", VLOOKUP(A1541, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1542" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1541" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1541" s="12">
+        <v>92.7</v>
+      </c>
+      <c r="E1541" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1541" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1541" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1542" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1542" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="B1542" s="1" t="str">
         <f>IF(A1542="", "", VLOOKUP(A1542, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1543" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1542" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1542" s="12">
+        <v>75.5</v>
+      </c>
+      <c r="E1542" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1542" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1542" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1543" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1543" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="B1543" s="1" t="str">
         <f>IF(A1543="", "", VLOOKUP(A1543, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1544" spans="2:2" x14ac:dyDescent="0.2">
+        <v>xai</v>
+      </c>
+      <c r="C1543" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1543" s="12">
+        <v>77.3</v>
+      </c>
+      <c r="E1543" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1543" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1543" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1544" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1544" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="B1544" s="1" t="str">
         <f>IF(A1544="", "", VLOOKUP(A1544, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1545" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1544" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1544" s="12">
+        <v>87.5</v>
+      </c>
+      <c r="E1544" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1544" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1544" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1545" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1545" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="B1545" s="1" t="str">
         <f>IF(A1545="", "", VLOOKUP(A1545, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1546" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1545" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1545" s="12">
+        <v>69</v>
+      </c>
+      <c r="E1545" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1545" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1545" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1546" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1546" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1546" s="1" t="str">
         <f>IF(A1546="", "", VLOOKUP(A1546, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1547" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1546" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1546" s="12">
+        <v>72</v>
+      </c>
+      <c r="E1546" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1546" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1546" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1547" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1547" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B1547" s="1" t="str">
         <f>IF(A1547="", "", VLOOKUP(A1547, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1548" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1547" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1547" s="12">
+        <v>75.8</v>
+      </c>
+      <c r="E1547" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1547" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1547" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1548" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1548" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="B1548" s="1" t="str">
         <f>IF(A1548="", "", VLOOKUP(A1548, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1549" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1548" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1548" s="12">
+        <v>51.1</v>
+      </c>
+      <c r="E1548" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1548" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1548" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1549" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1549" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="B1549" s="1" t="str">
         <f>IF(A1549="", "", VLOOKUP(A1549, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1550" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1549" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1549" s="12">
+        <v>70.5</v>
+      </c>
+      <c r="E1549" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1549" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1549" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1550" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1550" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="B1550" s="1" t="str">
         <f>IF(A1550="", "", VLOOKUP(A1550, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1551" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1550" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D1550" s="12">
+        <v>82.2</v>
+      </c>
+      <c r="E1550" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1550" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1550" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1551" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1551" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1551" s="1" t="str">
         <f>IF(A1551="", "", VLOOKUP(A1551, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1552" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1551" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D1551" s="12">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="E1551" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1551" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1551" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1552" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1552" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B1552" s="1" t="str">
         <f>IF(A1552="", "", VLOOKUP(A1552, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1553" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1552" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D1552" s="12">
+        <v>72</v>
+      </c>
+      <c r="E1552" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1552" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1552" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1553" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1553" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="B1553" s="1" t="str">
         <f>IF(A1553="", "", VLOOKUP(A1553, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1554" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1553" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D1553" s="12">
+        <v>72</v>
+      </c>
+      <c r="E1553" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1553" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1553" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1554" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1554" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="B1554" s="1" t="str">
         <f>IF(A1554="", "", VLOOKUP(A1554, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1555" spans="2:2" x14ac:dyDescent="0.2">
+        <v>xai</v>
+      </c>
+      <c r="C1554" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D1554" s="12">
+        <v>53.3</v>
+      </c>
+      <c r="E1554" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1554" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1554" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1555" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1555" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="B1555" s="1" t="str">
         <f>IF(A1555="", "", VLOOKUP(A1555, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1556" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1555" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D1555" s="12">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="E1555" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1555" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1555" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1556" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1556" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="B1556" s="1" t="str">
         <f>IF(A1556="", "", VLOOKUP(A1556, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1557" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1556" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1556" s="12">
+        <v>59.6</v>
+      </c>
+      <c r="E1556" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1556" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1556" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1557" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1557" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1557" s="1" t="str">
         <f>IF(A1557="", "", VLOOKUP(A1557, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1558" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1557" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1557" s="12">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="E1557" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1557" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1557" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1558" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1558" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B1558" s="1" t="str">
         <f>IF(A1558="", "", VLOOKUP(A1558, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1559" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1558" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1558" s="12">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="E1558" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1558" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1558" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1559" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1559" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="B1559" s="1" t="str">
         <f>IF(A1559="", "", VLOOKUP(A1559, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1560" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1559" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1559" s="12">
+        <v>72.5</v>
+      </c>
+      <c r="E1559" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1559" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1559" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1560" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1560" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="B1560" s="1" t="str">
         <f>IF(A1560="", "", VLOOKUP(A1560, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1561" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1560" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1560" s="12">
+        <v>54</v>
+      </c>
+      <c r="E1560" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1560" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1560" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1561" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1561" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1561" s="1" t="str">
         <f>IF(A1561="", "", VLOOKUP(A1561, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1562" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1561" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1561" s="12">
+        <v>48.6</v>
+      </c>
+      <c r="E1561" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1561" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1561" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1562" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1562" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B1562" s="1" t="str">
         <f>IF(A1562="", "", VLOOKUP(A1562, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1563" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1562" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1562" s="12">
+        <v>19.3</v>
+      </c>
+      <c r="E1562" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1562" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1562" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1563" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1563" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="B1563" s="1" t="str">
         <f>IF(A1563="", "", VLOOKUP(A1563, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1564" spans="2:2" x14ac:dyDescent="0.2">
+        <v>xai</v>
+      </c>
+      <c r="C1563" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1563" s="12">
+        <v>43.6</v>
+      </c>
+      <c r="E1563" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1563" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1563" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1564" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1564" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="B1564" s="1" t="str">
         <f>IF(A1564="", "", VLOOKUP(A1564, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1565" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1564" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1564" s="12">
+        <v>27.8</v>
+      </c>
+      <c r="E1564" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1564" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1564" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1565" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1565" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="B1565" s="1" t="str">
         <f>IF(A1565="", "", VLOOKUP(A1565, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1566" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1565" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1565" s="12">
+        <v>87.8</v>
+      </c>
+      <c r="E1565" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1565" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1565" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1566" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1566" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1566" s="1" t="str">
         <f>IF(A1566="", "", VLOOKUP(A1566, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1567" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1566" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1566" s="12">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="E1566" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1566" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1566" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1567" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1567" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B1567" s="1" t="str">
         <f>IF(A1567="", "", VLOOKUP(A1567, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1568" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1567" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1567" s="12">
+        <v>62.1</v>
+      </c>
+      <c r="E1567" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1567" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1567" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1568" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1568" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="B1568" s="1" t="str">
         <f>IF(A1568="", "", VLOOKUP(A1568, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1569" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1568" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1568" s="12">
+        <v>77.7</v>
+      </c>
+      <c r="E1568" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1568" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1568" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1569" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1569" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="B1569" s="1" t="str">
         <f>IF(A1569="", "", VLOOKUP(A1569, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1570" spans="2:2" x14ac:dyDescent="0.2">
+        <v>xai</v>
+      </c>
+      <c r="C1569" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1569" s="12">
+        <v>74.8</v>
+      </c>
+      <c r="E1569" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1569" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1569" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1570" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1570" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="B1570" s="1" t="str">
         <f>IF(A1570="", "", VLOOKUP(A1570, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1571" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1570" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1570" s="12">
+        <v>82</v>
+      </c>
+      <c r="E1570" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1570" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1570" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1571" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1571" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1571" s="1" t="str">
         <f>IF(A1571="", "", VLOOKUP(A1571, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1572" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1571" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1571" s="12">
+        <v>82.9</v>
+      </c>
+      <c r="E1571" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1571" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1571" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1572" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1572" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B1572" s="1" t="str">
         <f>IF(A1572="", "", VLOOKUP(A1572, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1573" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1572" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1572" s="12">
+        <v>81.599999999999994</v>
+      </c>
+      <c r="E1572" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1572" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1572" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1573" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1573" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="B1573" s="1" t="str">
         <f>IF(A1573="", "", VLOOKUP(A1573, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1574" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1573" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1573" s="12">
+        <v>76.5</v>
+      </c>
+      <c r="E1573" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1573" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1573" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1574" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1574" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="B1574" s="1" t="str">
         <f>IF(A1574="", "", VLOOKUP(A1574, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1575" spans="2:2" x14ac:dyDescent="0.2">
+        <v>xai</v>
+      </c>
+      <c r="C1574" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1574" s="12">
+        <v>76</v>
+      </c>
+      <c r="E1574" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1574" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1574" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1575" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1575" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="B1575" s="1" t="str">
         <f>IF(A1575="", "", VLOOKUP(A1575, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1576" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1575" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1575" s="12">
+        <v>58</v>
+      </c>
+      <c r="E1575" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1575" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1575" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1576" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1576" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1576" s="1" t="str">
         <f>IF(A1576="", "", VLOOKUP(A1576, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1577" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1576" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1576" s="12">
+        <v>57.1</v>
+      </c>
+      <c r="E1576" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1576" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1576" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1577" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1577" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B1577" s="1" t="str">
         <f>IF(A1577="", "", VLOOKUP(A1577, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1578" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1577" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1577" s="12">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="E1577" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1577" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1577" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1578" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1578" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="B1578" s="1" t="str">
         <f>IF(A1578="", "", VLOOKUP(A1578, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1579" spans="2:2" x14ac:dyDescent="0.2">
+        <v>xai</v>
+      </c>
+      <c r="C1578" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1578" s="12">
+        <v>34</v>
+      </c>
+      <c r="E1578" s="4">
+        <v>45813</v>
+      </c>
+      <c r="G1578" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1578" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1579" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1579" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="B1579" s="1" t="str">
         <f>IF(A1579="", "", VLOOKUP(A1579, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1580" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1579" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1579" s="12">
+        <v>86</v>
+      </c>
+      <c r="E1579" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1579" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="H1579" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="1580" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1580" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1580" s="1" t="str">
         <f>IF(A1580="", "", VLOOKUP(A1580, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1581" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1580" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1580" s="12">
+        <v>90</v>
+      </c>
+      <c r="E1580" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1580" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="H1580" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="1581" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1581" s="2" t="s">
+        <v>381</v>
+      </c>
       <c r="B1581" s="1" t="str">
         <f>IF(A1581="", "", VLOOKUP(A1581, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1582" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1581" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1581" s="12">
+        <v>93</v>
+      </c>
+      <c r="E1581" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1581" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="H1581" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="1582" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1582" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="B1582" s="1" t="str">
         <f>IF(A1582="", "", VLOOKUP(A1582, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1583" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1582" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1582" s="12">
+        <v>79</v>
+      </c>
+      <c r="E1582" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1582" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="H1582" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="1583" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1583" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1583" s="1" t="str">
         <f>IF(A1583="", "", VLOOKUP(A1583, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1584" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1583" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1583" s="12">
+        <v>81</v>
+      </c>
+      <c r="E1583" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1583" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="H1583" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="1584" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1584" s="2" t="s">
+        <v>381</v>
+      </c>
       <c r="B1584" s="1" t="str">
         <f>IF(A1584="", "", VLOOKUP(A1584, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1585" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1584" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1584" s="12">
+        <v>84</v>
+      </c>
+      <c r="E1584" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1584" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="H1584" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="1585" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1585" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="B1585" s="1" t="str">
         <f>IF(A1585="", "", VLOOKUP(A1585, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1586" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1585" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1585" s="12">
+        <v>1707</v>
+      </c>
+      <c r="E1585" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1585" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="H1585" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="1586" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1586" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1586" s="1" t="str">
         <f>IF(A1586="", "", VLOOKUP(A1586, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1587" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1586" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1586" s="12">
+        <v>2517</v>
+      </c>
+      <c r="E1586" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1586" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="H1586" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="1587" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1587" s="2" t="s">
+        <v>381</v>
+      </c>
       <c r="B1587" s="1" t="str">
         <f>IF(A1587="", "", VLOOKUP(A1587, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1588" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1587" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1587" s="12">
+        <v>2748</v>
+      </c>
+      <c r="E1587" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1587" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="H1587" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="1588" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1588" s="1" t="str">
         <f>IF(A1588="", "", VLOOKUP(A1588, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1589" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1589" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1589" s="1" t="str">
         <f>IF(A1589="", "", VLOOKUP(A1589, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1590" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1590" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1590" s="1" t="str">
         <f>IF(A1590="", "", VLOOKUP(A1590, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1591" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1591" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1591" s="1" t="str">
         <f>IF(A1591="", "", VLOOKUP(A1591, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1592" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1592" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1592" s="1" t="str">
         <f>IF(A1592="", "", VLOOKUP(A1592, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1593" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1593" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1593" s="1" t="str">
         <f>IF(A1593="", "", VLOOKUP(A1593, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1594" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1594" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1594" s="1" t="str">
         <f>IF(A1594="", "", VLOOKUP(A1594, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1595" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1595" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1595" s="1" t="str">
         <f>IF(A1595="", "", VLOOKUP(A1595, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1596" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1596" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1596" s="1" t="str">
         <f>IF(A1596="", "", VLOOKUP(A1596, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1597" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1597" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1597" s="1" t="str">
         <f>IF(A1597="", "", VLOOKUP(A1597, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1598" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1598" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1598" s="1" t="str">
         <f>IF(A1598="", "", VLOOKUP(A1598, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1599" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1599" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1599" s="1" t="str">
         <f>IF(A1599="", "", VLOOKUP(A1599, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1600" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1600" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1600" s="1" t="str">
         <f>IF(A1600="", "", VLOOKUP(A1600, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
@@ -42062,132 +43165,6 @@
     <row r="1708" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1708" s="1" t="str">
         <f>IF(A1708="", "", VLOOKUP(A1708, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1709" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1709" s="1" t="str">
-        <f>IF(A1709="", "", VLOOKUP(A1709, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1710" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1710" s="1" t="str">
-        <f>IF(A1710="", "", VLOOKUP(A1710, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1711" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1711" s="1" t="str">
-        <f>IF(A1711="", "", VLOOKUP(A1711, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1712" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1712" s="1" t="str">
-        <f>IF(A1712="", "", VLOOKUP(A1712, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1713" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1713" s="1" t="str">
-        <f>IF(A1713="", "", VLOOKUP(A1713, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1714" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1714" s="1" t="str">
-        <f>IF(A1714="", "", VLOOKUP(A1714, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1715" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1715" s="1" t="str">
-        <f>IF(A1715="", "", VLOOKUP(A1715, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1716" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1716" s="1" t="str">
-        <f>IF(A1716="", "", VLOOKUP(A1716, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1717" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1717" s="1" t="str">
-        <f>IF(A1717="", "", VLOOKUP(A1717, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1718" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1718" s="1" t="str">
-        <f>IF(A1718="", "", VLOOKUP(A1718, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1719" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1719" s="1" t="str">
-        <f>IF(A1719="", "", VLOOKUP(A1719, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1720" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1720" s="1" t="str">
-        <f>IF(A1720="", "", VLOOKUP(A1720, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1721" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1721" s="1" t="str">
-        <f>IF(A1721="", "", VLOOKUP(A1721, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1722" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1722" s="1" t="str">
-        <f>IF(A1722="", "", VLOOKUP(A1722, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1723" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1723" s="1" t="str">
-        <f>IF(A1723="", "", VLOOKUP(A1723, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1724" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1724" s="1" t="str">
-        <f>IF(A1724="", "", VLOOKUP(A1724, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1725" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1725" s="1" t="str">
-        <f>IF(A1725="", "", VLOOKUP(A1725, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1726" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1726" s="1" t="str">
-        <f>IF(A1726="", "", VLOOKUP(A1726, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1727" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1727" s="1" t="str">
-        <f>IF(A1727="", "", VLOOKUP(A1727, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1728" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1728" s="1" t="str">
-        <f>IF(A1728="", "", VLOOKUP(A1728, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1729" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1729" s="1" t="str">
-        <f>IF(A1729="", "", VLOOKUP(A1729, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
@@ -42688,6 +43665,57 @@
     <hyperlink ref="H1445" r:id="rId479" xr:uid="{56737B87-AF2D-8B4E-9148-D1D7D97E9F0B}"/>
     <hyperlink ref="H1449" r:id="rId480" xr:uid="{546A0AF9-07AF-5442-A39A-57F1C87310AE}"/>
     <hyperlink ref="H1453" r:id="rId481" xr:uid="{DF3E3343-E58E-3847-BD1A-89A144D9593C}"/>
+    <hyperlink ref="H1528" r:id="rId482" xr:uid="{3CCBE6AF-6A22-D247-A7B4-8513D443324E}"/>
+    <hyperlink ref="H1529" r:id="rId483" xr:uid="{EFBAF6B4-123B-B945-915D-8A0EA0AA0BB8}"/>
+    <hyperlink ref="H1530" r:id="rId484" xr:uid="{E62776C2-B90F-144A-8E67-C601EA8E617D}"/>
+    <hyperlink ref="H1531" r:id="rId485" xr:uid="{0298E14C-35D8-4C42-994B-73FAB966E14F}"/>
+    <hyperlink ref="H1532" r:id="rId486" xr:uid="{6C285EE5-B61D-2B4E-9489-416FD19A80F0}"/>
+    <hyperlink ref="H1533" r:id="rId487" xr:uid="{64DC3CF5-F8F4-544A-8DED-9F8B997E1C28}"/>
+    <hyperlink ref="H1534" r:id="rId488" xr:uid="{21487612-9DDF-7843-8730-4902AF13225D}"/>
+    <hyperlink ref="H1535" r:id="rId489" xr:uid="{292853B5-861A-A945-B444-1B9FC7DB047F}"/>
+    <hyperlink ref="H1536" r:id="rId490" xr:uid="{AD0A611E-60C6-764D-B802-B070B096310F}"/>
+    <hyperlink ref="H1537" r:id="rId491" xr:uid="{02FCD203-F947-EB45-96F7-F3ED65B828DB}"/>
+    <hyperlink ref="H1538" r:id="rId492" xr:uid="{FC0DDA79-1713-2C47-A406-90569D28B3DC}"/>
+    <hyperlink ref="H1539" r:id="rId493" xr:uid="{6C784008-B6E5-D247-A600-64FAF7C3FDF2}"/>
+    <hyperlink ref="H1540" r:id="rId494" xr:uid="{74256B43-DC22-5341-A3F7-7BEBA7E07101}"/>
+    <hyperlink ref="H1541" r:id="rId495" xr:uid="{6BE43163-AF2A-764B-B4B1-46D92DE896E5}"/>
+    <hyperlink ref="H1542" r:id="rId496" xr:uid="{9FB74206-9B12-A34A-B47A-16503F6F1D40}"/>
+    <hyperlink ref="H1543" r:id="rId497" xr:uid="{B7FBEFFF-0807-094B-9375-6896129DC4F5}"/>
+    <hyperlink ref="H1544" r:id="rId498" xr:uid="{FF7A1C00-295B-014B-845C-DE7F9138B25E}"/>
+    <hyperlink ref="H1545" r:id="rId499" xr:uid="{4B8E2E8A-BF3C-3F4C-846D-E455CE70D5C5}"/>
+    <hyperlink ref="H1546" r:id="rId500" xr:uid="{F52F0EDF-23E2-F84B-BF4E-F55C68E41DFA}"/>
+    <hyperlink ref="H1547" r:id="rId501" xr:uid="{B3179432-A2C1-3C44-A301-5E94D501B227}"/>
+    <hyperlink ref="H1548" r:id="rId502" xr:uid="{927970E4-ACD9-B448-9F01-AE4761E14A14}"/>
+    <hyperlink ref="H1549" r:id="rId503" xr:uid="{C55A777C-E4E7-A04F-923F-B123A2610B35}"/>
+    <hyperlink ref="H1550" r:id="rId504" xr:uid="{BE652F69-277C-D449-8362-B51E3509466D}"/>
+    <hyperlink ref="H1551" r:id="rId505" xr:uid="{146E53E0-E8F9-1D48-9656-E8D77CA6B513}"/>
+    <hyperlink ref="H1552" r:id="rId506" xr:uid="{12E826FD-3D30-1E4C-B481-CA61A71E994D}"/>
+    <hyperlink ref="H1553" r:id="rId507" xr:uid="{3DA49D3F-0AE2-E24C-8CEF-3DD85911FA01}"/>
+    <hyperlink ref="H1554" r:id="rId508" xr:uid="{D6D407B4-A06E-544D-92BA-0DAEDC7B6861}"/>
+    <hyperlink ref="H1555" r:id="rId509" xr:uid="{B1834AB3-2B72-F448-A761-90BE21746ACA}"/>
+    <hyperlink ref="H1556" r:id="rId510" xr:uid="{46AAFC3D-2239-9D43-9EC3-79D9B24FFA4F}"/>
+    <hyperlink ref="H1557" r:id="rId511" xr:uid="{C99B6F03-3988-9F46-AB35-253C6736CE0C}"/>
+    <hyperlink ref="H1558" r:id="rId512" xr:uid="{8C91AF81-E31B-1942-BD1A-F897D9BB0367}"/>
+    <hyperlink ref="H1559" r:id="rId513" xr:uid="{4F33404E-A644-E34B-9BD9-A79A4C01CAD4}"/>
+    <hyperlink ref="H1560" r:id="rId514" xr:uid="{E056E711-2E33-5F43-9392-5078FDE5257D}"/>
+    <hyperlink ref="H1561" r:id="rId515" xr:uid="{4597AAF2-8B28-5E4A-A06B-DA0B5F4714CD}"/>
+    <hyperlink ref="H1562" r:id="rId516" xr:uid="{E364B847-A16F-1844-BEE8-72EA06405AF0}"/>
+    <hyperlink ref="H1563" r:id="rId517" xr:uid="{ED0AD5BC-B13E-3249-85CE-311162352918}"/>
+    <hyperlink ref="H1564" r:id="rId518" xr:uid="{E7746EDA-30A6-A145-9219-54313300A4BA}"/>
+    <hyperlink ref="H1565" r:id="rId519" xr:uid="{EDE57972-9124-844C-B6EC-62F096FC0E5C}"/>
+    <hyperlink ref="H1566" r:id="rId520" xr:uid="{0C26E4DF-DF38-A445-B8F8-1997B19CC644}"/>
+    <hyperlink ref="H1567" r:id="rId521" xr:uid="{0810C50E-7B9F-124D-B9AC-D133E555A7BD}"/>
+    <hyperlink ref="H1568" r:id="rId522" xr:uid="{D94624C8-8BC6-024B-94FA-189937FF2DE2}"/>
+    <hyperlink ref="H1569" r:id="rId523" xr:uid="{FAFA1C01-00F3-3741-892B-A19E397C63F2}"/>
+    <hyperlink ref="H1570" r:id="rId524" xr:uid="{734CFD48-CB19-1246-9F19-DDF8C86ED1BF}"/>
+    <hyperlink ref="H1571" r:id="rId525" xr:uid="{812A09D1-8A88-9842-ACD6-79F756C45D22}"/>
+    <hyperlink ref="H1572" r:id="rId526" xr:uid="{0AA42575-E8F8-834A-87C6-70F0ABFCA012}"/>
+    <hyperlink ref="H1573" r:id="rId527" xr:uid="{2C2FADE5-FCAA-804E-876A-37F42CE15043}"/>
+    <hyperlink ref="H1574" r:id="rId528" xr:uid="{8746DD08-FFAE-FC4E-8889-F9651EED5DBE}"/>
+    <hyperlink ref="H1575" r:id="rId529" xr:uid="{31DD0407-1EEF-DD46-A281-1AAE4263C6CB}"/>
+    <hyperlink ref="H1576" r:id="rId530" xr:uid="{7437D822-26C2-0E46-BF34-CA9B6AB65521}"/>
+    <hyperlink ref="H1577" r:id="rId531" xr:uid="{F4673F55-9929-D54B-AC2D-38EBAA2D1B94}"/>
+    <hyperlink ref="H1578" r:id="rId532" xr:uid="{EF4857F4-1B65-7D43-A4B5-DA3B243B6201}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
Added Magistral and Midjourney Video v1
</commit_message>
<xml_diff>
--- a/data/benchmarks.xlsx
+++ b/data/benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sean/Coding/genai-explorer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DA2BFF-7F56-2E44-82FB-DBFE7EBCCA2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAD7722-EF21-6B40-9B3A-86D0DB10FFAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="57600" windowHeight="32400" activeTab="2" xr2:uid="{683877ED-707A-FC42-8592-F58A6955B3A6}"/>
   </bookViews>
@@ -19,8 +19,8 @@
   </sheets>
   <definedNames>
     <definedName name="benchmark_id">'benchmark-meta'!$A$2:$A$998</definedName>
-    <definedName name="model_id">'model-meta'!$A$2:$A$1025</definedName>
-    <definedName name="ModelMeta">'model-meta'!$A$1025:$B$1025</definedName>
+    <definedName name="model_id">'model-meta'!$A$2:$A$1026</definedName>
+    <definedName name="ModelMeta">'model-meta'!$A$1026:$B$1026</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7120" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7202" uniqueCount="385">
   <si>
     <t>model_id</t>
   </si>
@@ -1190,6 +1190,15 @@
   <si>
     <t>o3-pro</t>
   </si>
+  <si>
+    <t>magistral-medium</t>
+  </si>
+  <si>
+    <t>Magistral announcement</t>
+  </si>
+  <si>
+    <t>https://mistral.ai/news/magistral</t>
+  </si>
 </sst>
 </file>
 
@@ -1255,7 +1264,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1304,6 +1313,9 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1640,10 +1652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5579D913-ECD6-6A42-858D-C12502E32020}">
-  <dimension ref="A1:B79"/>
+  <dimension ref="A1:B80"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2054,15 +2066,15 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>56</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>6</v>
+        <v>382</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>6</v>
@@ -2070,7 +2082,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>6</v>
@@ -2078,7 +2090,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>6</v>
@@ -2086,7 +2098,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>122</v>
+        <v>60</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>6</v>
@@ -2094,7 +2106,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>49</v>
+        <v>122</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>6</v>
@@ -2102,7 +2114,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>6</v>
@@ -2110,7 +2122,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>6</v>
@@ -2118,7 +2130,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>123</v>
+        <v>38</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>6</v>
@@ -2126,7 +2138,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>41</v>
+        <v>123</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>6</v>
@@ -2134,7 +2146,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>6</v>
@@ -2142,7 +2154,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>381</v>
+        <v>7</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>6</v>
@@ -2150,7 +2162,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>34</v>
+        <v>381</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>6</v>
@@ -2158,7 +2170,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>6</v>
@@ -2166,15 +2178,15 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>352</v>
+        <v>39</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>116</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>112</v>
+        <v>352</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>116</v>
@@ -2182,7 +2194,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>145</v>
+        <v>112</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>116</v>
@@ -2190,7 +2202,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>105</v>
+        <v>145</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>116</v>
@@ -2198,7 +2210,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>116</v>
@@ -2206,23 +2218,23 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>302</v>
+        <v>131</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>337</v>
+        <v>302</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>324</v>
+        <v>118</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>323</v>
+        <v>337</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>324</v>
@@ -2230,7 +2242,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>324</v>
@@ -2238,7 +2250,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>324</v>
@@ -2246,7 +2258,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>324</v>
@@ -2254,7 +2266,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>356</v>
+        <v>329</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>324</v>
@@ -2262,7 +2274,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>324</v>
@@ -2270,7 +2282,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>324</v>
@@ -2278,16 +2290,24 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>324</v>
       </c>
     </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>359</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B69">
-    <sortCondition ref="B2:B69"/>
-    <sortCondition ref="A2:A69"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B70">
+    <sortCondition ref="B2:B70"/>
+    <sortCondition ref="A2:A70"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
@@ -3225,8 +3245,8 @@
   <dimension ref="A1:H1708"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1538" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1583" sqref="D1583"/>
+      <pane ySplit="1" topLeftCell="A1557" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1607" sqref="D1607"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -42443,174 +42463,534 @@
       </c>
     </row>
     <row r="1588" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1588" s="2" t="s">
+        <v>364</v>
+      </c>
       <c r="B1588" s="1" t="str">
         <f>IF(A1588="", "", VLOOKUP(A1588, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>mistral</v>
+      </c>
+      <c r="C1588" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1588" s="12">
+        <v>26.8</v>
+      </c>
+      <c r="E1588" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1588" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="H1588" s="13" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="1589" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1589" s="2" t="s">
+        <v>382</v>
+      </c>
       <c r="B1589" s="1" t="str">
         <f>IF(A1589="", "", VLOOKUP(A1589, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>mistral</v>
+      </c>
+      <c r="C1589" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1589" s="12">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="E1589" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1589" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="H1589" s="13" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="1590" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1590" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="B1590" s="1" t="str">
         <f>IF(A1590="", "", VLOOKUP(A1590, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>deepseek</v>
+      </c>
+      <c r="C1590" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1590" s="12">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="E1590" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1590" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="H1590" s="13" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="1591" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1591" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="B1591" s="1" t="str">
         <f>IF(A1591="", "", VLOOKUP(A1591, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>deepseek</v>
+      </c>
+      <c r="C1591" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1591" s="12">
+        <v>79.8</v>
+      </c>
+      <c r="E1591" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1591" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="H1591" s="13" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="1592" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1592" s="2" t="s">
+        <v>364</v>
+      </c>
       <c r="B1592" s="1" t="str">
         <f>IF(A1592="", "", VLOOKUP(A1592, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>mistral</v>
+      </c>
+      <c r="C1592" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1592" s="12">
+        <v>21.2</v>
+      </c>
+      <c r="E1592" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1592" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="H1592" s="13" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="1593" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1593" s="2" t="s">
+        <v>382</v>
+      </c>
       <c r="B1593" s="1" t="str">
         <f>IF(A1593="", "", VLOOKUP(A1593, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>mistral</v>
+      </c>
+      <c r="C1593" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1593" s="12">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="E1593" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1593" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="H1593" s="13" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="1594" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1594" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="B1594" s="1" t="str">
         <f>IF(A1594="", "", VLOOKUP(A1594, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>deepseek</v>
+      </c>
+      <c r="C1594" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1594" s="12">
+        <v>28.8</v>
+      </c>
+      <c r="E1594" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1594" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="H1594" s="13" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="1595" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1595" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="B1595" s="1" t="str">
         <f>IF(A1595="", "", VLOOKUP(A1595, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>deepseek</v>
+      </c>
+      <c r="C1595" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1595" s="12">
+        <v>70</v>
+      </c>
+      <c r="E1595" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1595" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="H1595" s="13" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="1596" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1596" s="2" t="s">
+        <v>364</v>
+      </c>
       <c r="B1596" s="1" t="str">
         <f>IF(A1596="", "", VLOOKUP(A1596, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>mistral</v>
+      </c>
+      <c r="C1596" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1596" s="12">
+        <v>59.6</v>
+      </c>
+      <c r="E1596" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1596" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="H1596" s="13" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="1597" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1597" s="2" t="s">
+        <v>382</v>
+      </c>
       <c r="B1597" s="1" t="str">
         <f>IF(A1597="", "", VLOOKUP(A1597, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>mistral</v>
+      </c>
+      <c r="C1597" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1597" s="12">
+        <v>70.8</v>
+      </c>
+      <c r="E1597" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1597" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="H1597" s="13" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="1598" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1598" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="B1598" s="1" t="str">
         <f>IF(A1598="", "", VLOOKUP(A1598, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>deepseek</v>
+      </c>
+      <c r="C1598" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1598" s="12">
+        <v>59.1</v>
+      </c>
+      <c r="E1598" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1598" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="H1598" s="13" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="1599" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1599" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="B1599" s="1" t="str">
         <f>IF(A1599="", "", VLOOKUP(A1599, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>deepseek</v>
+      </c>
+      <c r="C1599" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1599" s="12">
+        <v>71.5</v>
+      </c>
+      <c r="E1599" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1599" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="H1599" s="13" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="1600" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1600" s="2" t="s">
+        <v>364</v>
+      </c>
       <c r="B1600" s="1" t="str">
         <f>IF(A1600="", "", VLOOKUP(A1600, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1601" spans="2:2" x14ac:dyDescent="0.2">
+        <v>mistral</v>
+      </c>
+      <c r="C1600" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1600" s="12">
+        <v>29.1</v>
+      </c>
+      <c r="E1600" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1600" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="H1600" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1601" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1601" s="2" t="s">
+        <v>382</v>
+      </c>
       <c r="B1601" s="1" t="str">
         <f>IF(A1601="", "", VLOOKUP(A1601, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1602" spans="2:2" x14ac:dyDescent="0.2">
+        <v>mistral</v>
+      </c>
+      <c r="C1601" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1601" s="12">
+        <v>59.4</v>
+      </c>
+      <c r="E1601" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1601" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="H1601" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1602" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1602" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="B1602" s="1" t="str">
         <f>IF(A1602="", "", VLOOKUP(A1602, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1603" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1602" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1602" s="12">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="E1602" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1602" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="H1602" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1603" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1603" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="B1603" s="1" t="str">
         <f>IF(A1603="", "", VLOOKUP(A1603, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1604" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1603" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1603" s="12">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="E1603" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1603" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="H1603" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1604" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1604" s="2" t="s">
+        <v>364</v>
+      </c>
       <c r="B1604" s="1" t="str">
         <f>IF(A1604="", "", VLOOKUP(A1604, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1605" spans="2:2" x14ac:dyDescent="0.2">
+        <v>mistral</v>
+      </c>
+      <c r="C1604" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D1604" s="12">
+        <v>28.9</v>
+      </c>
+      <c r="E1604" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1604" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="H1604" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1605" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1605" s="2" t="s">
+        <v>382</v>
+      </c>
       <c r="B1605" s="1" t="str">
         <f>IF(A1605="", "", VLOOKUP(A1605, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1606" spans="2:2" x14ac:dyDescent="0.2">
+        <v>mistral</v>
+      </c>
+      <c r="C1605" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D1605" s="12">
+        <v>47.1</v>
+      </c>
+      <c r="E1605" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1605" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="H1605" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1606" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1606" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="B1606" s="1" t="str">
         <f>IF(A1606="", "", VLOOKUP(A1606, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1607" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1606" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D1606" s="12">
+        <v>49.6</v>
+      </c>
+      <c r="E1606" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1606" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="H1606" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1607" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1607" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="B1607" s="1" t="str">
         <f>IF(A1607="", "", VLOOKUP(A1607, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1608" spans="2:2" x14ac:dyDescent="0.2">
+        <v>deepseek</v>
+      </c>
+      <c r="C1607" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D1607" s="12">
+        <v>53.3</v>
+      </c>
+      <c r="E1607" s="4">
+        <v>45818</v>
+      </c>
+      <c r="G1607" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="H1607" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1608" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1608" s="1" t="str">
         <f>IF(A1608="", "", VLOOKUP(A1608, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1609" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1609" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1609" s="1" t="str">
         <f>IF(A1609="", "", VLOOKUP(A1609, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1610" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1610" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1610" s="1" t="str">
         <f>IF(A1610="", "", VLOOKUP(A1610, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1611" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1611" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1611" s="1" t="str">
         <f>IF(A1611="", "", VLOOKUP(A1611, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1612" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1612" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1612" s="1" t="str">
         <f>IF(A1612="", "", VLOOKUP(A1612, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1613" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1613" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1613" s="1" t="str">
         <f>IF(A1613="", "", VLOOKUP(A1613, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1614" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1614" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1614" s="1" t="str">
         <f>IF(A1614="", "", VLOOKUP(A1614, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1615" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1615" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1615" s="1" t="str">
         <f>IF(A1615="", "", VLOOKUP(A1615, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
       </c>
     </row>
-    <row r="1616" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1616" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1616" s="1" t="str">
         <f>IF(A1616="", "", VLOOKUP(A1616, 'model-meta'!A:B, 2, FALSE))</f>
         <v/>
@@ -43716,6 +44096,26 @@
     <hyperlink ref="H1576" r:id="rId530" xr:uid="{7437D822-26C2-0E46-BF34-CA9B6AB65521}"/>
     <hyperlink ref="H1577" r:id="rId531" xr:uid="{F4673F55-9929-D54B-AC2D-38EBAA2D1B94}"/>
     <hyperlink ref="H1578" r:id="rId532" xr:uid="{EF4857F4-1B65-7D43-A4B5-DA3B243B6201}"/>
+    <hyperlink ref="H1588" r:id="rId533" xr:uid="{5B66ABB7-B413-164E-B087-500840D55D93}"/>
+    <hyperlink ref="H1589" r:id="rId534" xr:uid="{3A2B39A6-174D-7F4C-AF30-6F0EF161D91D}"/>
+    <hyperlink ref="H1590" r:id="rId535" xr:uid="{81C931B7-73CF-9642-9EC5-DD2D4E422BC0}"/>
+    <hyperlink ref="H1591" r:id="rId536" xr:uid="{67465676-05F0-2B49-B431-C8963328C9D8}"/>
+    <hyperlink ref="H1592" r:id="rId537" xr:uid="{FA653625-5490-074D-A5F8-74C6BC8AE498}"/>
+    <hyperlink ref="H1593" r:id="rId538" xr:uid="{9DB5D651-DBEC-5C43-8DC0-44727EDBFB8B}"/>
+    <hyperlink ref="H1594" r:id="rId539" xr:uid="{528C837D-4809-4C42-AEDD-4A995E0DB5CD}"/>
+    <hyperlink ref="H1595" r:id="rId540" xr:uid="{382B6BD9-BFF0-7D41-AE07-E21B6C5283AD}"/>
+    <hyperlink ref="H1596" r:id="rId541" xr:uid="{87272CD3-0CDF-544F-9AC0-6D78925CEBE2}"/>
+    <hyperlink ref="H1597" r:id="rId542" xr:uid="{01D447C7-9994-1149-9DB3-9E7351C9C1BC}"/>
+    <hyperlink ref="H1598" r:id="rId543" xr:uid="{45419095-F309-8545-BC29-C8F33EAB50AD}"/>
+    <hyperlink ref="H1599" r:id="rId544" xr:uid="{4ADF440D-39E9-4B4B-91A7-D6E5C2D686F6}"/>
+    <hyperlink ref="H1600" r:id="rId545" xr:uid="{BD73899A-3B3C-9F41-9C08-0201A52F8448}"/>
+    <hyperlink ref="H1601" r:id="rId546" xr:uid="{A99C06BA-3831-6D44-ACA1-33905CDFA79D}"/>
+    <hyperlink ref="H1602" r:id="rId547" xr:uid="{9EF63C92-4CE0-5344-B03B-303648DA8DFC}"/>
+    <hyperlink ref="H1603" r:id="rId548" xr:uid="{49EBD42C-76EA-4E4F-87BA-371E59E68903}"/>
+    <hyperlink ref="H1604" r:id="rId549" xr:uid="{3491B5BC-5C65-414A-A704-630360B92E41}"/>
+    <hyperlink ref="H1605" r:id="rId550" xr:uid="{24E55C23-44D0-CD46-AC38-ED9C72B6CF9A}"/>
+    <hyperlink ref="H1606" r:id="rId551" xr:uid="{59FAB9EA-2B6B-0A44-9816-A3A39917728E}"/>
+    <hyperlink ref="H1607" r:id="rId552" xr:uid="{D23EBE6A-F307-EE4D-B0B7-A7CA4F5783C4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
Added GPT-5, GPT-OSS, Claude Opus 4.1, and Mistral Deep Research
</commit_message>
<xml_diff>
--- a/data/benchmarks.xlsx
+++ b/data/benchmarks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sean/Coding/genai-explorer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAD7722-EF21-6B40-9B3A-86D0DB10FFAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EBE7F2-6D65-FD4A-97FD-BBCBBA685C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="57600" windowHeight="32400" activeTab="2" xr2:uid="{683877ED-707A-FC42-8592-F58A6955B3A6}"/>
+    <workbookView xWindow="-67200" yWindow="0" windowWidth="67200" windowHeight="37800" activeTab="2" xr2:uid="{683877ED-707A-FC42-8592-F58A6955B3A6}"/>
   </bookViews>
   <sheets>
     <sheet name="model-meta" sheetId="3" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="benchmarks" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="benchmark_id">'benchmark-meta'!$A$2:$A$998</definedName>
-    <definedName name="model_id">'model-meta'!$A$2:$A$1026</definedName>
-    <definedName name="ModelMeta">'model-meta'!$A$1026:$B$1026</definedName>
+    <definedName name="benchmark_id">'benchmark-meta'!$A$2:$A$999</definedName>
+    <definedName name="model_id">'model-meta'!$A$2:$A$1033</definedName>
+    <definedName name="ModelMeta">'model-meta'!$A$1033:$B$1033</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7202" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7761" uniqueCount="409">
   <si>
     <t>model_id</t>
   </si>
@@ -1199,6 +1199,78 @@
   <si>
     <t>https://mistral.ai/news/magistral</t>
   </si>
+  <si>
+    <t>grok-4</t>
+  </si>
+  <si>
+    <t>https://x.ai/news/grok-4</t>
+  </si>
+  <si>
+    <t>Grok 4 announcement</t>
+  </si>
+  <si>
+    <t>human</t>
+  </si>
+  <si>
+    <t>humanity</t>
+  </si>
+  <si>
+    <t>arc-2</t>
+  </si>
+  <si>
+    <t>ARC v2</t>
+  </si>
+  <si>
+    <t>August 9th update</t>
+  </si>
+  <si>
+    <t>https://arcprize.org/leaderboard</t>
+  </si>
+  <si>
+    <t>gpt-5</t>
+  </si>
+  <si>
+    <t>Thinking 18K</t>
+  </si>
+  <si>
+    <t>Thinking 32K</t>
+  </si>
+  <si>
+    <t>Thinking 24K</t>
+  </si>
+  <si>
+    <t>claude-4-1-opus</t>
+  </si>
+  <si>
+    <t>https://www.anthropic.com/news/claude-opus-4-1</t>
+  </si>
+  <si>
+    <t>Claude Opus 4.1 announcement</t>
+  </si>
+  <si>
+    <t>gpt-oss-120b</t>
+  </si>
+  <si>
+    <t>gpt-oss-20b</t>
+  </si>
+  <si>
+    <t>GPT-OSS announcement</t>
+  </si>
+  <si>
+    <t>https://openai.com/index/introducing-gpt-oss/</t>
+  </si>
+  <si>
+    <t>gpt-5-mini</t>
+  </si>
+  <si>
+    <t>gpt-5-nano</t>
+  </si>
+  <si>
+    <t>GPT-5 announcement</t>
+  </si>
+  <si>
+    <t>https://openai.com/index/introducing-gpt-5/</t>
+  </si>
 </sst>
 </file>
 
@@ -1652,10 +1724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5579D913-ECD6-6A42-858D-C12502E32020}">
-  <dimension ref="A1:B80"/>
+  <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView topLeftCell="A22" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1818,15 +1890,15 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>208</v>
+        <v>398</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>120</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>115</v>
+        <v>208</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>120</v>
@@ -1834,7 +1906,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>330</v>
+        <v>115</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>120</v>
@@ -1842,7 +1914,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>120</v>
@@ -1850,15 +1922,15 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>106</v>
+        <v>331</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>117</v>
@@ -1866,15 +1938,15 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>153</v>
+        <v>108</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>353</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>109</v>
+        <v>153</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>353</v>
@@ -1882,7 +1954,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>353</v>
@@ -1890,7 +1962,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>171</v>
+        <v>134</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>353</v>
@@ -1898,7 +1970,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>353</v>
@@ -1906,7 +1978,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>353</v>
@@ -1914,7 +1986,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>353</v>
@@ -1922,7 +1994,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>353</v>
@@ -1930,7 +2002,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>103</v>
+        <v>206</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>353</v>
@@ -1938,7 +2010,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>207</v>
+        <v>103</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>353</v>
@@ -1946,7 +2018,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>281</v>
+        <v>207</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>353</v>
@@ -1954,7 +2026,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>353</v>
@@ -1962,7 +2034,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>353</v>
@@ -1970,15 +2042,15 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>111</v>
+        <v>283</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>118</v>
+        <v>353</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>201</v>
+        <v>111</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>118</v>
@@ -1986,7 +2058,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>118</v>
@@ -1994,7 +2066,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>118</v>
@@ -2002,7 +2074,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>114</v>
+        <v>197</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>118</v>
@@ -2010,7 +2082,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>118</v>
@@ -2018,7 +2090,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>310</v>
+        <v>107</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>118</v>
@@ -2026,15 +2098,15 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>113</v>
+        <v>310</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>364</v>
+        <v>113</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>119</v>
@@ -2042,7 +2114,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>311</v>
+        <v>364</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>119</v>
@@ -2050,7 +2122,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>119</v>
@@ -2058,7 +2130,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>367</v>
+        <v>316</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>119</v>
@@ -2066,23 +2138,23 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>382</v>
-      </c>
-      <c r="B51" s="17" t="s">
+        <v>367</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>6</v>
+        <v>382</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>6</v>
@@ -2090,7 +2162,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>6</v>
@@ -2098,7 +2170,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>6</v>
@@ -2106,7 +2178,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>122</v>
+        <v>60</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>6</v>
@@ -2114,7 +2186,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>49</v>
+        <v>122</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>6</v>
@@ -2122,7 +2194,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>6</v>
@@ -2130,7 +2202,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>6</v>
@@ -2138,7 +2210,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>123</v>
+        <v>38</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>6</v>
@@ -2146,7 +2218,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>41</v>
+        <v>123</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>6</v>
@@ -2154,7 +2226,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>6</v>
@@ -2162,7 +2234,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>381</v>
+        <v>7</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>6</v>
@@ -2170,7 +2242,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>34</v>
+        <v>381</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>6</v>
@@ -2178,7 +2250,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>6</v>
@@ -2186,111 +2258,111 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>352</v>
+        <v>39</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>116</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>112</v>
+        <v>401</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>116</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>145</v>
+        <v>402</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>116</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>105</v>
+        <v>394</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>116</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>131</v>
+        <v>405</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>116</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>302</v>
+        <v>406</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>118</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>337</v>
+        <v>352</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>324</v>
+        <v>116</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>323</v>
+        <v>112</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>324</v>
+        <v>116</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>327</v>
+        <v>145</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>324</v>
+        <v>116</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>328</v>
+        <v>105</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>324</v>
+        <v>116</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>329</v>
+        <v>131</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>324</v>
+        <v>116</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>356</v>
+        <v>385</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>324</v>
+        <v>116</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>357</v>
+        <v>302</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>324</v>
+        <v>118</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>358</v>
+        <v>337</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>324</v>
@@ -2298,16 +2370,80 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>359</v>
+        <v>323</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>324</v>
       </c>
     </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>327</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>328</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>329</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>356</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>357</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>358</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>359</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>388</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B70">
-    <sortCondition ref="B2:B70"/>
-    <sortCondition ref="A2:A70"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B76">
+    <sortCondition ref="B2:B76"/>
+    <sortCondition ref="A2:A76"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
@@ -2318,10 +2454,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59AE2281-1D1A-A84A-BB56-21F84F3D4C74}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3045,155 +3181,172 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B42" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="14" t="s">
+      <c r="C42" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D41" s="14"/>
-      <c r="E41" s="6" t="s">
+      <c r="D42" s="14"/>
+      <c r="E42" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="F41" s="13" t="s">
+      <c r="F42" s="13" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="F42" s="13" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>71</v>
+        <v>158</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>72</v>
+        <v>159</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>271</v>
+        <v>246</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>73</v>
+        <v>290</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>185</v>
+        <v>71</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>186</v>
+        <v>72</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E44" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="F44" s="13" t="s">
+      <c r="F45" s="13" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="6" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B46" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C46" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="E46" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="F45" s="13" t="s">
+      <c r="F46" s="13" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D46" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="F46" s="13" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="F47" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>374</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="F47" s="13" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>374</v>
       </c>
-      <c r="D48" s="3" t="b">
+      <c r="E48" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="D49" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="E48" s="6" t="s">
+      <c r="E49" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="F48" s="13" t="s">
+      <c r="F49" s="13" t="s">
         <v>285</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F48">
-    <sortCondition ref="C2:C48"/>
-    <sortCondition ref="B2:B48"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F49">
+    <sortCondition ref="C2:C49"/>
+    <sortCondition ref="B2:B49"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="F43" r:id="rId1" xr:uid="{C428F855-A740-2146-892A-AE962A8B2426}"/>
+    <hyperlink ref="F44" r:id="rId1" xr:uid="{C428F855-A740-2146-892A-AE962A8B2426}"/>
     <hyperlink ref="F39" r:id="rId2" xr:uid="{BE3015A8-0281-4F4C-9FFA-721D5996A168}"/>
     <hyperlink ref="F33" r:id="rId3" xr:uid="{85A7CD31-5345-DB49-824E-41B8190FF3B9}"/>
     <hyperlink ref="F38" r:id="rId4" xr:uid="{498C1F45-C7D5-CA42-9340-DAE23057D52F}"/>
@@ -3204,13 +3357,13 @@
     <hyperlink ref="F28" r:id="rId9" xr:uid="{C3518D16-5842-7D43-B90D-860BCE04532D}"/>
     <hyperlink ref="F2" r:id="rId10" xr:uid="{5D6BBAB9-6037-6440-8578-F21366566C18}"/>
     <hyperlink ref="F12" r:id="rId11" xr:uid="{CA19CF50-5BE5-D149-98B4-0B04D1EA57A6}"/>
-    <hyperlink ref="F45" r:id="rId12" xr:uid="{006F90FD-9C8A-DF44-BDB9-5B6799EEC795}"/>
+    <hyperlink ref="F46" r:id="rId12" xr:uid="{006F90FD-9C8A-DF44-BDB9-5B6799EEC795}"/>
     <hyperlink ref="F17" r:id="rId13" xr:uid="{815A6906-20F9-B641-BFF3-29E25824ABAE}"/>
     <hyperlink ref="F8" r:id="rId14" xr:uid="{070682E4-D777-B146-BC96-531161B5C73E}"/>
     <hyperlink ref="F9" r:id="rId15" xr:uid="{39A79189-9118-D94A-8A56-B28A49FA1F12}"/>
-    <hyperlink ref="F41" r:id="rId16" xr:uid="{49942D9D-D639-0A41-BA23-0E00678ED250}"/>
+    <hyperlink ref="F42" r:id="rId16" xr:uid="{49942D9D-D639-0A41-BA23-0E00678ED250}"/>
     <hyperlink ref="F16" r:id="rId17" xr:uid="{10D693AD-355E-9340-BB06-EA81D6A4C44C}"/>
-    <hyperlink ref="F46" r:id="rId18" xr:uid="{9129B512-49CB-1F4D-BE88-1B65416DA281}"/>
+    <hyperlink ref="F47" r:id="rId18" xr:uid="{9129B512-49CB-1F4D-BE88-1B65416DA281}"/>
     <hyperlink ref="F24" r:id="rId19" xr:uid="{526601CB-FBE3-0944-B10E-44D916F2B924}"/>
     <hyperlink ref="F40" r:id="rId20" xr:uid="{3C81540A-D7B0-E94B-BC36-338D3782F549}"/>
     <hyperlink ref="F19" r:id="rId21" xr:uid="{5E4DC5B0-C585-0D40-825C-A3323D39D779}"/>
@@ -3231,7 +3384,8 @@
     <hyperlink ref="F34" r:id="rId36" xr:uid="{487980E2-8CA2-6941-A610-A06B767DF071}"/>
     <hyperlink ref="F35" r:id="rId37" xr:uid="{598BD020-41C8-3142-B2F5-4A14A4D4CF25}"/>
     <hyperlink ref="F37" r:id="rId38" xr:uid="{56B274E2-A1EF-1047-85A2-47D5F4CD9978}"/>
-    <hyperlink ref="F47" r:id="rId39" xr:uid="{8E393312-6C83-A643-A78E-3AF75863B793}"/>
+    <hyperlink ref="F48" r:id="rId39" xr:uid="{8E393312-6C83-A643-A78E-3AF75863B793}"/>
+    <hyperlink ref="F41" r:id="rId40" xr:uid="{46EB542E-0B53-F842-A338-3C07834A272B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
@@ -3242,11 +3396,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A72D42-DDBC-2B44-AB6C-55AD4AA1061B}">
-  <dimension ref="A1:H1708"/>
+  <dimension ref="A1:H1735"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1557" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1607" sqref="D1607"/>
+      <pane ySplit="1" topLeftCell="A1686" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1735" sqref="D1735"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -42943,609 +43097,3153 @@
       </c>
     </row>
     <row r="1608" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1608" s="2" t="s">
+        <v>385</v>
+      </c>
       <c r="B1608" s="1" t="str">
         <f>IF(A1608="", "", VLOOKUP(A1608, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>xai</v>
+      </c>
+      <c r="C1608" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1608" s="12">
+        <v>25.4</v>
+      </c>
+      <c r="E1608" s="4">
+        <v>45847</v>
+      </c>
+      <c r="G1608" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1608" s="13" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="1609" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1609" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1609" s="1" t="str">
         <f>IF(A1609="", "", VLOOKUP(A1609, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>openai</v>
+      </c>
+      <c r="C1609" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1609" s="12">
+        <v>21</v>
+      </c>
+      <c r="E1609" s="4">
+        <v>45847</v>
+      </c>
+      <c r="G1609" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1609" s="13" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="1610" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1610" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="B1610" s="1" t="str">
         <f>IF(A1610="", "", VLOOKUP(A1610, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1610" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1610" s="12">
+        <v>21.6</v>
+      </c>
+      <c r="E1610" s="4">
+        <v>45847</v>
+      </c>
+      <c r="G1610" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1610" s="13" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="1611" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1611" s="2" t="s">
+        <v>385</v>
+      </c>
       <c r="B1611" s="1" t="str">
         <f>IF(A1611="", "", VLOOKUP(A1611, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>xai</v>
+      </c>
+      <c r="C1611" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1611" s="12">
+        <v>87.5</v>
+      </c>
+      <c r="E1611" s="4">
+        <v>45847</v>
+      </c>
+      <c r="G1611" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1611" s="13" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="1612" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1612" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="B1612" s="1" t="str">
         <f>IF(A1612="", "", VLOOKUP(A1612, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1612" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1612" s="12">
+        <v>86.4</v>
+      </c>
+      <c r="E1612" s="4">
+        <v>45847</v>
+      </c>
+      <c r="G1612" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1612" s="13" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="1613" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1613" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1613" s="1" t="str">
         <f>IF(A1613="", "", VLOOKUP(A1613, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>openai</v>
+      </c>
+      <c r="C1613" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1613" s="12">
+        <v>83.3</v>
+      </c>
+      <c r="E1613" s="4">
+        <v>45847</v>
+      </c>
+      <c r="G1613" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1613" s="13" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="1614" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1614" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="B1614" s="1" t="str">
         <f>IF(A1614="", "", VLOOKUP(A1614, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>anthropic</v>
+      </c>
+      <c r="C1614" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1614" s="12">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="E1614" s="4">
+        <v>45847</v>
+      </c>
+      <c r="G1614" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1614" s="13" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="1615" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1615" s="2" t="s">
+        <v>385</v>
+      </c>
       <c r="B1615" s="1" t="str">
         <f>IF(A1615="", "", VLOOKUP(A1615, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>xai</v>
+      </c>
+      <c r="C1615" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1615" s="12">
+        <v>79</v>
+      </c>
+      <c r="E1615" s="4">
+        <v>45847</v>
+      </c>
+      <c r="G1615" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1615" s="13" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="1616" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1616" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="B1616" s="1" t="str">
         <f>IF(A1616="", "", VLOOKUP(A1616, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1617" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1616" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1616" s="12">
+        <v>74.2</v>
+      </c>
+      <c r="E1616" s="4">
+        <v>45847</v>
+      </c>
+      <c r="G1616" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1616" s="13" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="1617" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1617" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1617" s="1" t="str">
         <f>IF(A1617="", "", VLOOKUP(A1617, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1618" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1617" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1617" s="12">
+        <v>72</v>
+      </c>
+      <c r="E1617" s="4">
+        <v>45847</v>
+      </c>
+      <c r="G1617" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1617" s="13" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="1618" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1618" s="2" t="s">
+        <v>385</v>
+      </c>
       <c r="B1618" s="1" t="str">
         <f>IF(A1618="", "", VLOOKUP(A1618, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1619" spans="2:2" x14ac:dyDescent="0.2">
+        <v>xai</v>
+      </c>
+      <c r="C1618" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1618" s="12">
+        <v>91.7</v>
+      </c>
+      <c r="E1618" s="4">
+        <v>45847</v>
+      </c>
+      <c r="G1618" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1618" s="13" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="1619" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1619" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1619" s="1" t="str">
         <f>IF(A1619="", "", VLOOKUP(A1619, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1620" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1619" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1619" s="12">
+        <v>88.9</v>
+      </c>
+      <c r="E1619" s="4">
+        <v>45847</v>
+      </c>
+      <c r="G1619" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1619" s="13" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="1620" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1620" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="B1620" s="1" t="str">
         <f>IF(A1620="", "", VLOOKUP(A1620, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1621" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1620" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1620" s="12">
+        <v>88</v>
+      </c>
+      <c r="E1620" s="4">
+        <v>45847</v>
+      </c>
+      <c r="G1620" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1620" s="13" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="1621" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1621" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="B1621" s="1" t="str">
         <f>IF(A1621="", "", VLOOKUP(A1621, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1622" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1621" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1621" s="12">
+        <v>75.5</v>
+      </c>
+      <c r="E1621" s="4">
+        <v>45847</v>
+      </c>
+      <c r="G1621" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1621" s="13" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="1622" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1622" s="2" t="s">
+        <v>385</v>
+      </c>
       <c r="B1622" s="1" t="str">
         <f>IF(A1622="", "", VLOOKUP(A1622, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1623" spans="2:2" x14ac:dyDescent="0.2">
+        <v>xai</v>
+      </c>
+      <c r="C1622" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1622" s="12">
+        <v>15.9</v>
+      </c>
+      <c r="E1622" s="4">
+        <v>45847</v>
+      </c>
+      <c r="G1622" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1622" s="13" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="1623" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1623" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="B1623" s="1" t="str">
         <f>IF(A1623="", "", VLOOKUP(A1623, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1624" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1623" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1623" s="12">
+        <v>8.6</v>
+      </c>
+      <c r="E1623" s="4">
+        <v>45847</v>
+      </c>
+      <c r="G1623" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1623" s="13" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="1624" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1624" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1624" s="1" t="str">
         <f>IF(A1624="", "", VLOOKUP(A1624, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1625" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1624" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1624" s="12">
+        <v>6.5</v>
+      </c>
+      <c r="E1624" s="4">
+        <v>45847</v>
+      </c>
+      <c r="G1624" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1624" s="13" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="1625" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1625" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="B1625" s="1" t="str">
         <f>IF(A1625="", "", VLOOKUP(A1625, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1626" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1625" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1625" s="12">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E1625" s="4">
+        <v>45847</v>
+      </c>
+      <c r="G1625" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1625" s="13" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="1626" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1626" s="2" t="s">
+        <v>388</v>
+      </c>
       <c r="B1626" s="1" t="str">
         <f>IF(A1626="", "", VLOOKUP(A1626, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1627" spans="2:2" x14ac:dyDescent="0.2">
+        <v>humanity</v>
+      </c>
+      <c r="C1626" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1626" s="12">
+        <v>98</v>
+      </c>
+      <c r="E1626" s="4">
+        <v>45878</v>
+      </c>
+      <c r="G1626" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1626" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1627" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1627" s="2" t="s">
+        <v>385</v>
+      </c>
       <c r="B1627" s="1" t="str">
         <f>IF(A1627="", "", VLOOKUP(A1627, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1628" spans="2:2" x14ac:dyDescent="0.2">
+        <v>xai</v>
+      </c>
+      <c r="C1627" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1627" s="12">
+        <v>66.7</v>
+      </c>
+      <c r="E1627" s="4">
+        <v>45878</v>
+      </c>
+      <c r="F1627" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1627" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1627" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1628" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1628" s="2" t="s">
+        <v>394</v>
+      </c>
       <c r="B1628" s="1" t="str">
         <f>IF(A1628="", "", VLOOKUP(A1628, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1629" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1628" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1628" s="12">
+        <v>65.7</v>
+      </c>
+      <c r="E1628" s="4">
+        <v>45878</v>
+      </c>
+      <c r="F1628" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1628" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1628" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1629" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1629" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1629" s="1" t="str">
         <f>IF(A1629="", "", VLOOKUP(A1629, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1630" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1629" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1629" s="12">
+        <v>60.8</v>
+      </c>
+      <c r="E1629" s="4">
+        <v>45878</v>
+      </c>
+      <c r="F1629" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1629" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1629" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1630" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1630" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B1630" s="1" t="str">
         <f>IF(A1630="", "", VLOOKUP(A1630, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1631" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1630" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1630" s="12">
+        <v>58.7</v>
+      </c>
+      <c r="E1630" s="4">
+        <v>45878</v>
+      </c>
+      <c r="F1630" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1630" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1630" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1631" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1631" s="2" t="s">
+        <v>381</v>
+      </c>
       <c r="B1631" s="1" t="str">
         <f>IF(A1631="", "", VLOOKUP(A1631, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1632" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1631" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1631" s="12">
+        <v>59.3</v>
+      </c>
+      <c r="E1631" s="4">
+        <v>45878</v>
+      </c>
+      <c r="F1631" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1631" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1631" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1632" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1632" s="2" t="s">
+        <v>373</v>
+      </c>
       <c r="B1632" s="1" t="str">
         <f>IF(A1632="", "", VLOOKUP(A1632, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1633" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1632" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1632" s="12">
+        <v>40</v>
+      </c>
+      <c r="E1632" s="4">
+        <v>45878</v>
+      </c>
+      <c r="F1632" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="G1632" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1632" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1633" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1633" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="B1633" s="1" t="str">
         <f>IF(A1633="", "", VLOOKUP(A1633, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1634" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1633" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1633" s="12">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="E1633" s="4">
+        <v>45878</v>
+      </c>
+      <c r="F1633" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="G1633" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1633" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1634" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1634" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="B1634" s="1" t="str">
         <f>IF(A1634="", "", VLOOKUP(A1634, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1635" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1634" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1634" s="12">
+        <v>37</v>
+      </c>
+      <c r="E1634" s="4">
+        <v>45878</v>
+      </c>
+      <c r="F1634" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="G1634" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1634" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1635" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1635" s="2" t="s">
+        <v>206</v>
+      </c>
       <c r="B1635" s="1" t="str">
         <f>IF(A1635="", "", VLOOKUP(A1635, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1636" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1635" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1635" s="12">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="E1635" s="4">
+        <v>45878</v>
+      </c>
+      <c r="F1635" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="G1635" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1635" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1636" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1636" s="2" t="s">
+        <v>388</v>
+      </c>
       <c r="B1636" s="1" t="str">
         <f>IF(A1636="", "", VLOOKUP(A1636, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1637" spans="2:2" x14ac:dyDescent="0.2">
+        <v>humanity</v>
+      </c>
+      <c r="C1636" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1636" s="12">
+        <v>100</v>
+      </c>
+      <c r="E1636" s="4">
+        <v>45878</v>
+      </c>
+      <c r="G1636" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1636" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1637" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1637" s="2" t="s">
+        <v>385</v>
+      </c>
       <c r="B1637" s="1" t="str">
         <f>IF(A1637="", "", VLOOKUP(A1637, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1638" spans="2:2" x14ac:dyDescent="0.2">
+        <v>xai</v>
+      </c>
+      <c r="C1637" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1637" s="12">
+        <v>16</v>
+      </c>
+      <c r="E1637" s="4">
+        <v>45878</v>
+      </c>
+      <c r="F1637" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1637" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1637" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1638" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1638" s="2" t="s">
+        <v>394</v>
+      </c>
       <c r="B1638" s="1" t="str">
         <f>IF(A1638="", "", VLOOKUP(A1638, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1639" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1638" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1638" s="12">
+        <v>9.9</v>
+      </c>
+      <c r="E1638" s="4">
+        <v>45878</v>
+      </c>
+      <c r="F1638" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1638" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1638" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1639" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1639" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1639" s="1" t="str">
         <f>IF(A1639="", "", VLOOKUP(A1639, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1640" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1639" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1639" s="12">
+        <v>6.5</v>
+      </c>
+      <c r="E1639" s="4">
+        <v>45878</v>
+      </c>
+      <c r="F1639" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1639" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1639" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1640" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1640" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B1640" s="1" t="str">
         <f>IF(A1640="", "", VLOOKUP(A1640, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1641" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1640" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1640" s="12">
+        <v>6.1</v>
+      </c>
+      <c r="E1640" s="4">
+        <v>45878</v>
+      </c>
+      <c r="F1640" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1640" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1640" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1641" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1641" s="2" t="s">
+        <v>381</v>
+      </c>
       <c r="B1641" s="1" t="str">
         <f>IF(A1641="", "", VLOOKUP(A1641, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1642" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1641" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1641" s="12">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E1641" s="4">
+        <v>45878</v>
+      </c>
+      <c r="F1641" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1641" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1641" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1642" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1642" s="2" t="s">
+        <v>373</v>
+      </c>
       <c r="B1642" s="1" t="str">
         <f>IF(A1642="", "", VLOOKUP(A1642, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1643" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1642" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1642" s="12">
+        <v>5.9</v>
+      </c>
+      <c r="E1642" s="4">
+        <v>45878</v>
+      </c>
+      <c r="F1642" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="G1642" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1642" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1643" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1643" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="B1643" s="1" t="str">
         <f>IF(A1643="", "", VLOOKUP(A1643, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1644" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1643" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1643" s="12">
+        <v>8.6</v>
+      </c>
+      <c r="E1643" s="4">
+        <v>45878</v>
+      </c>
+      <c r="F1643" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="G1643" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1643" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1644" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1644" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="B1644" s="1" t="str">
         <f>IF(A1644="", "", VLOOKUP(A1644, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1645" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1644" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1644" s="12">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E1644" s="4">
+        <v>45878</v>
+      </c>
+      <c r="F1644" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="G1644" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1644" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1645" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1645" s="2" t="s">
+        <v>206</v>
+      </c>
       <c r="B1645" s="1" t="str">
         <f>IF(A1645="", "", VLOOKUP(A1645, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1646" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1645" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1645" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="E1645" s="4">
+        <v>45878</v>
+      </c>
+      <c r="F1645" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="G1645" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="H1645" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1646" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1646" s="2" t="s">
+        <v>398</v>
+      </c>
       <c r="B1646" s="1" t="str">
         <f>IF(A1646="", "", VLOOKUP(A1646, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1647" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1646" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1646" s="12">
+        <v>74.5</v>
+      </c>
+      <c r="E1646" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1646" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1646" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1647" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1647" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="B1647" s="1" t="str">
         <f>IF(A1647="", "", VLOOKUP(A1647, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1648" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1647" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1647" s="12">
+        <v>72.5</v>
+      </c>
+      <c r="E1647" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1647" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1647" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1648" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1648" s="2" t="s">
+        <v>373</v>
+      </c>
       <c r="B1648" s="1" t="str">
         <f>IF(A1648="", "", VLOOKUP(A1648, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1649" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1648" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1648" s="12">
+        <v>72.7</v>
+      </c>
+      <c r="E1648" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1648" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1648" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1649" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1649" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1649" s="1" t="str">
         <f>IF(A1649="", "", VLOOKUP(A1649, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1650" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1649" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1649" s="12">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="E1649" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1649" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1649" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1650" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1650" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="B1650" s="1" t="str">
         <f>IF(A1650="", "", VLOOKUP(A1650, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1651" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1650" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1650" s="12">
+        <v>67.2</v>
+      </c>
+      <c r="E1650" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1650" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1650" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1651" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1651" s="2" t="s">
+        <v>398</v>
+      </c>
       <c r="B1651" s="1" t="str">
         <f>IF(A1651="", "", VLOOKUP(A1651, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1652" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1651" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1651" s="12">
+        <v>80.900000000000006</v>
+      </c>
+      <c r="E1651" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1651" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1651" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1652" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1652" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="B1652" s="1" t="str">
         <f>IF(A1652="", "", VLOOKUP(A1652, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1653" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1652" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1652" s="12">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="E1652" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1652" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1652" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1653" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1653" s="2" t="s">
+        <v>373</v>
+      </c>
       <c r="B1653" s="1" t="str">
         <f>IF(A1653="", "", VLOOKUP(A1653, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1654" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1653" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1653" s="12">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="E1653" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1653" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1653" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1654" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1654" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1654" s="1" t="str">
         <f>IF(A1654="", "", VLOOKUP(A1654, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1655" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1654" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1654" s="12">
+        <v>83.3</v>
+      </c>
+      <c r="E1654" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1654" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1654" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1655" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1655" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="B1655" s="1" t="str">
         <f>IF(A1655="", "", VLOOKUP(A1655, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1656" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1655" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1655" s="12">
+        <v>86.4</v>
+      </c>
+      <c r="E1655" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1655" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1655" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1656" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1656" s="2" t="s">
+        <v>398</v>
+      </c>
       <c r="B1656" s="1" t="str">
         <f>IF(A1656="", "", VLOOKUP(A1656, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1657" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1656" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1656" s="12">
+        <v>56</v>
+      </c>
+      <c r="E1656" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1656" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1656" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1657" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1657" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="B1657" s="1" t="str">
         <f>IF(A1657="", "", VLOOKUP(A1657, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1658" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1657" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1657" s="12">
+        <v>59.6</v>
+      </c>
+      <c r="E1657" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1657" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1657" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1658" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1658" s="2" t="s">
+        <v>373</v>
+      </c>
       <c r="B1658" s="1" t="str">
         <f>IF(A1658="", "", VLOOKUP(A1658, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1659" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1658" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1658" s="12">
+        <v>60</v>
+      </c>
+      <c r="E1658" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1658" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1658" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1659" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1659" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1659" s="1" t="str">
         <f>IF(A1659="", "", VLOOKUP(A1659, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1660" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1659" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1659" s="12">
+        <v>52</v>
+      </c>
+      <c r="E1659" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1659" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1659" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1660" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1660" s="2" t="s">
+        <v>398</v>
+      </c>
       <c r="B1660" s="1" t="str">
         <f>IF(A1660="", "", VLOOKUP(A1660, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1661" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1660" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1660" s="12">
+        <v>82.4</v>
+      </c>
+      <c r="E1660" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1660" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1660" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1661" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1661" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="B1661" s="1" t="str">
         <f>IF(A1661="", "", VLOOKUP(A1661, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1662" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1661" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1661" s="12">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="E1661" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1661" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1661" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1662" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1662" s="2" t="s">
+        <v>373</v>
+      </c>
       <c r="B1662" s="1" t="str">
         <f>IF(A1662="", "", VLOOKUP(A1662, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1663" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1662" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1662" s="12">
+        <v>80.5</v>
+      </c>
+      <c r="E1662" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1662" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1662" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1663" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1663" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1663" s="1" t="str">
         <f>IF(A1663="", "", VLOOKUP(A1663, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1664" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1663" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1663" s="12">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="E1663" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1663" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1663" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1664" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1664" s="2" t="s">
+        <v>398</v>
+      </c>
       <c r="B1664" s="1" t="str">
         <f>IF(A1664="", "", VLOOKUP(A1664, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1665" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1664" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1664" s="12">
+        <v>89.5</v>
+      </c>
+      <c r="E1664" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1664" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1664" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1665" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1665" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="B1665" s="1" t="str">
         <f>IF(A1665="", "", VLOOKUP(A1665, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1666" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1665" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1665" s="12">
+        <v>88.8</v>
+      </c>
+      <c r="E1665" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1665" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1665" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1666" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1666" s="2" t="s">
+        <v>373</v>
+      </c>
       <c r="B1666" s="1" t="str">
         <f>IF(A1666="", "", VLOOKUP(A1666, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1667" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1666" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1666" s="12">
+        <v>86.5</v>
+      </c>
+      <c r="E1666" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1666" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1666" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1667" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1667" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1667" s="1" t="str">
         <f>IF(A1667="", "", VLOOKUP(A1667, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1668" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1667" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1667" s="12">
+        <v>88.8</v>
+      </c>
+      <c r="E1667" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1667" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1667" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1668" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1668" s="2" t="s">
+        <v>398</v>
+      </c>
       <c r="B1668" s="1" t="str">
         <f>IF(A1668="", "", VLOOKUP(A1668, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1669" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1668" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1668" s="12">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="E1668" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1668" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1668" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1669" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1669" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="B1669" s="1" t="str">
         <f>IF(A1669="", "", VLOOKUP(A1669, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1670" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1669" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1669" s="12">
+        <v>76.5</v>
+      </c>
+      <c r="E1669" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1669" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1669" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1670" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1670" s="2" t="s">
+        <v>373</v>
+      </c>
       <c r="B1670" s="1" t="str">
         <f>IF(A1670="", "", VLOOKUP(A1670, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1671" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1670" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1670" s="12">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="E1670" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1670" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1670" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1671" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1671" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1671" s="1" t="str">
         <f>IF(A1671="", "", VLOOKUP(A1671, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1672" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1671" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1671" s="12">
+        <v>82.9</v>
+      </c>
+      <c r="E1671" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1671" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1671" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1672" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1672" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="B1672" s="1" t="str">
         <f>IF(A1672="", "", VLOOKUP(A1672, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1673" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1672" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1672" s="12">
+        <v>82</v>
+      </c>
+      <c r="E1672" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1672" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1672" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1673" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1673" s="2" t="s">
+        <v>398</v>
+      </c>
       <c r="B1673" s="1" t="str">
         <f>IF(A1673="", "", VLOOKUP(A1673, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1674" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1673" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1673" s="12">
+        <v>78</v>
+      </c>
+      <c r="E1673" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1673" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1673" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1674" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1674" s="2" t="s">
+        <v>372</v>
+      </c>
       <c r="B1674" s="1" t="str">
         <f>IF(A1674="", "", VLOOKUP(A1674, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1675" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1674" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1674" s="12">
+        <v>75.5</v>
+      </c>
+      <c r="E1674" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1674" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1674" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1675" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1675" s="2" t="s">
+        <v>373</v>
+      </c>
       <c r="B1675" s="1" t="str">
         <f>IF(A1675="", "", VLOOKUP(A1675, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1676" spans="2:2" x14ac:dyDescent="0.2">
+        <v>anthropic</v>
+      </c>
+      <c r="C1675" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1675" s="12">
+        <v>70.5</v>
+      </c>
+      <c r="E1675" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1675" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1675" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1676" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1676" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1676" s="1" t="str">
         <f>IF(A1676="", "", VLOOKUP(A1676, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1677" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1676" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1676" s="12">
+        <v>88.9</v>
+      </c>
+      <c r="E1676" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1676" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1676" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1677" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1677" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="B1677" s="1" t="str">
         <f>IF(A1677="", "", VLOOKUP(A1677, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1678" spans="2:2" x14ac:dyDescent="0.2">
+        <v>google-deepmind</v>
+      </c>
+      <c r="C1677" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1677" s="12">
+        <v>88</v>
+      </c>
+      <c r="E1677" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1677" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="H1677" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="1678" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1678" s="2" t="s">
+        <v>401</v>
+      </c>
       <c r="B1678" s="1" t="str">
         <f>IF(A1678="", "", VLOOKUP(A1678, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1679" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1678" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1678" s="12">
+        <v>2622</v>
+      </c>
+      <c r="E1678" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1678" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1678" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1679" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1679" s="2" t="s">
+        <v>402</v>
+      </c>
       <c r="B1679" s="1" t="str">
         <f>IF(A1679="", "", VLOOKUP(A1679, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1680" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1679" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1679" s="12">
+        <v>2516</v>
+      </c>
+      <c r="E1679" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1679" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1679" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1680" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1680" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1680" s="1" t="str">
         <f>IF(A1680="", "", VLOOKUP(A1680, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1681" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1680" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1680" s="12">
+        <v>2706</v>
+      </c>
+      <c r="E1680" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1680" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1680" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1681" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1681" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B1681" s="1" t="str">
         <f>IF(A1681="", "", VLOOKUP(A1681, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1682" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1681" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1681" s="12">
+        <v>2719</v>
+      </c>
+      <c r="E1681" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1681" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1681" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1682" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1682" s="2" t="s">
+        <v>401</v>
+      </c>
       <c r="B1682" s="1" t="str">
         <f>IF(A1682="", "", VLOOKUP(A1682, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1683" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1682" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1682" s="12">
+        <v>19</v>
+      </c>
+      <c r="E1682" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1682" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1682" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1683" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1683" s="2" t="s">
+        <v>402</v>
+      </c>
       <c r="B1683" s="1" t="str">
         <f>IF(A1683="", "", VLOOKUP(A1683, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1684" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1683" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1683" s="12">
+        <v>17.3</v>
+      </c>
+      <c r="E1683" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1683" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1683" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1684" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1684" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1684" s="1" t="str">
         <f>IF(A1684="", "", VLOOKUP(A1684, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1685" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1684" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1684" s="12">
+        <v>24.9</v>
+      </c>
+      <c r="E1684" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1684" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1684" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1685" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1685" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B1685" s="1" t="str">
         <f>IF(A1685="", "", VLOOKUP(A1685, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1686" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1685" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1685" s="12">
+        <v>17.7</v>
+      </c>
+      <c r="E1685" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1685" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1685" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1686" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1686" s="2" t="s">
+        <v>401</v>
+      </c>
       <c r="B1686" s="1" t="str">
         <f>IF(A1686="", "", VLOOKUP(A1686, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1687" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1686" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1686" s="12">
+        <v>96.6</v>
+      </c>
+      <c r="E1686" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1686" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1686" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1687" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1687" s="2" t="s">
+        <v>402</v>
+      </c>
       <c r="B1687" s="1" t="str">
         <f>IF(A1687="", "", VLOOKUP(A1687, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1688" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1687" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1687" s="12">
+        <v>96</v>
+      </c>
+      <c r="E1687" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1687" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1687" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1688" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1688" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1688" s="1" t="str">
         <f>IF(A1688="", "", VLOOKUP(A1688, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1689" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1688" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1688" s="12">
+        <v>95.2</v>
+      </c>
+      <c r="E1688" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1688" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1688" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1689" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1689" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B1689" s="1" t="str">
         <f>IF(A1689="", "", VLOOKUP(A1689, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1690" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1689" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1689" s="12">
+        <v>98.7</v>
+      </c>
+      <c r="E1689" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1689" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1689" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1690" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1690" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="B1690" s="1" t="str">
         <f>IF(A1690="", "", VLOOKUP(A1690, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1691" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1690" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1690" s="12">
+        <v>87.3</v>
+      </c>
+      <c r="E1690" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1690" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1690" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1691" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1691" s="2" t="s">
+        <v>401</v>
+      </c>
       <c r="B1691" s="1" t="str">
         <f>IF(A1691="", "", VLOOKUP(A1691, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1692" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1691" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1691" s="12">
+        <v>97.9</v>
+      </c>
+      <c r="E1691" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1691" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1691" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1692" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1692" s="2" t="s">
+        <v>402</v>
+      </c>
       <c r="B1692" s="1" t="str">
         <f>IF(A1692="", "", VLOOKUP(A1692, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1693" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1692" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1692" s="12">
+        <v>98.7</v>
+      </c>
+      <c r="E1692" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1692" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1692" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1693" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1693" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1693" s="1" t="str">
         <f>IF(A1693="", "", VLOOKUP(A1693, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1694" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1693" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1693" s="12">
+        <v>98.4</v>
+      </c>
+      <c r="E1693" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1693" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1693" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1694" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1694" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B1694" s="1" t="str">
         <f>IF(A1694="", "", VLOOKUP(A1694, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1695" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1694" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1694" s="12">
+        <v>99.5</v>
+      </c>
+      <c r="E1694" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1694" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1694" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1695" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1695" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="B1695" s="1" t="str">
         <f>IF(A1695="", "", VLOOKUP(A1695, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1696" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1695" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1695" s="12">
+        <v>86.5</v>
+      </c>
+      <c r="E1695" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1695" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1695" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1696" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1696" s="2" t="s">
+        <v>401</v>
+      </c>
       <c r="B1696" s="1" t="str">
         <f>IF(A1696="", "", VLOOKUP(A1696, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1697" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1696" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1696" s="12">
+        <v>80.099999999999994</v>
+      </c>
+      <c r="E1696" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1696" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1696" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1697" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1697" s="2" t="s">
+        <v>402</v>
+      </c>
       <c r="B1697" s="1" t="str">
         <f>IF(A1697="", "", VLOOKUP(A1697, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1698" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1697" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1697" s="12">
+        <v>71.5</v>
+      </c>
+      <c r="E1697" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1697" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1697" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1698" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1698" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1698" s="1" t="str">
         <f>IF(A1698="", "", VLOOKUP(A1698, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1699" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1698" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1698" s="12">
+        <v>83.3</v>
+      </c>
+      <c r="E1698" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1698" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1698" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1699" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1699" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B1699" s="1" t="str">
         <f>IF(A1699="", "", VLOOKUP(A1699, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1700" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1699" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1699" s="12">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="E1699" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1699" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1699" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1700" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1700" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="B1700" s="1" t="str">
         <f>IF(A1700="", "", VLOOKUP(A1700, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1701" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1700" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1700" s="12">
+        <v>77</v>
+      </c>
+      <c r="E1700" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1700" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1700" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1701" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1701" s="2" t="s">
+        <v>401</v>
+      </c>
       <c r="B1701" s="1" t="str">
         <f>IF(A1701="", "", VLOOKUP(A1701, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1702" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1701" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1701" s="12">
+        <v>90</v>
+      </c>
+      <c r="E1701" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1701" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1701" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1702" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1702" s="2" t="s">
+        <v>402</v>
+      </c>
       <c r="B1702" s="1" t="str">
         <f>IF(A1702="", "", VLOOKUP(A1702, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1703" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1702" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1702" s="12">
+        <v>85.3</v>
+      </c>
+      <c r="E1702" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1702" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1702" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1703" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1703" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1703" s="1" t="str">
         <f>IF(A1703="", "", VLOOKUP(A1703, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1704" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1703" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1703" s="12">
+        <v>93.4</v>
+      </c>
+      <c r="E1703" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1703" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1703" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1704" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1704" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B1704" s="1" t="str">
         <f>IF(A1704="", "", VLOOKUP(A1704, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1705" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1704" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1704" s="12">
+        <v>93</v>
+      </c>
+      <c r="E1704" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1704" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1704" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1705" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1705" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="B1705" s="1" t="str">
         <f>IF(A1705="", "", VLOOKUP(A1705, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1706" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1705" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1705" s="12">
+        <v>87</v>
+      </c>
+      <c r="E1705" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1705" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1705" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1706" s="2" t="s">
+        <v>401</v>
+      </c>
       <c r="B1706" s="1" t="str">
         <f>IF(A1706="", "", VLOOKUP(A1706, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1707" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1706" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1706" s="12">
+        <v>67.8</v>
+      </c>
+      <c r="E1706" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1706" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1706" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1707" s="2" t="s">
+        <v>402</v>
+      </c>
       <c r="B1707" s="1" t="str">
         <f>IF(A1707="", "", VLOOKUP(A1707, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="1708" spans="2:2" x14ac:dyDescent="0.2">
+        <v>openai</v>
+      </c>
+      <c r="C1707" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1707" s="12">
+        <v>54.8</v>
+      </c>
+      <c r="E1707" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1707" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1707" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1708" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1708" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B1708" s="1" t="str">
         <f>IF(A1708="", "", VLOOKUP(A1708, 'model-meta'!A:B, 2, FALSE))</f>
-        <v/>
+        <v>openai</v>
+      </c>
+      <c r="C1708" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1708" s="12">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="E1708" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1708" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1708" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1709" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1709" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1709" s="1" t="str">
+        <f>IF(A1709="", "", VLOOKUP(A1709, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1709" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1709" s="12">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="E1709" s="4">
+        <v>45874</v>
+      </c>
+      <c r="G1709" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1709" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="1710" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1710" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B1710" s="1" t="str">
+        <f>IF(A1710="", "", VLOOKUP(A1710, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1710" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1710" s="12">
+        <v>99.6</v>
+      </c>
+      <c r="E1710" s="4">
+        <v>45876</v>
+      </c>
+      <c r="F1710" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1710" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1710" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1711" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1711" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1711" s="1" t="str">
+        <f>IF(A1711="", "", VLOOKUP(A1711, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1711" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1711" s="12">
+        <v>98.4</v>
+      </c>
+      <c r="E1711" s="4">
+        <v>45876</v>
+      </c>
+      <c r="G1711" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1711" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1712" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1712" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1712" s="1" t="str">
+        <f>IF(A1712="", "", VLOOKUP(A1712, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1712" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1712" s="12">
+        <v>42.1</v>
+      </c>
+      <c r="E1712" s="4">
+        <v>45876</v>
+      </c>
+      <c r="G1712" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1712" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1713" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1713" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B1713" s="1" t="str">
+        <f>IF(A1713="", "", VLOOKUP(A1713, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1713" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1713" s="12">
+        <v>87.3</v>
+      </c>
+      <c r="E1713" s="4">
+        <v>45876</v>
+      </c>
+      <c r="F1713" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1713" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1713" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1714" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1714" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1714" s="1" t="str">
+        <f>IF(A1714="", "", VLOOKUP(A1714, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1714" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1714" s="12">
+        <v>83.3</v>
+      </c>
+      <c r="E1714" s="4">
+        <v>45876</v>
+      </c>
+      <c r="G1714" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1714" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1715" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1715" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1715" s="1" t="str">
+        <f>IF(A1715="", "", VLOOKUP(A1715, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1715" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1715" s="12">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="E1715" s="4">
+        <v>45876</v>
+      </c>
+      <c r="G1715" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1715" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1716" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1716" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B1716" s="1" t="str">
+        <f>IF(A1716="", "", VLOOKUP(A1716, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1716" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1716" s="12">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="E1716" s="4">
+        <v>45876</v>
+      </c>
+      <c r="F1716" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1716" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1716" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1717" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1717" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1717" s="1" t="str">
+        <f>IF(A1717="", "", VLOOKUP(A1717, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1717" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1717" s="12">
+        <v>24.3</v>
+      </c>
+      <c r="E1717" s="4">
+        <v>45876</v>
+      </c>
+      <c r="G1717" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1717" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1718" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1718" s="1" t="str">
+        <f>IF(A1718="", "", VLOOKUP(A1718, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1718" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1718" s="12">
+        <v>5.3</v>
+      </c>
+      <c r="E1718" s="4">
+        <v>45876</v>
+      </c>
+      <c r="G1718" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1718" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1719" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1719" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B1719" s="1" t="str">
+        <f>IF(A1719="", "", VLOOKUP(A1719, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1719" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1719" s="12">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="E1719" s="4">
+        <v>45876</v>
+      </c>
+      <c r="G1719" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1719" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1720" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1720" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1720" s="1" t="str">
+        <f>IF(A1720="", "", VLOOKUP(A1720, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1720" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1720" s="12">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="E1720" s="4">
+        <v>45876</v>
+      </c>
+      <c r="G1720" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1720" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1721" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1721" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1721" s="1" t="str">
+        <f>IF(A1721="", "", VLOOKUP(A1721, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1721" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1721" s="12">
+        <v>30.8</v>
+      </c>
+      <c r="E1721" s="4">
+        <v>45876</v>
+      </c>
+      <c r="G1721" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1721" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1722" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1722" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B1722" s="1" t="str">
+        <f>IF(A1722="", "", VLOOKUP(A1722, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1722" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D1722" s="12">
+        <v>88</v>
+      </c>
+      <c r="E1722" s="4">
+        <v>45876</v>
+      </c>
+      <c r="F1722" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1722" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1722" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1723" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1723" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1723" s="1" t="str">
+        <f>IF(A1723="", "", VLOOKUP(A1723, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1723" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D1723" s="12">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="E1723" s="4">
+        <v>45876</v>
+      </c>
+      <c r="G1723" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1723" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1724" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1724" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1724" s="1" t="str">
+        <f>IF(A1724="", "", VLOOKUP(A1724, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1724" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D1724" s="12">
+        <v>25.8</v>
+      </c>
+      <c r="E1724" s="4">
+        <v>45876</v>
+      </c>
+      <c r="G1724" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1724" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1725" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1725" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B1725" s="1" t="str">
+        <f>IF(A1725="", "", VLOOKUP(A1725, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1725" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1725" s="12">
+        <v>54.9</v>
+      </c>
+      <c r="E1725" s="4">
+        <v>45876</v>
+      </c>
+      <c r="F1725" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1725" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1725" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1726" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1726" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1726" s="1" t="str">
+        <f>IF(A1726="", "", VLOOKUP(A1726, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1726" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1726" s="12">
+        <v>49.7</v>
+      </c>
+      <c r="E1726" s="4">
+        <v>45876</v>
+      </c>
+      <c r="G1726" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1726" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1727" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1727" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B1727" s="1" t="str">
+        <f>IF(A1727="", "", VLOOKUP(A1727, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1727" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1727" s="12">
+        <v>99</v>
+      </c>
+      <c r="E1727" s="4">
+        <v>45876</v>
+      </c>
+      <c r="F1727" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1727" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1727" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1728" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1728" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1728" s="1" t="str">
+        <f>IF(A1728="", "", VLOOKUP(A1728, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1728" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1728" s="12">
+        <v>98.4</v>
+      </c>
+      <c r="E1728" s="4">
+        <v>45876</v>
+      </c>
+      <c r="G1728" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1728" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1729" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1729" s="1" t="str">
+        <f>IF(A1729="", "", VLOOKUP(A1729, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1729" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1729" s="12">
+        <v>61</v>
+      </c>
+      <c r="E1729" s="4">
+        <v>45876</v>
+      </c>
+      <c r="G1729" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1729" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1730" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B1730" s="1" t="str">
+        <f>IF(A1730="", "", VLOOKUP(A1730, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1730" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1730" s="12">
+        <v>84.2</v>
+      </c>
+      <c r="E1730" s="4">
+        <v>45876</v>
+      </c>
+      <c r="F1730" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1730" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1730" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1731" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1731" s="1" t="str">
+        <f>IF(A1731="", "", VLOOKUP(A1731, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1731" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1731" s="12">
+        <v>82.9</v>
+      </c>
+      <c r="E1731" s="4">
+        <v>45876</v>
+      </c>
+      <c r="G1731" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1731" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1732" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1732" s="1" t="str">
+        <f>IF(A1732="", "", VLOOKUP(A1732, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1732" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1732" s="12">
+        <v>72.2</v>
+      </c>
+      <c r="E1732" s="4">
+        <v>45876</v>
+      </c>
+      <c r="G1732" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1732" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1733" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B1733" s="1" t="str">
+        <f>IF(A1733="", "", VLOOKUP(A1733, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1733" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1733" s="12">
+        <v>81.099999999999994</v>
+      </c>
+      <c r="E1733" s="4">
+        <v>45876</v>
+      </c>
+      <c r="F1733" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1733" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1733" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1734" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1734" s="1" t="str">
+        <f>IF(A1734="", "", VLOOKUP(A1734, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1734" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1734" s="12">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="E1734" s="4">
+        <v>45876</v>
+      </c>
+      <c r="G1734" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1734" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1735" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1735" s="1" t="str">
+        <f>IF(A1735="", "", VLOOKUP(A1735, 'model-meta'!A:B, 2, FALSE))</f>
+        <v>openai</v>
+      </c>
+      <c r="C1735" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1735" s="12">
+        <v>58.8</v>
+      </c>
+      <c r="E1735" s="4">
+        <v>45876</v>
+      </c>
+      <c r="G1735" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="H1735" s="13" t="s">
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -44116,6 +46814,134 @@
     <hyperlink ref="H1605" r:id="rId550" xr:uid="{24E55C23-44D0-CD46-AC38-ED9C72B6CF9A}"/>
     <hyperlink ref="H1606" r:id="rId551" xr:uid="{59FAB9EA-2B6B-0A44-9816-A3A39917728E}"/>
     <hyperlink ref="H1607" r:id="rId552" xr:uid="{D23EBE6A-F307-EE4D-B0B7-A7CA4F5783C4}"/>
+    <hyperlink ref="H1608" r:id="rId553" xr:uid="{7A3AF815-1A14-1E48-817A-2C4929B796E7}"/>
+    <hyperlink ref="H1609" r:id="rId554" xr:uid="{66C534CF-4AF4-3445-AA07-87FDBD7D40CD}"/>
+    <hyperlink ref="H1610" r:id="rId555" xr:uid="{C6D766DC-800B-6549-9489-448CA0B7D720}"/>
+    <hyperlink ref="H1611" r:id="rId556" xr:uid="{3664ED4E-B5F0-614A-8DF4-4A5B743E7829}"/>
+    <hyperlink ref="H1612" r:id="rId557" xr:uid="{CBD3A8BA-5AFD-664A-8583-82B167F14933}"/>
+    <hyperlink ref="H1613" r:id="rId558" xr:uid="{D7773A6A-1D64-414C-8F6E-B5C96D5BA5C9}"/>
+    <hyperlink ref="H1614" r:id="rId559" xr:uid="{C35FAFA7-06DF-5D46-8C6C-1E04736915E4}"/>
+    <hyperlink ref="H1615" r:id="rId560" xr:uid="{8A6C93BC-7F2F-6B4E-9F29-6A6A83C86306}"/>
+    <hyperlink ref="H1616" r:id="rId561" xr:uid="{F7E354E7-0E49-8C4D-AD7D-47277852BD96}"/>
+    <hyperlink ref="H1617" r:id="rId562" xr:uid="{E6F33DD9-6728-2E47-8578-01B2F2DE2353}"/>
+    <hyperlink ref="H1618" r:id="rId563" xr:uid="{FF5E59E7-0A35-304E-BB52-342EC7AA62A7}"/>
+    <hyperlink ref="H1619" r:id="rId564" xr:uid="{83E49053-2A9A-8642-BA8E-3778435ECE4E}"/>
+    <hyperlink ref="H1620" r:id="rId565" xr:uid="{4DAE9978-E6F0-974A-BD25-0E04AB00E839}"/>
+    <hyperlink ref="H1621" r:id="rId566" xr:uid="{43C02D72-2E18-DC47-B699-3C6EC28EC02F}"/>
+    <hyperlink ref="H1622" r:id="rId567" xr:uid="{D5F27602-1940-324F-9392-07881489981E}"/>
+    <hyperlink ref="H1623" r:id="rId568" xr:uid="{3015F1EF-8C4E-F44A-A8C2-85F358FC61E2}"/>
+    <hyperlink ref="H1624" r:id="rId569" xr:uid="{5C99FCBC-2F66-3A45-A9B3-FB0629F32F9B}"/>
+    <hyperlink ref="H1625" r:id="rId570" xr:uid="{9E4C8E7D-FB6E-5E41-B9D1-085465D889A3}"/>
+    <hyperlink ref="H1626" r:id="rId571" xr:uid="{A6B3C3A3-B958-C44E-97B4-F521DC00512B}"/>
+    <hyperlink ref="H1627" r:id="rId572" xr:uid="{A305428D-5DF9-2E4F-9B8D-37D66C437304}"/>
+    <hyperlink ref="H1628" r:id="rId573" xr:uid="{EA761249-657F-3943-AA53-10EC00FBD6AA}"/>
+    <hyperlink ref="H1629" r:id="rId574" xr:uid="{7BB543DE-DDC3-DA44-83B0-DBF40C30AAF1}"/>
+    <hyperlink ref="H1630" r:id="rId575" xr:uid="{E08D1EBC-7ADB-D64E-A7EC-7606F202A06B}"/>
+    <hyperlink ref="H1631" r:id="rId576" xr:uid="{F8510E55-971D-E442-B303-573737C7458D}"/>
+    <hyperlink ref="H1632" r:id="rId577" xr:uid="{739F093A-9F58-7645-BC31-CD067BA1D15D}"/>
+    <hyperlink ref="H1633" r:id="rId578" xr:uid="{64311555-D5A3-3045-9F5C-986252F6B92B}"/>
+    <hyperlink ref="H1634" r:id="rId579" xr:uid="{81555A89-970D-354D-AC35-E311F3DD4370}"/>
+    <hyperlink ref="H1635" r:id="rId580" xr:uid="{85604A83-FF11-D54D-893D-319F6773BF78}"/>
+    <hyperlink ref="H1636" r:id="rId581" xr:uid="{02156D01-8E28-E54E-A435-2A2302866375}"/>
+    <hyperlink ref="H1637" r:id="rId582" xr:uid="{9CAAC756-0EEC-A94C-9C78-844F10A161C5}"/>
+    <hyperlink ref="H1638" r:id="rId583" xr:uid="{6C494BEA-0704-EC4A-9968-291C27126E1C}"/>
+    <hyperlink ref="H1639" r:id="rId584" xr:uid="{F9695BA2-E911-0A47-AA01-6C02A0D67B20}"/>
+    <hyperlink ref="H1640" r:id="rId585" xr:uid="{60EC7910-9E21-CD47-877E-7E937E5349A6}"/>
+    <hyperlink ref="H1641" r:id="rId586" xr:uid="{81BEFDAA-4427-E448-AB00-12EB90E7715F}"/>
+    <hyperlink ref="H1642" r:id="rId587" xr:uid="{2B236A75-6FC1-A340-B83C-BDF75DF596D9}"/>
+    <hyperlink ref="H1643" r:id="rId588" xr:uid="{47465E08-9754-714C-858B-8D29B7C63297}"/>
+    <hyperlink ref="H1644" r:id="rId589" xr:uid="{2D912739-DFE4-B54F-9FFF-9B26F1590D0F}"/>
+    <hyperlink ref="H1645" r:id="rId590" xr:uid="{387C54DD-9B44-ED4E-B5E1-F8E1F3D43D5F}"/>
+    <hyperlink ref="H1646" r:id="rId591" xr:uid="{EF5AFC47-2ECC-2046-9DA4-F46748FAEFCA}"/>
+    <hyperlink ref="H1647" r:id="rId592" xr:uid="{0C455FE0-568D-A642-85E7-558A3C54955B}"/>
+    <hyperlink ref="H1648" r:id="rId593" xr:uid="{70629203-18F8-5D4E-A45F-7B6C77821356}"/>
+    <hyperlink ref="H1649" r:id="rId594" xr:uid="{6F5EC17F-4E83-A649-81C7-456429DF7141}"/>
+    <hyperlink ref="H1650" r:id="rId595" xr:uid="{228E47AD-62E5-3549-A511-80F8840B2C4C}"/>
+    <hyperlink ref="H1651" r:id="rId596" xr:uid="{55808C7D-F071-6D4F-BDF8-11297D1619BB}"/>
+    <hyperlink ref="H1652" r:id="rId597" xr:uid="{E3214740-1836-A840-9675-92425D245471}"/>
+    <hyperlink ref="H1653" r:id="rId598" xr:uid="{D8593883-F97F-9242-B125-B6CE70E5C625}"/>
+    <hyperlink ref="H1654" r:id="rId599" xr:uid="{C60E8F01-8F33-1340-A6FA-1FDF5B7D528C}"/>
+    <hyperlink ref="H1655" r:id="rId600" xr:uid="{EB14DBE4-0614-974F-86B6-8B78D62EF365}"/>
+    <hyperlink ref="H1656" r:id="rId601" xr:uid="{EDBF5038-7C6D-364E-A531-47A8C862A08B}"/>
+    <hyperlink ref="H1657" r:id="rId602" xr:uid="{557AF491-E3ED-3B43-B33A-559F8335F3E5}"/>
+    <hyperlink ref="H1658" r:id="rId603" xr:uid="{74C3F453-B9F0-BE4B-9A1E-11AD88CC2B4C}"/>
+    <hyperlink ref="H1659" r:id="rId604" xr:uid="{A3D2B94A-A210-DA47-83C3-8210BBCF31B7}"/>
+    <hyperlink ref="H1660" r:id="rId605" xr:uid="{D0A7CA6A-B96D-4041-8625-FA77EFDDD895}"/>
+    <hyperlink ref="H1661" r:id="rId606" xr:uid="{430F7A26-74A0-1A4C-A729-3902EADED61C}"/>
+    <hyperlink ref="H1662" r:id="rId607" xr:uid="{76E00E40-6C02-7341-B4F4-EDD28A410109}"/>
+    <hyperlink ref="H1663" r:id="rId608" xr:uid="{CDC3FCF1-8245-3443-A26B-04F415B36DE1}"/>
+    <hyperlink ref="H1664" r:id="rId609" xr:uid="{4D301495-3CBA-A247-8365-FB6663BA9B83}"/>
+    <hyperlink ref="H1665" r:id="rId610" xr:uid="{025D5882-3AF1-824F-A771-87CB25CE2E45}"/>
+    <hyperlink ref="H1666" r:id="rId611" xr:uid="{A52E01B6-C983-BD41-9A68-797EF9B43594}"/>
+    <hyperlink ref="H1667" r:id="rId612" xr:uid="{A203E43C-78E9-EF45-929A-5A7AD2CFBCD2}"/>
+    <hyperlink ref="H1668" r:id="rId613" xr:uid="{A66ED99D-C947-3F4B-90ED-F8C113C207DE}"/>
+    <hyperlink ref="H1669" r:id="rId614" xr:uid="{AAD8003F-56FA-614E-B700-350A09676A82}"/>
+    <hyperlink ref="H1670" r:id="rId615" xr:uid="{35952AC0-78F4-9246-B511-357CBBB8ED10}"/>
+    <hyperlink ref="H1671" r:id="rId616" xr:uid="{FCAFD2FE-A727-4A47-82FE-AC2FB14B249B}"/>
+    <hyperlink ref="H1672" r:id="rId617" xr:uid="{06D33AAE-D3CB-894C-AEAD-C5D80688E869}"/>
+    <hyperlink ref="H1673" r:id="rId618" xr:uid="{25E4596D-6C74-2A4D-97DC-082E9A4C7C94}"/>
+    <hyperlink ref="H1674" r:id="rId619" xr:uid="{8750D15C-3A95-824A-83F8-6E87C0FBE5B8}"/>
+    <hyperlink ref="H1675" r:id="rId620" xr:uid="{91261DA2-2F3B-0C4C-B52B-854A6902A695}"/>
+    <hyperlink ref="H1676" r:id="rId621" xr:uid="{E3E84663-E05E-1043-9326-75BF5D386866}"/>
+    <hyperlink ref="H1677" r:id="rId622" xr:uid="{FD276219-0DB8-ED42-861C-DF4007CABB15}"/>
+    <hyperlink ref="H1678" r:id="rId623" xr:uid="{79E4926B-06E2-C24B-A9A1-616637A87BB6}"/>
+    <hyperlink ref="H1679" r:id="rId624" xr:uid="{2E0D377B-1022-3B4A-A0DE-6044C4D03DB5}"/>
+    <hyperlink ref="H1680" r:id="rId625" xr:uid="{F2E33443-3C01-1C4E-BF1A-A50D0C21B1A6}"/>
+    <hyperlink ref="H1681" r:id="rId626" xr:uid="{5744907B-694B-7C47-A1A4-47E25866A5D3}"/>
+    <hyperlink ref="H1682" r:id="rId627" xr:uid="{61C3D29F-9ECD-0740-91CD-59B832CA5276}"/>
+    <hyperlink ref="H1683" r:id="rId628" xr:uid="{2CEE1B8B-8168-5F45-8D6B-6721285943FA}"/>
+    <hyperlink ref="H1684" r:id="rId629" xr:uid="{AEBCD03A-FACA-8843-B2A4-D3D8CBC8BB27}"/>
+    <hyperlink ref="H1685" r:id="rId630" xr:uid="{FE355A89-18FB-B440-8337-CE27517FFFC9}"/>
+    <hyperlink ref="H1686" r:id="rId631" xr:uid="{56BB1E37-C058-D848-9B23-7D5CE4E8B395}"/>
+    <hyperlink ref="H1687" r:id="rId632" xr:uid="{8CCC3535-EF85-3441-9C50-DF3B8BB87F94}"/>
+    <hyperlink ref="H1688" r:id="rId633" xr:uid="{C142E440-64A0-2E43-A24C-06253E4D269E}"/>
+    <hyperlink ref="H1689" r:id="rId634" xr:uid="{6B9704CB-0311-BD40-805B-FF7415DE9DD0}"/>
+    <hyperlink ref="H1691" r:id="rId635" xr:uid="{2F4A7389-EDD0-9E49-AA0D-2B7E7ACD6BD6}"/>
+    <hyperlink ref="H1692" r:id="rId636" xr:uid="{D28ADCDB-DB66-A344-A830-EF84DA48FFE3}"/>
+    <hyperlink ref="H1693" r:id="rId637" xr:uid="{C3706150-EE58-AD4D-96CC-DE7466703F95}"/>
+    <hyperlink ref="H1694" r:id="rId638" xr:uid="{8BC944C1-C137-884D-A0E5-1C56A62A39E0}"/>
+    <hyperlink ref="H1696" r:id="rId639" xr:uid="{93F1905C-DD03-BB46-AC5F-E03B0B33614B}"/>
+    <hyperlink ref="H1697" r:id="rId640" xr:uid="{6482A0C8-93E0-F743-A15B-2D4F3B26AB0B}"/>
+    <hyperlink ref="H1698" r:id="rId641" xr:uid="{3300330F-147D-684A-8E83-44EE76655BAF}"/>
+    <hyperlink ref="H1699" r:id="rId642" xr:uid="{95648783-CA30-AB48-B324-C55F1A0C19E4}"/>
+    <hyperlink ref="H1701" r:id="rId643" xr:uid="{DA582D09-465F-8243-BC80-8DB78C190C0E}"/>
+    <hyperlink ref="H1702" r:id="rId644" xr:uid="{962A3A4E-6DE2-FA4A-8E83-33709FC9E6D5}"/>
+    <hyperlink ref="H1703" r:id="rId645" xr:uid="{9520F1D7-EAC8-6146-9886-19199366DF58}"/>
+    <hyperlink ref="H1704" r:id="rId646" xr:uid="{787861BC-AD48-6347-AF1B-30667B4FBA5A}"/>
+    <hyperlink ref="H1706" r:id="rId647" xr:uid="{0CB4CBCD-993F-7341-AAA3-B7BB5E235263}"/>
+    <hyperlink ref="H1707" r:id="rId648" xr:uid="{DFCCAD56-3904-8643-93D6-2EB65AA36863}"/>
+    <hyperlink ref="H1708" r:id="rId649" xr:uid="{F8640F4E-C085-C745-8F48-CA96FC178DB3}"/>
+    <hyperlink ref="H1709" r:id="rId650" xr:uid="{3B783F80-A04E-E647-A125-B2F0C00BA55E}"/>
+    <hyperlink ref="H1690" r:id="rId651" xr:uid="{B6EF0B58-524D-8648-91F8-268B859009CC}"/>
+    <hyperlink ref="H1695" r:id="rId652" xr:uid="{5ABFF573-E411-C542-9678-C46EAB29BAA4}"/>
+    <hyperlink ref="H1700" r:id="rId653" xr:uid="{B42D5C33-64DA-9D4D-91A7-4C64FF441E04}"/>
+    <hyperlink ref="H1705" r:id="rId654" xr:uid="{A8CD367E-4746-5D45-B0FB-9FE0F0469EF3}"/>
+    <hyperlink ref="H1710" r:id="rId655" xr:uid="{E0A3BE36-EAD9-C842-B356-50C37482B435}"/>
+    <hyperlink ref="H1711" r:id="rId656" xr:uid="{758E5159-D599-0C46-901D-886931D7F6BA}"/>
+    <hyperlink ref="H1712" r:id="rId657" xr:uid="{69F53A18-51F1-0F4F-9785-F0895E8E2EB3}"/>
+    <hyperlink ref="H1713" r:id="rId658" xr:uid="{8393BE72-FAB5-574E-8A2B-EC286BEA82C2}"/>
+    <hyperlink ref="H1714" r:id="rId659" xr:uid="{6EAD7963-7FD1-264D-B9A3-671E27236246}"/>
+    <hyperlink ref="H1715" r:id="rId660" xr:uid="{726C6730-FEAD-2B4C-B526-011DCC927CE6}"/>
+    <hyperlink ref="H1716" r:id="rId661" xr:uid="{6AA4FB79-2E77-DD4E-90B7-9EEAE1A58E64}"/>
+    <hyperlink ref="H1717" r:id="rId662" xr:uid="{B0830BC9-C490-644B-B0A3-0FB57246B8B8}"/>
+    <hyperlink ref="H1718" r:id="rId663" xr:uid="{389EBB7B-07EC-974E-9F93-95BD184A548F}"/>
+    <hyperlink ref="H1719" r:id="rId664" xr:uid="{4344FF6B-85FE-0042-BABD-8803C6870585}"/>
+    <hyperlink ref="H1720" r:id="rId665" xr:uid="{B53DE928-36DC-9C4B-9FBF-B1DA87290925}"/>
+    <hyperlink ref="H1721" r:id="rId666" xr:uid="{8667133B-5B69-6146-A4BE-F4C17D34A180}"/>
+    <hyperlink ref="H1722" r:id="rId667" xr:uid="{60481A41-6A1F-C14C-905E-0BE6F7BD5BAA}"/>
+    <hyperlink ref="H1723" r:id="rId668" xr:uid="{9732E39D-D177-434A-ACCE-E3B8AB8D9537}"/>
+    <hyperlink ref="H1724" r:id="rId669" xr:uid="{72F10CF2-5722-A14F-B173-9590225323BF}"/>
+    <hyperlink ref="H1725" r:id="rId670" xr:uid="{271E839E-A00A-9A48-B112-7CF1EBBCF2F3}"/>
+    <hyperlink ref="H1726" r:id="rId671" xr:uid="{885B8AF6-B9EF-1A46-9F06-530023C5F08D}"/>
+    <hyperlink ref="H1727" r:id="rId672" xr:uid="{EEC2B560-23EB-1847-B3CD-A7D82B2CAA66}"/>
+    <hyperlink ref="H1728" r:id="rId673" xr:uid="{A0B9C114-DBAB-1C40-BB5A-52AE59F08D0F}"/>
+    <hyperlink ref="H1729" r:id="rId674" xr:uid="{B0F361B0-9CCF-814C-ABF2-9867C88DB270}"/>
+    <hyperlink ref="H1730" r:id="rId675" xr:uid="{20EB009D-4798-E242-8968-329C80758A21}"/>
+    <hyperlink ref="H1731" r:id="rId676" xr:uid="{5373BD8C-53B0-DD4F-B88C-30EDF46C72B9}"/>
+    <hyperlink ref="H1732" r:id="rId677" xr:uid="{BFC4C31D-7543-1C43-A591-ABF845C800C5}"/>
+    <hyperlink ref="H1733" r:id="rId678" xr:uid="{C008EB7E-D51B-B64C-B752-72EA2C847C0C}"/>
+    <hyperlink ref="H1734" r:id="rId679" xr:uid="{5961189A-BD28-1B43-A7EC-5CE7A28698B1}"/>
+    <hyperlink ref="H1735" r:id="rId680" xr:uid="{66A39ABC-EF16-7044-A91A-29AEFCB54558}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>